<commit_message>
docs:[U888-62] added all data excels
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarangkumar/Documents/Software/Fall 2021/ENSF607/Course Project/ensf-607-608-project/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4837C4F5-96ED-4245-B73B-D2C58EFF6760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B496310-9AE1-1745-8FCF-DC55D98371F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="720" windowWidth="31100" windowHeight="19480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animals" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
   <si>
     <t>a_animalid</t>
   </si>
@@ -316,13 +314,100 @@
   </si>
   <si>
     <t>Revolution treatment</t>
+  </si>
+  <si>
+    <t>Limp Walk</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Inflammed limb</t>
+  </si>
+  <si>
+    <t>Bladder Infection</t>
+  </si>
+  <si>
+    <t>chronic kidney disease</t>
+  </si>
+  <si>
+    <t>Upset Stomach</t>
+  </si>
+  <si>
+    <t>Nighttime terror</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Howling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pregnant </t>
+  </si>
+  <si>
+    <t>Not sleeping</t>
+  </si>
+  <si>
+    <t>image1.png</t>
+  </si>
+  <si>
+    <t>image2.png</t>
+  </si>
+  <si>
+    <t>image4.png</t>
+  </si>
+  <si>
+    <t>image7.png</t>
+  </si>
+  <si>
+    <t>image6.png</t>
+  </si>
+  <si>
+    <t>image5.png</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billy </t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Cyrus</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Homer</t>
+  </si>
+  <si>
+    <t>Simposon</t>
+  </si>
+  <si>
+    <t>Miley</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Lighter</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +538,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1166,15 +1257,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="10.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1315,7 @@
         <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_type,a_breed,a_birthdate,a_sex,a_status,a_ownerid,a_tattoonum,a_rfidnumber,a_microchipnumber,a_weight,a_coatcolor,a_continuousmedication) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1237,32 +1330,32 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>344457461</v>
+        <v>165835067</v>
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>156207221</v>
+        <v>247543542</v>
       </c>
       <c r="K2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>317171422</v>
+        <v>319807825</v>
       </c>
       <c r="M2" t="s">
         <v>72</v>
       </c>
       <c r="P2" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="P2:P7" ca="1" si="0">_xlfn.CONCAT("(",
 A2, ",""",
 B2, """,""",
 C2, """,",
@@ -1277,10 +1370,10 @@
 IF(L2="","NULL",_xlfn.CONCAT("""",L2,"""")), ",""",
 M2, """,",
 IF(N2="","NULL",_xlfn.CONCAT("""",N2,"""")), "),")</f>
-        <v>(1,"Ace","Dog","German shepherd",NULL,"1",3,1,344457461,"156207221","317171422",NULL,"Black",NULL),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>(1,"Ace","Dog","German shepherd",NULL,"0",1,1,165835067,"247543542","319807825",NULL,"Black",NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1294,51 +1387,37 @@
         <v>58</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" ca="1" si="1">RANDBETWEEN(0,3)</f>
+        <f t="shared" ref="G3:G8" ca="1" si="2">RANDBETWEEN(0,3)</f>
         <v>1</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:K8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
-        <v>277594776</v>
+        <f t="shared" ref="I3:K8" ca="1" si="3">RANDBETWEEN(123456789,345678912)</f>
+        <v>264394967</v>
       </c>
       <c r="J3">
-        <f t="shared" ca="1" si="2"/>
-        <v>193650314</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>257881478</v>
       </c>
       <c r="K3">
-        <f t="shared" ca="1" si="2"/>
-        <v>335265545</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>208784783</v>
       </c>
       <c r="M3" t="s">
         <v>66</v>
       </c>
       <c r="P3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A3, ",""",
-B3, """,""",
-C3, """,",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")), ",",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")), ",""",
-F3, """,",
-G3, ",",
-H3, ",",
-I3, ",""",
-J3, """,""",
-K3, """,",
-IF(L3="","NULL",_xlfn.CONCAT("""",L3,"""")), ",""",
-M3, """,",
-IF(N3="","NULL",_xlfn.CONCAT("""",N3,"""")), "),")</f>
-        <v>(2,"Ampersand","Monkey","Capuchin monkey",NULL,"1",1,2,277594776,"193650314","335265545",NULL,"Brown",NULL),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>(2,"Ampersand","Monkey","Capuchin monkey",NULL,"0",1,2,264394967,"257881478","208784783",NULL,"Brown",NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1349,51 +1428,37 @@
         <v>49</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="2"/>
-        <v>321598182</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>263603009</v>
       </c>
       <c r="J4">
-        <f t="shared" ca="1" si="2"/>
-        <v>270000705</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>222088925</v>
       </c>
       <c r="K4">
-        <f t="shared" ca="1" si="2"/>
-        <v>295644874</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>314011986</v>
       </c>
       <c r="M4" t="s">
         <v>73</v>
       </c>
       <c r="P4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A4, ",""",
-B4, """,""",
-C4, """,",
-IF(D4="","NULL",_xlfn.CONCAT("""",D4,"""")), ",",
-IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")), ",""",
-F4, """,",
-G4, ",",
-H4, ",",
-I4, ",""",
-J4, """,""",
-K4, """,",
-IF(L4="","NULL",_xlfn.CONCAT("""",L4,"""")), ",""",
-M4, """,",
-IF(N4="","NULL",_xlfn.CONCAT("""",N4,"""")), "),")</f>
-        <v>(3,"Bat Cow","Cow",NULL,NULL,"0",0,1,321598182,"270000705","295644874",NULL,"Brown, White",NULL),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>(3,"Bat Cow","Cow",NULL,NULL,"0",2,1,263603009,"222088925","314011986",NULL,"Brown, White",NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1407,51 +1472,37 @@
         <v>51</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="2"/>
-        <v>153339220</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>208704960</v>
       </c>
       <c r="J5">
-        <f t="shared" ca="1" si="2"/>
-        <v>286486427</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>247473515</v>
       </c>
       <c r="K5">
-        <f t="shared" ca="1" si="2"/>
-        <v>319444557</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>226898378</v>
       </c>
       <c r="M5" t="s">
         <v>74</v>
       </c>
       <c r="P5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A5, ",""",
-B5, """,""",
-C5, """,",
-IF(D5="","NULL",_xlfn.CONCAT("""",D5,"""")), ",",
-IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")), ",""",
-F5, """,",
-G5, ",",
-H5, ",",
-I5, ",""",
-J5, """,""",
-K5, """,",
-IF(L5="","NULL",_xlfn.CONCAT("""",L5,"""")), ",""",
-M5, """,",
-IF(N5="","NULL",_xlfn.CONCAT("""",N5,"""")), "),")</f>
-        <v>(4,"Comet","Horse","Canadian horse",NULL,"1",3,3,153339220,"286486427","319444557",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>(4,"Comet","Horse","Canadian horse",NULL,"1",1,3,208704960,"247473515","226898378",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1465,51 +1516,37 @@
         <v>62</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6">
-        <f t="shared" ca="1" si="2"/>
-        <v>343643439</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>266888163</v>
       </c>
       <c r="J6">
-        <f t="shared" ca="1" si="2"/>
-        <v>234086782</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>288875156</v>
       </c>
       <c r="K6">
-        <f t="shared" ca="1" si="2"/>
-        <v>301255230</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>235082133</v>
       </c>
       <c r="M6" t="s">
         <v>74</v>
       </c>
       <c r="P6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A6, ",""",
-B6, """,""",
-C6, """,",
-IF(D6="","NULL",_xlfn.CONCAT("""",D6,"""")), ",",
-IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")), ",""",
-F6, """,",
-G6, ",",
-H6, ",",
-I6, ",""",
-J6, """,""",
-K6, """,",
-IF(L6="","NULL",_xlfn.CONCAT("""",L6,"""")), ",""",
-M6, """,",
-IF(N6="","NULL",_xlfn.CONCAT("""",N6,"""")), "),")</f>
-        <v>(5,"Krypto","Dog","Labrador retriever",NULL,"1",1,3,343643439,"234086782","301255230",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>(5,"Krypto","Dog","Labrador retriever",NULL,"1",0,3,266888163,"288875156","235082133",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1523,51 +1560,37 @@
         <v>71</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="2"/>
-        <v>323543197</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>306112853</v>
       </c>
       <c r="J7">
-        <f t="shared" ca="1" si="2"/>
-        <v>344346978</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>134150622</v>
       </c>
       <c r="K7">
-        <f t="shared" ca="1" si="2"/>
-        <v>141709910</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>323373371</v>
       </c>
       <c r="M7" t="s">
         <v>74</v>
       </c>
       <c r="P7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A7, ",""",
-B7, """,""",
-C7, """,",
-IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")), ",",
-IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")), ",""",
-F7, """,",
-G7, ",",
-H7, ",",
-I7, ",""",
-J7, """,""",
-K7, """,",
-IF(L7="","NULL",_xlfn.CONCAT("""",L7,"""")), ",""",
-M7, """,",
-IF(N7="","NULL",_xlfn.CONCAT("""",N7,"""")), "),")</f>
-        <v>(6,"Snowy","Dog","Wire Fox Terrier",NULL,"1",1,4,323543197,"344346978","141709910",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="0"/>
+        <v>(6,"Snowy","Dog","Wire Fox Terrier",NULL,"0",3,4,306112853,"134150622","323373371",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1581,27 +1604,27 @@
         <v>50</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8">
-        <f t="shared" ca="1" si="2"/>
-        <v>334391225</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>148452974</v>
       </c>
       <c r="J8">
-        <f t="shared" ca="1" si="2"/>
-        <v>150189186</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>342360641</v>
       </c>
       <c r="K8">
-        <f t="shared" ca="1" si="2"/>
-        <v>214085954</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>136678103</v>
       </c>
       <c r="M8" t="s">
         <v>75</v>
@@ -1622,7 +1645,7 @@
 IF(L8="","NULL",_xlfn.CONCAT("""",L8,"""")), ",""",
 M8, """,",
 IF(N8="","NULL",_xlfn.CONCAT("""",N8,"""")), ");")</f>
-        <v>(7,"Streaky","Cat","Abyssinian",NULL,"1",2,3,334391225,"150189186","214085954",NULL,"Orange",NULL);</v>
+        <v>(7,"Streaky","Cat","Abyssinian",NULL,"0",2,3,148452974,"342360641","136678103",NULL,"Orange",NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -1635,16 +1658,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B2892-340A-4DA8-A00C-A7D7ACDCDE8B}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="30.77734375" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="1" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1674,7 +1699,7 @@
         <v xml:space="preserve">INSERT INTO owners (o_ownerid,o_firstname,o_middlename,o_lastname,o_role,o_contactnumber,o_emailid,o_address) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1689,7 +1714,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4038593444</v>
+        <v>4031743423</v>
       </c>
       <c r="G2" t="str">
         <f>_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
@@ -1700,10 +1725,10 @@
       </c>
       <c r="J2" t="str">
         <f ca="1">_xlfn.CONCAT("(",A2,",""",B2,""",""",C2,""",""",D2,""",",IF(E2="","NULL",E2),",""",F2,""",""",G2,""",""",H2,"""),")</f>
-        <v>(1,"Damian","Bruce","Wayne",NULL,"4038593444","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>(1,"Damian","Bruce","Wayne",NULL,"4031743423","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1715,7 +1740,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F7" ca="1" si="0">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4035903903</v>
+        <v>4033906233</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" si="1">_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
@@ -1723,10 +1748,10 @@
       </c>
       <c r="J3" t="str">
         <f ca="1">_xlfn.CONCAT("(",A3,",""",B3,""",""",C3,""",""",D3,""",",IF(E3="","NULL",E3),",""",F3,""",""",G3,""",""",H3,"""),")</f>
-        <v>(2,"Yorrick","","Brown",NULL,"4035903903","yorrick.brown@ucalgary.ca",""),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>(2,"Yorrick","","Brown",NULL,"4033906233","yorrick.brown@ucalgary.ca",""),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1741,7 +1766,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>4038465191</v>
+        <v>4031617502</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
@@ -1752,10 +1777,10 @@
       </c>
       <c r="J4" t="str">
         <f ca="1">_xlfn.CONCAT("(",A4,",""",B4,""",""",C4,""",""",D4,""",",IF(E4="","NULL",E4),",""",F4,""",""",G4,""",""",H4,"""),")</f>
-        <v>(3,"Clark","Joseph","Kent",NULL,"4038465191","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>(3,"Clark","Joseph","Kent",NULL,"4031617502","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1764,7 +1789,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4036778106</v>
+        <v>4039872693</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -1775,10 +1800,10 @@
       </c>
       <c r="J5" t="str">
         <f ca="1">_xlfn.CONCAT("(",A5,",""",B5,""",""",C5,""",""",D5,""",",IF(E5="","NULL",E5),",""",F5,""",""",G5,""",""",H5,"""),")</f>
-        <v>(4,"Tintin","","",NULL,"4036778106","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>(4,"Tintin","","",NULL,"4039872693","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1790,7 +1815,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4038264135</v>
+        <v>4039960231</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -1801,10 +1826,10 @@
       </c>
       <c r="J6" t="str">
         <f ca="1">_xlfn.CONCAT("(",A6,",""",B6,""",""",C6,""",""",D6,""",",IF(E6="","NULL",E6),",""",F6,""",""",G6,""",""",H6,"""),")</f>
-        <v>(5,"UCalgary","","",0,"4038264135","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>(5,"UCalgary","","",0,"4039960231","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1816,7 +1841,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4036073933</v>
+        <v>4034565624</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -1827,7 +1852,7 @@
       </c>
       <c r="J7" t="str">
         <f ca="1">_xlfn.CONCAT("(",A7,",""",B7,""",""",C7,""",""",D7,""",",IF(E7="","NULL",E7),",""",F7,""",""",G7,""",""",H7,""");")</f>
-        <v>(6,"James","","Gunn",NULL,"4036073933","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+        <v>(6,"James","","Gunn",NULL,"4034565624","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
       </c>
     </row>
   </sheetData>
@@ -1837,16 +1862,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A0186-44D9-498E-B660-5B0A566DD134}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="10.77734375" customWidth="1"/>
+    <col min="1" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -1861,6 +1888,169 @@
       </c>
       <c r="E1" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO owners (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO owners (u_userid,u_firstname,u_middlename,u_lastname,u_role,email,password) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT("(",
+A2,",""",
+B2,""",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
+        <v>(1,"Damian","Bruce","Wayne","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I7" si="0">_xlfn.CONCAT("(",
+A3,",""",
+B3,""",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
+        <v>(2,"Tony",NULL,"Stark","2"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,"Clark","Joseph","Kent","3"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,"Billy ","Ray","Cyrus","2"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,"Bob","Homer","Simposon","2"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,"Miley","Ray",NULL,"1"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="str">
+        <f>_xlfn.CONCAT("(",
+A8,",""",
+B8,""",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
+        <v>(7,"Chris",NULL,"Lighter","2");</v>
       </c>
     </row>
   </sheetData>
@@ -1870,16 +2060,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4EAFE5-CE5B-467E-B9FE-9E32C463D99E}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.77734375" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -1888,6 +2080,128 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="E1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos (",A1,",",B1,",",C1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO photos (p_photoid,p_animalid,p_photolink) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),"","),")</f>
+        <v>(1,"3","image1.png"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E7" ca="1" si="1">_xlfn.CONCAT("(",
+A3,",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),"","),")</f>
+        <v>(2,"5","image2.png"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(3,"7","image4.png"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(4,"7",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(5,"3","image7.png"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(6,"6","image6.png"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8,",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),"",")",";")</f>
+        <v>(7,"4","image5.png");</v>
       </c>
     </row>
   </sheetData>
@@ -1897,16 +2211,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B89DC6B-9FAC-4B83-94B7-9C2F8C662292}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1922,108 +2242,204 @@
       <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO treatments (",A1,",",B1,",",C1,",",D1,",",E1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>85</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",""",
+B2,""",""",
+C2,""",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
+        <v>(1,"Physical exam","6","44538","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>86</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>44539</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G8" ca="1" si="1">_xlfn.CONCAT("(",
+A3,",""",
+B3,""",""",
+C3,""",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
+        <v>(2,"Blood work","3","44539","2"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>87</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(3,"Da2pp","1","44540","5"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>88</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(4,"dental cleaning","1","44538","3"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>89</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(5,"drontal deworm","2","44539","4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>90</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(6,"rabies vaccination","1","44540","2"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>91</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
       </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8,",""",
+B8,""",""",
+C8,""",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
+        <v>(7,"Revolution treatment","3","44538","4");</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E769BC6-8AA4-47AC-8CDF-52C74C698B1A}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2041,6 +2457,195 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO issues (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_animalid,i_detecteddate,i_raisedby,i_isresolved) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44538</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")), ",""",
+C2,""",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),"","),")</f>
+        <v>(1,"Limp Walk","2","44538","1","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44177</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H2:H6" ca="1" si="1">_xlfn.CONCAT("(",
+A3,",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")), ",""",
+C3,""",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"","),")</f>
+        <v>(2,NULL,"2","44177","1","1"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44332</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(3,"Diabetes","3","44332","2","0"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44345</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(4,"Inflammed limb","2","44345","1",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(5,"Bladder Infection","1",NULL,"5",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44517</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A7,",",
+IF(B7="","NULL",_xlfn.CONCAT("""",B7,"""")), ",""",
+C7,""",",
+IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),",",
+IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
+IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),"","),")</f>
+        <v>(6,"chronic kidney disease","6","44517","3","0"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44517</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8, ",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")), ",""",
+C8, """,",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")), ",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),"",")",";")</f>
+        <v>(7,"Upset Stomach","5","44517","2",NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -2050,16 +2655,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18B5F6C-A8DA-4DBA-AEF7-E7170CF7C840}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -2074,6 +2683,177 @@
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="G1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO comments (",A1,",",B1,",",C1,",",D1,",",E1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO comments (c_commentid,c_commentdesc,c_animalid,c_commentdate,c_commenter) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44538</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",",
+IF(B2="","""No Comment Provided""",_xlfn.CONCAT("""",B2,"""")), ",""",
+C2,""",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
+        <v>(1,"Nighttime terror","1","44538","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44539</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
+A3,",",
+IF(B3="","""No Comment Provided""",_xlfn.CONCAT("""",B3,"""")), ",""",
+C3,""",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
+        <v>(2,"Howling ","4","44539","5"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44540</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>(3,"Pregnant ","3","44540","1"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44538</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>(4,"No Comment Provided","7","44538","2"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44539</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>(5,"No Comment Provided","4","44539","6"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44540</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>(6,"No Comment Provided","1","44540","4"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44538</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8,",",
+IF(B8="","""No Comment Provided""",_xlfn.CONCAT("""",B8,"""")), ",""",
+C8,""",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
+        <v>(7,"Not sleeping","7","44538","1");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build: [U888-62] changing user names to distinguish from owners
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarangkumar/Documents/Software/Fall 2021/ENSF607/Course Project/ensf-607-608-project/sql/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B496310-9AE1-1745-8FCF-DC55D98371F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C06394-31D5-4493-8BB7-5EC300DBA95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="720" windowWidth="31100" windowHeight="19480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animals" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="124">
   <si>
     <t>a_animalid</t>
   </si>
@@ -364,43 +366,52 @@
     <t>image5.png</t>
   </si>
   <si>
-    <t>Tony</t>
-  </si>
-  <si>
-    <t>Stark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billy </t>
-  </si>
-  <si>
-    <t>Ray</t>
-  </si>
-  <si>
-    <t>Cyrus</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Homer</t>
-  </si>
-  <si>
-    <t>Simposon</t>
-  </si>
-  <si>
-    <t>Miley</t>
-  </si>
-  <si>
-    <t>Chris</t>
-  </si>
-  <si>
-    <t>Lighter</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Boorman</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Attendant</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>passw0rd</t>
+  </si>
+  <si>
+    <t>u_email</t>
+  </si>
+  <si>
+    <t>u_password</t>
+  </si>
+  <si>
+    <t>u_status</t>
   </si>
 </sst>
 </file>
@@ -1257,17 +1268,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="10.83203125" customWidth="1"/>
-    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="13" width="10.77734375" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_type,a_breed,a_birthdate,a_sex,a_status,a_ownerid,a_tattoonum,a_rfidnumber,a_microchipnumber,a_weight,a_coatcolor,a_continuousmedication) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1330,26 +1339,26 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>165835067</v>
+        <v>138039084</v>
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>247543542</v>
+        <v>285536264</v>
       </c>
       <c r="K2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>319807825</v>
+        <v>277546517</v>
       </c>
       <c r="M2" t="s">
         <v>72</v>
@@ -1370,10 +1379,10 @@
 IF(L2="","NULL",_xlfn.CONCAT("""",L2,"""")), ",""",
 M2, """,",
 IF(N2="","NULL",_xlfn.CONCAT("""",N2,"""")), "),")</f>
-        <v>(1,"Ace","Dog","German shepherd",NULL,"0",1,1,165835067,"247543542","319807825",NULL,"Black",NULL),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>(1,"Ace","Dog","German shepherd",NULL,"1",3,1,138039084,"285536264","277546517",NULL,"Black",NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1388,36 +1397,36 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G8" ca="1" si="2">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:K8" ca="1" si="3">RANDBETWEEN(123456789,345678912)</f>
-        <v>264394967</v>
+        <v>194727122</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="3"/>
-        <v>257881478</v>
+        <v>260056280</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="3"/>
-        <v>208784783</v>
+        <v>188889486</v>
       </c>
       <c r="M3" t="s">
         <v>66</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(2,"Ampersand","Monkey","Capuchin monkey",NULL,"0",1,2,264394967,"257881478","208784783",NULL,"Brown",NULL),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>(2,"Ampersand","Monkey","Capuchin monkey",NULL,"1",3,2,194727122,"260056280","188889486",NULL,"Brown",NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1429,36 +1438,36 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>263603009</v>
+        <v>139497739</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="3"/>
-        <v>222088925</v>
+        <v>151077950</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="3"/>
-        <v>314011986</v>
+        <v>312442503</v>
       </c>
       <c r="M4" t="s">
         <v>73</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(3,"Bat Cow","Cow",NULL,NULL,"0",2,1,263603009,"222088925","314011986",NULL,"Brown, White",NULL),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>(3,"Bat Cow","Cow",NULL,NULL,"1",1,1,139497739,"151077950","312442503",NULL,"Brown, White",NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1477,32 +1486,32 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="3"/>
-        <v>208704960</v>
+        <v>253209323</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="3"/>
-        <v>247473515</v>
+        <v>305652047</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="3"/>
-        <v>226898378</v>
+        <v>201438972</v>
       </c>
       <c r="M5" t="s">
         <v>74</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(4,"Comet","Horse","Canadian horse",NULL,"1",1,3,208704960,"247473515","226898378",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>(4,"Comet","Horse","Canadian horse",NULL,"1",0,3,253209323,"305652047","201438972",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1521,32 +1530,32 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
-        <v>266888163</v>
+        <v>210159141</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="3"/>
-        <v>288875156</v>
+        <v>306907987</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="3"/>
-        <v>235082133</v>
+        <v>126906260</v>
       </c>
       <c r="M6" t="s">
         <v>74</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(5,"Krypto","Dog","Labrador retriever",NULL,"1",0,3,266888163,"288875156","235082133",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>(5,"Krypto","Dog","Labrador retriever",NULL,"1",3,3,210159141,"306907987","126906260",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1565,32 +1574,32 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
-        <v>306112853</v>
+        <v>318552784</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="3"/>
-        <v>134150622</v>
+        <v>135395544</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="3"/>
-        <v>323373371</v>
+        <v>253799414</v>
       </c>
       <c r="M7" t="s">
         <v>74</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(6,"Snowy","Dog","Wire Fox Terrier",NULL,"0",3,4,306112853,"134150622","323373371",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>(6,"Snowy","Dog","Wire Fox Terrier",NULL,"0",1,4,318552784,"135395544","253799414",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1605,26 +1614,26 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
-        <v>148452974</v>
+        <v>195074624</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="3"/>
-        <v>342360641</v>
+        <v>124340346</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="3"/>
-        <v>136678103</v>
+        <v>217603266</v>
       </c>
       <c r="M8" t="s">
         <v>75</v>
@@ -1645,7 +1654,7 @@
 IF(L8="","NULL",_xlfn.CONCAT("""",L8,"""")), ",""",
 M8, """,",
 IF(N8="","NULL",_xlfn.CONCAT("""",N8,"""")), ");")</f>
-        <v>(7,"Streaky","Cat","Abyssinian",NULL,"0",2,3,148452974,"342360641","136678103",NULL,"Orange",NULL);</v>
+        <v>(7,"Streaky","Cat","Abyssinian",NULL,"1",1,3,195074624,"124340346","217603266",NULL,"Orange",NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -1658,18 +1667,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B2892-340A-4DA8-A00C-A7D7ACDCDE8B}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="1" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1699,7 +1706,7 @@
         <v xml:space="preserve">INSERT INTO owners (o_ownerid,o_firstname,o_middlename,o_lastname,o_role,o_contactnumber,o_emailid,o_address) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1714,7 +1721,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4031743423</v>
+        <v>4032418394</v>
       </c>
       <c r="G2" t="str">
         <f>_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
@@ -1725,10 +1732,10 @@
       </c>
       <c r="J2" t="str">
         <f ca="1">_xlfn.CONCAT("(",A2,",""",B2,""",""",C2,""",""",D2,""",",IF(E2="","NULL",E2),",""",F2,""",""",G2,""",""",H2,"""),")</f>
-        <v>(1,"Damian","Bruce","Wayne",NULL,"4031743423","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>(1,"Damian","Bruce","Wayne",NULL,"4032418394","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1740,7 +1747,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F7" ca="1" si="0">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4033906233</v>
+        <v>4035456532</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" si="1">_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
@@ -1748,10 +1755,10 @@
       </c>
       <c r="J3" t="str">
         <f ca="1">_xlfn.CONCAT("(",A3,",""",B3,""",""",C3,""",""",D3,""",",IF(E3="","NULL",E3),",""",F3,""",""",G3,""",""",H3,"""),")</f>
-        <v>(2,"Yorrick","","Brown",NULL,"4033906233","yorrick.brown@ucalgary.ca",""),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>(2,"Yorrick","","Brown",NULL,"4035456532","yorrick.brown@ucalgary.ca",""),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1766,7 +1773,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>4031617502</v>
+        <v>4032691400</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
@@ -1777,10 +1784,10 @@
       </c>
       <c r="J4" t="str">
         <f ca="1">_xlfn.CONCAT("(",A4,",""",B4,""",""",C4,""",""",D4,""",",IF(E4="","NULL",E4),",""",F4,""",""",G4,""",""",H4,"""),")</f>
-        <v>(3,"Clark","Joseph","Kent",NULL,"4031617502","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>(3,"Clark","Joseph","Kent",NULL,"4032691400","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1789,7 +1796,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4039872693</v>
+        <v>4036339516</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -1800,10 +1807,10 @@
       </c>
       <c r="J5" t="str">
         <f ca="1">_xlfn.CONCAT("(",A5,",""",B5,""",""",C5,""",""",D5,""",",IF(E5="","NULL",E5),",""",F5,""",""",G5,""",""",H5,"""),")</f>
-        <v>(4,"Tintin","","",NULL,"4039872693","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>(4,"Tintin","","",NULL,"4036339516","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1815,7 +1822,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4039960231</v>
+        <v>4037379697</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -1826,10 +1833,10 @@
       </c>
       <c r="J6" t="str">
         <f ca="1">_xlfn.CONCAT("(",A6,",""",B6,""",""",C6,""",""",D6,""",",IF(E6="","NULL",E6),",""",F6,""",""",G6,""",""",H6,"""),")</f>
-        <v>(5,"UCalgary","","",0,"4039960231","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>(5,"UCalgary","","",0,"4037379697","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1839,9 +1846,12 @@
       <c r="D7" t="s">
         <v>78</v>
       </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4034565624</v>
+        <v>4039747282</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -1852,7 +1862,7 @@
       </c>
       <c r="J7" t="str">
         <f ca="1">_xlfn.CONCAT("(",A7,",""",B7,""",""",C7,""",""",D7,""",",IF(E7="","NULL",E7),",""",F7,""",""",G7,""",""",H7,""");")</f>
-        <v>(6,"James","","Gunn",NULL,"4034565624","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+        <v>(6,"James","","Gunn",2,"4039747282","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
       </c>
     </row>
   </sheetData>
@@ -1862,18 +1872,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A0186-44D9-498E-B660-5B0A566DD134}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="10.83203125" customWidth="1"/>
+    <col min="1" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -1890,147 +1900,204 @@
         <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO users (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,",",H1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO users (u_userid,u_firstname,u_middlename,u_lastname,u_role,u_email,u_password,u_status) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
+        <v>greg.boorman@ucalgary.ca</v>
+      </c>
+      <c r="G2" t="s">
         <v>120</v>
       </c>
-      <c r="I1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO owners (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO owners (u_userid,u_firstname,u_middlename,u_lastname,u_role,email,password) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="str">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
         <f>_xlfn.CONCAT("(",
 A2,",""",
 B2,""",",
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
-        <v>(1,"Damian","Bruce","Wayne","1"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+E2,",""",
+F2,""",""",
+G2,""",",
+H2,"),")</f>
+        <v>(1,"Greg",NULL,"Boorman",0,"greg.boorman@ucalgary.ca","passw0rd",1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I7" si="0">_xlfn.CONCAT("(",
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F8" si="0">_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
+        <v>teacher.admin@ucalgary.ca</v>
+      </c>
+      <c r="G3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J7" si="1">_xlfn.CONCAT("(",
 A3,",""",
 B3,""",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
-        <v>(2,"Tony",NULL,"Stark","2"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+E3,",""",
+F3,""",""",
+G3,""",",
+H3,"),")</f>
+        <v>(2,"Teacher",NULL,"Admin",0,"teacher.admin@ucalgary.ca","passw0rd",0),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="I4" t="str">
+        <v>2</v>
+      </c>
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>(3,"Clark","Joseph","Kent","3"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>technician.a@ucalgary.ca</v>
+      </c>
+      <c r="G4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,"Technician",NULL,"A",2,"technician.a@ucalgary.ca","passw0rd",0),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
         <v>112</v>
       </c>
       <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="I5" t="str">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>(4,"Billy ","Ray","Cyrus","2"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>attendant.b@ucalgary.ca</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,"Attendant",NULL,"B",1,"attendant.b@ucalgary.ca","passw0rd",0),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="str">
+        <v>3</v>
+      </c>
+      <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>(5,"Bob","Homer","Simposon","2"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>teacher.c@ucalgary.ca</v>
+      </c>
+      <c r="G6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,"Teacher",NULL,"C",3,"teacher.c@ucalgary.ca","passw0rd",0),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" t="s">
-        <v>111</v>
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>118</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="str">
+        <v>4</v>
+      </c>
+      <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>(6,"Miley","Ray",NULL,"1"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>student.d@ucalgary.ca</v>
+      </c>
+      <c r="G7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,"Student",NULL,"D",4,"student.d@ucalgary.ca","passw0rd",0),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2038,19 +2105,32 @@
         <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="I8" t="str">
+        <v>4</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>student.e@ucalgary.ca</v>
+      </c>
+      <c r="G8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
         <f>_xlfn.CONCAT("(",
 A8,",""",
 B8,""",",
 IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
-        <v>(7,"Chris",NULL,"Lighter","2");</v>
+E8,",""",
+F8,""",""",
+G8,""",",
+H8,");")</f>
+        <v>(7,"Student",NULL,"E",4,"student.e@ucalgary.ca","passw0rd",0);</v>
       </c>
     </row>
   </sheetData>
@@ -2062,16 +2142,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4EAFE5-CE5B-467E-B9FE-9E32C463D99E}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" customWidth="1"/>
+    <col min="1" max="3" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -2086,7 +2164,7 @@
         <v xml:space="preserve">INSERT INTO photos (p_photoid,p_animalid,p_photolink) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2105,13 +2183,13 @@
         <v>(1,"3","image1.png"),</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
@@ -2121,71 +2199,71 @@
 A3,",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),"","),")</f>
-        <v>(2,"5","image2.png"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>(2,"6","image2.png"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>104</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(3,"7","image4.png"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>(3,"6","image4.png"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(4,"7",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>(4,"1",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>105</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(5,"3","image7.png"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>(5,"1","image7.png"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>106</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(6,"6","image6.png"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>(6,"5","image6.png"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2213,20 +2291,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B89DC6B-9FAC-4B83-94B7-9C2F8C662292}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -2247,7 +2323,7 @@
         <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2274,7 +2350,7 @@
         <v>(1,"Physical exam","6","44538","1"),</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2292,7 +2368,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G8" ca="1" si="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="G3:G7" ca="1" si="1">_xlfn.CONCAT("(",
 A3,",""",
 B3,""",""",
 C3,""",",
@@ -2301,7 +2377,7 @@
         <v>(2,"Blood work","3","44539","2"),</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2310,7 +2386,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
@@ -2320,10 +2396,10 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(3,"Da2pp","1","44540","5"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(3,"Da2pp","7","44540","5"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2345,7 +2421,7 @@
         <v>(4,"dental cleaning","1","44538","3"),</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2354,7 +2430,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
@@ -2364,10 +2440,10 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(5,"drontal deworm","2","44539","4"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(5,"drontal deworm","5","44539","4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2376,7 +2452,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
@@ -2386,10 +2462,10 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(6,"rabies vaccination","1","44540","2"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(6,"rabies vaccination","2","44540","2"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2398,7 +2474,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
@@ -2413,7 +2489,7 @@
 C8,""",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
-        <v>(7,"Revolution treatment","3","44538","4");</v>
+        <v>(7,"Revolution treatment","2","44538","4");</v>
       </c>
     </row>
   </sheetData>
@@ -2426,20 +2502,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E769BC6-8AA4-47AC-8CDF-52C74C698B1A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" customWidth="1"/>
+    <col min="5" max="6" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2463,7 +2537,7 @@
         <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_animalid,i_detecteddate,i_raisedby,i_isresolved) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2494,13 +2568,13 @@
         <v>(1,"Limp Walk","2","44538","1","1"),</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>44177</v>
@@ -2512,17 +2586,17 @@
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H2:H6" ca="1" si="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="H3:H6" ca="1" si="1">_xlfn.CONCAT("(",
 A3,",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")), ",""",
 C3,""",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"","),")</f>
-        <v>(2,NULL,"2","44177","1","1"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>(2,NULL,"7","44177","1","1"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2547,7 +2621,7 @@
         <v>(3,"Diabetes","3","44332","2","0"),</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2556,7 +2630,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>44345</v>
@@ -2566,10 +2640,10 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(4,"Inflammed limb","2","44345","1",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>(4,"Inflammed limb","1","44345","1",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2578,7 +2652,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
@@ -2586,10 +2660,10 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(5,"Bladder Infection","1",NULL,"5",NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>(5,"Bladder Infection","5",NULL,"5",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2598,7 +2672,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>44517</v>
@@ -2617,10 +2691,10 @@
 IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),",",
 IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
 IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),"","),")</f>
-        <v>(6,"chronic kidney disease","6","44517","3","0"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>(6,"chronic kidney disease","1","44517","3","0"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2629,7 +2703,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>44517</v>
@@ -2645,7 +2719,7 @@
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")), ",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),"",")",";")</f>
-        <v>(7,"Upset Stomach","5","44517","2",NULL);</v>
+        <v>(7,"Upset Stomach","6","44517","2",NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -2661,14 +2735,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -2689,7 +2763,7 @@
         <v xml:space="preserve">INSERT INTO comments (c_commentid,c_commentdesc,c_animalid,c_commentdate,c_commenter) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2698,14 +2772,14 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2714,10 +2788,10 @@
 C2,""",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
-        <v>(1,"Nighttime terror","1","44538","1"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(1,"Nighttime terror","3","44538","7"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2733,7 +2807,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
@@ -2742,10 +2816,10 @@
 C3,""",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
-        <v>(2,"Howling ","4","44539","5"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(2,"Howling ","4","44539","3"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2754,41 +2828,41 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(3,"Pregnant ","3","44540","1"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(3,"Pregnant ","6","44540","4"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(4,"No Comment Provided","7","44538","2"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(4,"No Comment Provided","5","44538","7"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2801,34 +2875,34 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(5,"No Comment Provided","4","44539","6"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(5,"No Comment Provided","4","44539","2"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(6,"No Comment Provided","1","44540","4"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>(6,"No Comment Provided","2","44540","5"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2844,7 +2918,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2853,7 +2927,7 @@
 C8,""",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
-        <v>(7,"Not sleeping","7","44538","1");</v>
+        <v>(7,"Not sleeping","7","44538","2");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: [U888-62] added additional columns in excel
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C06394-31D5-4493-8BB7-5EC300DBA95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B8F7C7-8BA9-490D-8485-2161BBD4138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animals" sheetId="1" r:id="rId1"/>
     <sheet name="owners" sheetId="6" r:id="rId2"/>
     <sheet name="users" sheetId="7" r:id="rId3"/>
-    <sheet name="photos" sheetId="5" r:id="rId4"/>
-    <sheet name="treatments" sheetId="4" r:id="rId5"/>
-    <sheet name="issues" sheetId="3" r:id="rId6"/>
-    <sheet name="comments" sheetId="2" r:id="rId7"/>
+    <sheet name="weights" sheetId="8" r:id="rId4"/>
+    <sheet name="photos" sheetId="5" r:id="rId5"/>
+    <sheet name="comments" sheetId="2" r:id="rId6"/>
+    <sheet name="issues" sheetId="3" r:id="rId7"/>
+    <sheet name="treatments" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">animals!$A$1:$N$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">animals!$A$1:$S$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="145">
   <si>
     <t>a_animalid</t>
   </si>
@@ -78,9 +79,6 @@
     <t>a_tattoonum</t>
   </si>
   <si>
-    <t>a_weight</t>
-  </si>
-  <si>
     <t>c_animalid</t>
   </si>
   <si>
@@ -135,9 +133,6 @@
     <t>o_ownerid</t>
   </si>
   <si>
-    <t>o_role</t>
-  </si>
-  <si>
     <t>u_firstname</t>
   </si>
   <si>
@@ -408,10 +403,79 @@
     <t>u_email</t>
   </si>
   <si>
-    <t>u_password</t>
-  </si>
-  <si>
     <t>u_status</t>
+  </si>
+  <si>
+    <t>w_weightid</t>
+  </si>
+  <si>
+    <t>w_animalid</t>
+  </si>
+  <si>
+    <t>w_recorddate</t>
+  </si>
+  <si>
+    <t>w_massinkg</t>
+  </si>
+  <si>
+    <t>w_recordedby</t>
+  </si>
+  <si>
+    <t>a_species</t>
+  </si>
+  <si>
+    <t>a_subspecies</t>
+  </si>
+  <si>
+    <t>a_region</t>
+  </si>
+  <si>
+    <t>a_profilepic</t>
+  </si>
+  <si>
+    <t>a_citytattoo</t>
+  </si>
+  <si>
+    <t>a_distinctfeature</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>u_joiningdate</t>
+  </si>
+  <si>
+    <t>u_activationdate</t>
+  </si>
+  <si>
+    <t>u_terminationdate</t>
+  </si>
+  <si>
+    <t>u_passwordhash</t>
+  </si>
+  <si>
+    <t>u_passwordsalt</t>
+  </si>
+  <si>
+    <t>p_photodesc</t>
+  </si>
+  <si>
+    <t>p_alttext</t>
+  </si>
+  <si>
+    <t>p_uploader</t>
+  </si>
+  <si>
+    <t>p_uploaddate</t>
+  </si>
+  <si>
+    <t>t_drugname</t>
+  </si>
+  <si>
+    <t>t_drugdose</t>
+  </si>
+  <si>
+    <t>t_deliverymethod</t>
   </si>
 </sst>
 </file>
@@ -1266,17 +1330,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="10.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,377 +1365,465 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO animals (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,",",H1,",",I1,",",J1,",",K1,",",L1,",",M1,",",N1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_type,a_breed,a_birthdate,a_sex,a_status,a_ownerid,a_tattoonum,a_rfidnumber,a_microchipnumber,a_weight,a_coatcolor,a_continuousmedication) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO animals (",A1,",",B1,",",F1,",",E1,",",I1,",",H1,",",J1,",",K1,",",M1,",",O1,",",P1,",",S1,",",Q1,",",R1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_type,a_breed,a_birthdate,a_sex,a_status,a_ownerid,a_tattoonum,a_rfidnumber,a_microchipnumber,a_distinctfeature,a_coatcolor,a_continuousmedication) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2">
         <f ca="1">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>3</v>
-      </c>
-      <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>138039084</v>
-      </c>
-      <c r="J2">
+        <v>290496842</v>
+      </c>
+      <c r="O2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>285536264</v>
-      </c>
-      <c r="K2">
+        <v>239725619</v>
+      </c>
+      <c r="P2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>277546517</v>
-      </c>
-      <c r="M2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P2" t="str">
-        <f t="shared" ref="P2:P7" ca="1" si="0">_xlfn.CONCAT("(",
+        <v>220683862</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
 A2, ",""",
 B2, """,""",
-C2, """,",
-IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")), ",",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")), ",""",
 F2, """,",
-G2, ",",
-H2, ",",
-I2, ",""",
-J2, """,""",
-K2, """,",
-IF(L2="","NULL",_xlfn.CONCAT("""",L2,"""")), ",""",
-M2, """,",
-IF(N2="","NULL",_xlfn.CONCAT("""",N2,"""")), "),")</f>
-        <v>(1,"Ace","Dog","German shepherd",NULL,"1",3,1,138039084,"285536264","277546517",NULL,"Black",NULL),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")), ",",
+IF(I2="","NULL",_xlfn.CONCAT("""",I2,"""")), ",""",
+H2, """,",
+J2, ",",
+K2, ",",
+M2, ",""",
+O2, """,""",
+P2, """,",
+IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")), ",""",
+Q2, """,",
+IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")), "),")</f>
+        <v>(1,"Ace","","German shepherd",NULL,"1",1,1,290496842,"239725619","220683862",NULL,"Black",NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" ca="1" si="2">RANDBETWEEN(0,3)</f>
-        <v>3</v>
-      </c>
       <c r="H3">
+        <f t="shared" ref="H3:H8" ca="1" si="0">RANDBETWEEN(0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" ca="1" si="1">RANDBETWEEN(0,3)</f>
         <v>2</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:K8" ca="1" si="3">RANDBETWEEN(123456789,345678912)</f>
-        <v>194727122</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ca="1" si="3"/>
-        <v>260056280</v>
-      </c>
       <c r="K3">
-        <f t="shared" ca="1" si="3"/>
-        <v>188889486</v>
-      </c>
-      <c r="M3" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(2,"Ampersand","Monkey","Capuchin monkey",NULL,"1",3,2,194727122,"260056280","188889486",NULL,"Brown",NULL),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:P8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
+        <v>242471416</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ca="1" si="2"/>
+        <v>284231022</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ca="1" si="2"/>
+        <v>205149893</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A3, ",""",
+B3, """,""",
+F3, """,",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")), ",",
+IF(I3="","NULL",_xlfn.CONCAT("""",I3,"""")), ",""",
+H3, """,",
+J3, ",",
+K3, ",",
+M3, ",""",
+O3, """,""",
+P3, """,",
+IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")), ",""",
+Q3, """,",
+IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")), "),")</f>
+        <v>(2,"Ampersand","","Capuchin monkey",NULL,"0",2,2,242471416,"284231022","205149893",NULL,"Brown",NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="M4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <f t="shared" ca="1" si="3"/>
-        <v>139497739</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ca="1" si="3"/>
-        <v>151077950</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ca="1" si="3"/>
-        <v>312442503</v>
-      </c>
-      <c r="M4" t="s">
-        <v>73</v>
-      </c>
-      <c r="P4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(3,"Bat Cow","Cow",NULL,NULL,"1",1,1,139497739,"151077950","312442503",NULL,"Brown, White",NULL),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>342414252</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ca="1" si="2"/>
+        <v>283226903</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ca="1" si="2"/>
+        <v>162866305</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A4, ",""",
+B4, """,""",
+F4, """,",
+IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")), ",",
+IF(I4="","NULL",_xlfn.CONCAT("""",I4,"""")), ",""",
+H4, """,",
+J4, ",",
+K4, ",",
+M4, ",""",
+O4, """,""",
+P4, """,",
+IF(S4="","NULL",_xlfn.CONCAT("""",S4,"""")), ",""",
+Q4, """,",
+IF(R4="","NULL",_xlfn.CONCAT("""",R4,"""")), "),")</f>
+        <v>(3,"Bat Cow","Dairy",NULL,NULL,"0",0,1,342414252,"283226903","162866305",NULL,"Brown, White",NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="M5">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ca="1" si="3"/>
-        <v>253209323</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ca="1" si="3"/>
-        <v>305652047</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ca="1" si="3"/>
-        <v>201438972</v>
-      </c>
-      <c r="M5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(4,"Comet","Horse","Canadian horse",NULL,"1",0,3,253209323,"305652047","201438972",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>330261357</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="2"/>
+        <v>328276606</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ca="1" si="2"/>
+        <v>137148850</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A5, ",""",
+B5, """,""",
+F5, """,",
+IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")), ",",
+IF(I5="","NULL",_xlfn.CONCAT("""",I5,"""")), ",""",
+H5, """,",
+J5, ",",
+K5, ",",
+M5, ",""",
+O5, """,""",
+P5, """,",
+IF(S5="","NULL",_xlfn.CONCAT("""",S5,"""")), ",""",
+Q5, """,",
+IF(R5="","NULL",_xlfn.CONCAT("""",R5,"""")), "),")</f>
+        <v>(4,"Comet","","Canadian horse",NULL,"0",3,3,330261357,"328276606","137148850",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="M6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ca="1" si="3"/>
-        <v>210159141</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ca="1" si="3"/>
-        <v>306907987</v>
-      </c>
-      <c r="K6">
-        <f t="shared" ca="1" si="3"/>
-        <v>126906260</v>
-      </c>
-      <c r="M6" t="s">
-        <v>74</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(5,"Krypto","Dog","Labrador retriever",NULL,"1",3,3,210159141,"306907987","126906260",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>304150765</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="2"/>
+        <v>290197552</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ca="1" si="2"/>
+        <v>211837689</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A6, ",""",
+B6, """,""",
+F6, """,",
+IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")), ",",
+IF(I6="","NULL",_xlfn.CONCAT("""",I6,"""")), ",""",
+H6, """,",
+J6, ",",
+K6, ",",
+M6, ",""",
+O6, """,""",
+P6, """,",
+IF(S6="","NULL",_xlfn.CONCAT("""",S6,"""")), ",""",
+Q6, """,",
+IF(R6="","NULL",_xlfn.CONCAT("""",R6,"""")), "),")</f>
+        <v>(5,"Krypto","","Labrador retriever",NULL,"0",2,3,304150765,"290197552","211837689",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="M7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ca="1" si="3"/>
-        <v>318552784</v>
-      </c>
-      <c r="J7">
-        <f t="shared" ca="1" si="3"/>
-        <v>135395544</v>
-      </c>
-      <c r="K7">
-        <f t="shared" ca="1" si="3"/>
-        <v>253799414</v>
-      </c>
-      <c r="M7" t="s">
-        <v>74</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(6,"Snowy","Dog","Wire Fox Terrier",NULL,"0",1,4,318552784,"135395544","253799414",NULL,"White",NULL),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>327208653</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="2"/>
+        <v>258909036</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ca="1" si="2"/>
+        <v>288072947</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A7, ",""",
+B7, """,""",
+F7, """,",
+IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")), ",",
+IF(I7="","NULL",_xlfn.CONCAT("""",I7,"""")), ",""",
+H7, """,",
+J7, ",",
+K7, ",",
+M7, ",""",
+O7, """,""",
+P7, """,",
+IF(S7="","NULL",_xlfn.CONCAT("""",S7,"""")), ",""",
+Q7, """,",
+IF(R7="","NULL",_xlfn.CONCAT("""",R7,"""")), "),")</f>
+        <v>(6,"Snowy","","Wire Fox Terrier",NULL,"0",0,4,327208653,"258909036","288072947",NULL,"White",NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="M8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ca="1" si="3"/>
-        <v>195074624</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ca="1" si="3"/>
-        <v>124340346</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ca="1" si="3"/>
-        <v>217603266</v>
-      </c>
-      <c r="M8" t="s">
-        <v>75</v>
-      </c>
-      <c r="P8" t="str">
+        <v>312583075</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="2"/>
+        <v>196013643</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ca="1" si="2"/>
+        <v>156362035</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>73</v>
+      </c>
+      <c r="U8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
 A8, ",""",
 B8, """,""",
-C8, """,",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")), ",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",""",
 F8, """,",
-G8, ",",
-H8, ",",
-I8, ",""",
-J8, """,""",
-K8, """,",
-IF(L8="","NULL",_xlfn.CONCAT("""",L8,"""")), ",""",
-M8, """,",
-IF(N8="","NULL",_xlfn.CONCAT("""",N8,"""")), ");")</f>
-        <v>(7,"Streaky","Cat","Abyssinian",NULL,"1",1,3,195074624,"124340346","217603266",NULL,"Orange",NULL);</v>
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
+IF(I8="","NULL",_xlfn.CONCAT("""",I8,"""")), ",""",
+H8, """,",
+J8, ",",
+K8, ",",
+M8, ",""",
+O8, """,""",
+P8, """,",
+IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")), ",""",
+Q8, """,",
+IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")), ");")</f>
+        <v>(7,"Streaky","","Abyssinian",NULL,"0",0,3,312583075,"196013643","156362035",NULL,"Orange",NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -1665,204 +1834,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B2892-340A-4DA8-A00C-A7D7ACDCDE8B}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="30.77734375" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="1" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO owners (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,",",H1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO owners (o_ownerid,o_firstname,o_middlename,o_lastname,o_role,o_contactnumber,o_emailid,o_address) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO owners (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO owners (o_ownerid,o_firstname,o_middlename,o_lastname,o_contactnumber,o_emailid,o_address) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
       <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2">
+        <v>58</v>
+      </c>
+      <c r="E2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4032418394</v>
-      </c>
-      <c r="G2" t="str">
+        <v>4033889224</v>
+      </c>
+      <c r="F2" t="str">
         <f>_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
         <v>damian.bruce.wayne@ucalgary.ca</v>
       </c>
-      <c r="H2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A2,",""",B2,""",""",C2,""",""",D2,""",",IF(E2="","NULL",E2),",""",F2,""",""",G2,""",""",H2,"""),")</f>
-        <v>(1,"Damian","Bruce","Wayne",NULL,"4032418394","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",A2,",""",B2,""",""",C2,""",""",D2,""",",",""",E2,""",""",F2,""",""",G2,"""),")</f>
+        <v>(1,"Damian","Bruce","Wayne",,"4033889224","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F7" ca="1" si="0">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4035456532</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G7" si="1">_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" ca="1" si="0">RANDBETWEEN(4031111111,4039999999)</f>
+        <v>4036511734</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
         <v>yorrick.brown@ucalgary.ca</v>
       </c>
-      <c r="J3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A3,",""",B3,""",""",C3,""",""",D3,""",",IF(E3="","NULL",E3),",""",F3,""",""",G3,""",""",H3,"""),")</f>
-        <v>(2,"Yorrick","","Brown",NULL,"4035456532","yorrick.brown@ucalgary.ca",""),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I3" t="str">
+        <f ca="1">_xlfn.CONCAT("(",A3,",""",B3,""",""",C3,""",""",D3,""",",",""",E3,""",""",F3,""",""",G3,"""),")</f>
+        <v>(2,"Yorrick","","Brown",,"4036511734","yorrick.brown@ucalgary.ca",""),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4031715373</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT(LOWER(B4),IF(C4="","",_xlfn.CONCAT(".",LOWER(C4))),IF(D4="","",_xlfn.CONCAT(".",LOWER(D4))),"@ucalgary.ca")</f>
+        <v>clark.joseph.kent@ucalgary.ca</v>
+      </c>
+      <c r="G4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>4032691400</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="1"/>
-        <v>clark.joseph.kent@ucalgary.ca</v>
-      </c>
-      <c r="H4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A4,",""",B4,""",""",C4,""",""",D4,""",",IF(E4="","NULL",E4),",""",F4,""",""",G4,""",""",H4,"""),")</f>
-        <v>(3,"Clark","Joseph","Kent",NULL,"4032691400","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I4" t="str">
+        <f ca="1">_xlfn.CONCAT("(",A4,",""",B4,""",""",C4,""",""",D4,""",",",""",E4,""",""",F4,""",""",G4,"""),")</f>
+        <v>(3,"Clark","Joseph","Kent",,"4031715373","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5">
+        <v>67</v>
+      </c>
+      <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>4036339516</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="1"/>
+        <v>4033987193</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(LOWER(B5),IF(C5="","",_xlfn.CONCAT(".",LOWER(C5))),IF(D5="","",_xlfn.CONCAT(".",LOWER(D5))),"@ucalgary.ca")</f>
         <v>tintin@ucalgary.ca</v>
       </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A5,",""",B5,""",""",C5,""",""",D5,""",",IF(E5="","NULL",E5),",""",F5,""",""",G5,""",""",H5,"""),")</f>
-        <v>(4,"Tintin","","",NULL,"4036339516","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="str">
+        <f ca="1">_xlfn.CONCAT("(",A5,",""",B5,""",""",C5,""",""",D5,""",",",""",E5,""",""",F5,""",""",G5,"""),")</f>
+        <v>(4,"Tintin","","",,"4033987193","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4037379697</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
+        <v>4031745433</v>
+      </c>
+      <c r="F6" t="str">
+        <f>_xlfn.CONCAT(LOWER(B6),IF(C6="","",_xlfn.CONCAT(".",LOWER(C6))),IF(D6="","",_xlfn.CONCAT(".",LOWER(D6))),"@ucalgary.ca")</f>
         <v>ucalgary@ucalgary.ca</v>
       </c>
-      <c r="H6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A6,",""",B6,""",""",C6,""",""",D6,""",",IF(E6="","NULL",E6),",""",F6,""",""",G6,""",""",H6,"""),")</f>
-        <v>(5,"UCalgary","","",0,"4037379697","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="str">
+        <f ca="1">_xlfn.CONCAT("(",A6,",""",B6,""",""",C6,""",""",D6,""",",",""",E6,""",""",F6,""",""",G6,"""),")</f>
+        <v>(5,"UCalgary","","",,"4031745433","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4039747282</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
+        <v>4034877564</v>
+      </c>
+      <c r="F7" t="str">
+        <f>_xlfn.CONCAT(LOWER(B7),IF(C7="","",_xlfn.CONCAT(".",LOWER(C7))),IF(D7="","",_xlfn.CONCAT(".",LOWER(D7))),"@ucalgary.ca")</f>
         <v>james.gunn@ucalgary.ca</v>
       </c>
-      <c r="H7" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A7,",""",B7,""",""",C7,""",""",D7,""",",IF(E7="","NULL",E7),",""",F7,""",""",G7,""",""",H7,""");")</f>
-        <v>(6,"James","","Gunn",2,"4039747282","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" t="str">
+        <f ca="1">_xlfn.CONCAT("(",A7,",""",B7,""",""",C7,""",""",D7,""",",",""",E7,""",""",F7,""",""",G7,""");")</f>
+        <v>(6,"James","","Gunn",,"4034877564","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
       </c>
     </row>
   </sheetData>
@@ -1872,264 +2032,276 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A0186-44D9-498E-B660-5B0A566DD134}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.77734375" customWidth="1"/>
+    <col min="1" max="8" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO users (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,",",H1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO users (u_userid,u_firstname,u_middlename,u_lastname,u_role,u_email,u_password,u_status) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO users (",A1,",",E1,",",F1,",",G1,",",H1,",",I1,",",J1,",",L1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO users (u_userid,u_firstname,u_middlename,u_lastname,u_role,u_email,u_passwordhash,u_status) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="F2" t="str">
-        <f>_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT(LOWER(E2),IF(F2="","",_xlfn.CONCAT(".",LOWER(F2))),IF(G2="","",_xlfn.CONCAT(".",LOWER(G2))),"@ucalgary.ca")</f>
         <v>greg.boorman@ucalgary.ca</v>
       </c>
-      <c r="G2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H2">
+      <c r="J2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="J2" t="str">
+      <c r="N2" t="str">
         <f>_xlfn.CONCAT("(",
 A2,",""",
-B2,""",",
-IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
-IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
-E2,",""",
-F2,""",""",
-G2,""",",
-H2,"),")</f>
+E2,""",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
+H2,",""",
+I2,""",""",
+J2,""",",
+L2,"),")</f>
         <v>(1,"Greg",NULL,"Boorman",0,"greg.boorman@ucalgary.ca","passw0rd",1),</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F8" si="0">_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
-        <v>teacher.admin@ucalgary.ca</v>
+      <c r="E3" t="s">
+        <v>108</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J7" si="1">_xlfn.CONCAT("(",
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I8" si="0">_xlfn.CONCAT(LOWER(E3),IF(F3="","",_xlfn.CONCAT(".",LOWER(F3))),IF(G3="","",_xlfn.CONCAT(".",LOWER(G3))),"@ucalgary.ca")</f>
+        <v>teacher.admin@ucalgary.ca</v>
+      </c>
+      <c r="J3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N7" si="1">_xlfn.CONCAT("(",
 A3,",""",
-B3,""",",
-IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
-E3,",""",
-F3,""",""",
-G3,""",",
-H3,"),")</f>
+E3,""",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
+IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
+H3,",""",
+I3,""",""",
+J3,""",",
+L3,"),")</f>
         <v>(2,"Teacher",NULL,"Admin",0,"teacher.admin@ucalgary.ca","passw0rd",0),</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>111</v>
       </c>
-      <c r="E4">
+      <c r="G4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="F4" t="str">
+      <c r="I4" t="str">
         <f t="shared" si="0"/>
         <v>technician.a@ucalgary.ca</v>
       </c>
-      <c r="G4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4">
+      <c r="J4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
-      <c r="J4" t="str">
+      <c r="N4" t="str">
         <f t="shared" si="1"/>
         <v>(3,"Technician",NULL,"A",2,"technician.a@ucalgary.ca","passw0rd",0),</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="F5" t="str">
+      <c r="I5" t="str">
         <f t="shared" si="0"/>
         <v>attendant.b@ucalgary.ca</v>
       </c>
-      <c r="G5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5">
+      <c r="J5" t="s">
+        <v>118</v>
+      </c>
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="J5" t="str">
+      <c r="N5" t="str">
         <f t="shared" si="1"/>
         <v>(4,"Attendant",NULL,"B",1,"attendant.b@ucalgary.ca","passw0rd",0),</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="F6" t="str">
+      <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>teacher.c@ucalgary.ca</v>
       </c>
-      <c r="G6" t="s">
-        <v>120</v>
-      </c>
-      <c r="H6">
+      <c r="J6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="J6" t="str">
+      <c r="N6" t="str">
         <f t="shared" si="1"/>
         <v>(5,"Teacher",NULL,"C",3,"teacher.c@ucalgary.ca","passw0rd",0),</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="F7" t="str">
+      <c r="I7" t="str">
         <f t="shared" si="0"/>
         <v>student.d@ucalgary.ca</v>
       </c>
-      <c r="G7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H7">
+      <c r="J7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L7">
         <v>0</v>
       </c>
-      <c r="J7" t="str">
+      <c r="N7" t="str">
         <f t="shared" si="1"/>
         <v>(6,"Student",NULL,"D",4,"student.d@ucalgary.ca","passw0rd",0),</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
         <v>117</v>
       </c>
-      <c r="D8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8">
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="F8" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="0"/>
         <v>student.e@ucalgary.ca</v>
       </c>
-      <c r="G8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H8">
+      <c r="J8" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8">
         <v>0</v>
       </c>
-      <c r="J8" t="str">
+      <c r="N8" t="str">
         <f>_xlfn.CONCAT("(",
 A8,",""",
-B8,""",",
-IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
-E8,",""",
-F8,""",""",
-G8,""",",
-H8,");")</f>
+E8,""",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
+IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),",",
+H8,",""",
+I8,""",""",
+J8,""",",
+L8,");")</f>
         <v>(7,"Student",NULL,"E",4,"student.e@ucalgary.ca","passw0rd",0);</v>
       </c>
     </row>
@@ -2139,147 +2311,325 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3D06D0-BF1F-4225-AF4B-50DA628F29F9}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos (",A1,",",E1,",",C1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO photos (w_weightid,w_animalid,w_recorddate) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),"","),")</f>
+        <v>(1,"5",NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A3,",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),"","),")</f>
+        <v>(2,"1",NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A4,",",
+IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")),",",
+IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),"","),")</f>
+        <v>(3,"3",NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G5" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A5,",",
+IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")),",",
+IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),"","),")</f>
+        <v>(4,"5",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A6,",",
+IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")),",",
+IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),"","),")</f>
+        <v>(5,"3",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G7" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A7,",",
+IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
+IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),"","),")</f>
+        <v>(6,"7",NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8,",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),"",")",";")</f>
+        <v>(7,"1",NULL);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4EAFE5-CE5B-467E-B9FE-9E32C463D99E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="10.77734375" customWidth="1"/>
+    <col min="1" max="7" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO photos (",A1,",",B1,",",C1,") VALUES ")</f>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos (",A1,",",C1,",",D1,") VALUES ")</f>
         <v xml:space="preserve">INSERT INTO photos (p_photoid,p_animalid,p_photolink) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" t="str">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
 A2,",",
-IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
-IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),"","),")</f>
-        <v>(1,"3","image1.png"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),"","),")</f>
+        <v>(1,"7","image1.png"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E7" ca="1" si="1">_xlfn.CONCAT("(",
+      <c r="C3">
+        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
 A3,",",
-IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
-IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),"","),")</f>
-        <v>(2,"6","image2.png"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),"","),")</f>
+        <v>(2,"1","image2.png"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(3,"6","image4.png"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A4,",",
+IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),",",
+IF(D4="","NULL",_xlfn.CONCAT("""",D4,"""")),"","),")</f>
+        <v>(3,"3","image4.png"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(4,"1",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="I5" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A5,",",
+IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),",",
+IF(D5="","NULL",_xlfn.CONCAT("""",D5,"""")),"","),")</f>
+        <v>(4,"4",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(5,"1","image7.png"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A6,",",
+IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),",",
+IF(D6="","NULL",_xlfn.CONCAT("""",D6,"""")),"","),")</f>
+        <v>(5,"3","image7.png"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(6,"5","image6.png"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A7,",",
+IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),",",
+IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),"","),")</f>
+        <v>(6,"2","image6.png"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="str">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
 A8,",",
-IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
-IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),"",")",";")</f>
-        <v>(7,"4","image5.png");</v>
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),"",")",";")</f>
+        <v>(7,"3","image5.png");</v>
       </c>
     </row>
   </sheetData>
@@ -2287,453 +2637,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B89DC6B-9FAC-4B83-94B7-9C2F8C662292}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO treatments (",A1,",",B1,",",C1,",",D1,",",E1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2">
-        <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44538</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A2,",""",
-B2,""",""",
-C2,""",",
-IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
-        <v>(1,"Physical exam","6","44538","1"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44539</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G7" ca="1" si="1">_xlfn.CONCAT("(",
-A3,",""",
-B3,""",""",
-C3,""",",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
-        <v>(2,"Blood work","3","44539","2"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44540</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(3,"Da2pp","7","44540","5"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44538</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(4,"dental cleaning","1","44538","3"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44539</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(5,"drontal deworm","5","44539","4"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44540</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(6,"rabies vaccination","2","44540","2"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44538</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="G8" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A8,",""",
-B8,""",""",
-C8,""",",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
-        <v>(7,"Revolution treatment","2","44538","4");</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E769BC6-8AA4-47AC-8CDF-52C74C698B1A}">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="6" width="10.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO issues (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_animalid,i_detecteddate,i_raisedby,i_isresolved) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2">
-        <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44538</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A2,",",
-IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")), ",""",
-C2,""",",
-IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
-IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),"","),")</f>
-        <v>(1,"Limp Walk","2","44538","1","1"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44177</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H6" ca="1" si="1">_xlfn.CONCAT("(",
-A3,",",
-IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")), ",""",
-C3,""",",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
-IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"","),")</f>
-        <v>(2,NULL,"7","44177","1","1"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44332</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(3,"Diabetes","3","44332","2","0"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44345</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(4,"Inflammed limb","1","44345","1",NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>(5,"Bladder Infection","5",NULL,"5",NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44517</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A7,",",
-IF(B7="","NULL",_xlfn.CONCAT("""",B7,"""")), ",""",
-C7,""",",
-IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),",",
-IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
-IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),"","),")</f>
-        <v>(6,"chronic kidney disease","1","44517","3","0"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44517</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A8, ",",
-IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")), ",""",
-C8, """,",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")), ",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
-IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),"",")",";")</f>
-        <v>(7,"Upset Stomach","6","44517","2",NULL);</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18B5F6C-A8DA-4DBA-AEF7-E7170CF7C840}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2744,19 +2652,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO comments (",A1,",",B1,",",C1,",",D1,",",E1,") VALUES ")</f>
@@ -2768,18 +2676,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2788,7 +2696,7 @@
 C2,""",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
-        <v>(1,"Nighttime terror","3","44538","7"),</v>
+        <v>(1,"Nighttime terror","5","44538","2"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2796,18 +2704,18 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>44539</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
@@ -2816,7 +2724,7 @@
 C3,""",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
-        <v>(2,"Howling ","4","44539","3"),</v>
+        <v>(2,"Howling ","3","44539","7"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2824,7 +2732,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
@@ -2835,11 +2743,11 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(3,"Pregnant ","6","44540","4"),</v>
+        <v>(3,"Pregnant ","6","44540","2"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2848,18 +2756,18 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(4,"No Comment Provided","5","44538","7"),</v>
+        <v>(4,"No Comment Provided","1","44538","5"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2868,18 +2776,18 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(5,"No Comment Provided","4","44539","2"),</v>
+        <v>(5,"No Comment Provided","7","44539","5"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2907,11 +2815,11 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
@@ -2927,10 +2835,478 @@
 C8,""",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
-        <v>(7,"Not sleeping","7","44538","2");</v>
+        <v>(7,"Not sleeping","2","44538","2");</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E769BC6-8AA4-47AC-8CDF-52C74C698B1A}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="6" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO issues (",A1,",",B1,",",D1,",",C1,",",E1,",",F1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_animalid,i_detecteddate,i_raisedby,i_isresolved) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44538</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")), ",""",
+D2,""",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),"","),")</f>
+        <v>(1,"Limp Walk","1","44538","1","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44177</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A3,",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")), ",""",
+D3,""",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"","),")</f>
+        <v>(2,NULL,"7","44177","1","1"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44332</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A4,",",
+IF(B4="","NULL",_xlfn.CONCAT("""",B4,"""")), ",""",
+D4,""",",
+IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),",",
+IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")),",",
+IF(F4="","NULL",_xlfn.CONCAT("""",F4,"""")),"","),")</f>
+        <v>(3,"Diabetes","3","44332","2","0"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44345</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A5,",",
+IF(B5="","NULL",_xlfn.CONCAT("""",B5,"""")), ",""",
+D5,""",",
+IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),",",
+IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")),",",
+IF(F5="","NULL",_xlfn.CONCAT("""",F5,"""")),"","),")</f>
+        <v>(4,"Inflammed limb","6","44345","1",NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A6,",",
+IF(B6="","NULL",_xlfn.CONCAT("""",B6,"""")), ",""",
+D6,""",",
+IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),",",
+IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")),",",
+IF(F6="","NULL",_xlfn.CONCAT("""",F6,"""")),"","),")</f>
+        <v>(5,"Bladder Infection","6",NULL,"5",NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44517</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A7,",",
+IF(B7="","NULL",_xlfn.CONCAT("""",B7,"""")), ",""",
+D7,""",",
+IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),",",
+IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
+IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),"","),")</f>
+        <v>(6,"chronic kidney disease","3","44517","3","0"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44517</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8, ",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")), ",""",
+D8, """,",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")), ",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),"",")",";")</f>
+        <v>(7,"Upset Stomach","3","44517","2",NULL);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B89DC6B-9FAC-4B83-94B7-9C2F8C662292}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO treatments (",A1,",",B1,",",F1,",",G1,",",H1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44538</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A2,",""",
+B2,""",""",
+F2,""",",
+IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
+IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"","),")</f>
+        <v>(1,"Physical exam","7","44538","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44539</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J7" ca="1" si="1">_xlfn.CONCAT("(",
+A3,",""",
+B3,""",""",
+F3,""",",
+IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
+IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"","),")</f>
+        <v>(2,"Blood work","5","44539","2"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44540</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(3,"Da2pp","1","44540","5"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44538</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(4,"dental cleaning","4","44538","3"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44539</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(5,"drontal deworm","1","44539","4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44540</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>(6,"rabies vaccination","4","44540","2"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44538</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="J8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+A8,",""",
+B8,""",""",
+F8,""",",
+IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),",",
+IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),"",")",";")</f>
+        <v>(7,"Revolution treatment","7","44538","4");</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: [U888-62] updated excel formulas
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B8F7C7-8BA9-490D-8485-2161BBD4138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9F67C6-8C9F-4984-ADEC-167AB72A1127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="170">
   <si>
     <t>a_animalid</t>
   </si>
@@ -400,9 +400,6 @@
     <t>passw0rd</t>
   </si>
   <si>
-    <t>u_email</t>
-  </si>
-  <si>
     <t>u_status</t>
   </si>
   <si>
@@ -476,6 +473,84 @@
   </si>
   <si>
     <t>t_deliverymethod</t>
+  </si>
+  <si>
+    <t>sleeping pills</t>
+  </si>
+  <si>
+    <t>he can fly</t>
+  </si>
+  <si>
+    <t>HOC sha</t>
+  </si>
+  <si>
+    <t>ORE esd</t>
+  </si>
+  <si>
+    <t>NKN sds</t>
+  </si>
+  <si>
+    <t>HIS sdm</t>
+  </si>
+  <si>
+    <t>YSE mlc</t>
+  </si>
+  <si>
+    <t>JSD sda</t>
+  </si>
+  <si>
+    <t>DLF kjs</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Ape</t>
+  </si>
+  <si>
+    <t>Canine</t>
+  </si>
+  <si>
+    <t>Bovine</t>
+  </si>
+  <si>
+    <t>Feline</t>
+  </si>
+  <si>
+    <t>Gallopping</t>
+  </si>
+  <si>
+    <t>high jumps</t>
+  </si>
+  <si>
+    <t>bat-shaped patch on face</t>
+  </si>
+  <si>
+    <t>spotted</t>
+  </si>
+  <si>
+    <t>long ears</t>
+  </si>
+  <si>
+    <t>u_emailid</t>
   </si>
 </sst>
 </file>
@@ -1365,10 +1440,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1377,7 +1452,7 @@
         <v>43</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>9</v>
@@ -1392,13 +1467,13 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>8</v>
@@ -1413,11 +1488,30 @@
         <v>4</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO animals (",A1,",",B1,",",F1,",",E1,",",I1,",",H1,",",J1,",",K1,",",M1,",",O1,",",P1,",",S1,",",Q1,",",R1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_type,a_breed,a_birthdate,a_sex,a_status,a_ownerid,a_tattoonum,a_rfidnumber,a_microchipnumber,a_distinctfeature,a_coatcolor,a_continuousmedication) VALUES </v>
+        <f>_xlfn.CONCAT("INSERT INTO animals (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,",",
+G1,",",
+H1,",",
+I1,",",
+J1,",",
+K1,",",
+L1,",",
+M1,",",
+N1,",",
+O1,",",
+P1,",",
+Q1,",",
+S1,",",
+R1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_species,a_subspecies,a_breed,a_type,a_region,a_sex,a_birthdate,a_status,a_ownerid,a_profilepic,a_tattoonum,a_citytattoo,a_rfidnumber,a_microchipnumber,a_coatcolor,a_distinctfeature,a_continuousmedication) VALUES </v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -1430,52 +1524,75 @@
       <c r="C2" t="s">
         <v>46</v>
       </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
       <c r="E2" t="s">
         <v>61</v>
       </c>
+      <c r="G2" t="s">
+        <v>153</v>
+      </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>43070</v>
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="M2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>290496842</v>
+        <v>164519616</v>
+      </c>
+      <c r="N2" t="s">
+        <v>146</v>
       </c>
       <c r="O2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>239725619</v>
+        <v>193563577</v>
       </c>
       <c r="P2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>220683862</v>
+        <v>220698998</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
       </c>
+      <c r="R2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" t="s">
+        <v>145</v>
+      </c>
       <c r="U2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A2, ",""",
-B2, """,""",
-F2, """,",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")), ",",
-IF(I2="","NULL",_xlfn.CONCAT("""",I2,"""")), ",""",
-H2, """,",
-J2, ",",
-K2, ",",
-M2, ",""",
-O2, """,""",
-P2, """,",
-IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")), ",""",
-Q2, """,",
-IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")), "),")</f>
-        <v>(1,"Ace","","German shepherd",NULL,"1",1,1,290496842,"239725619","220683862",NULL,"Black",NULL),</v>
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
+IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),",",
+IF(I2="","NULL",_xlfn.CONCAT("""",TEXT(I2,"YYYY-MM-DD"),"""")),",",
+IF(J2="","NULL",_xlfn.CONCAT("""",J2,"""")),",",
+IF(K2="","NULL",_xlfn.CONCAT("""",K2,"""")),",",
+IF(L2="","NULL",_xlfn.CONCAT("""",L2,"""")),",",
+IF(M2="","NULL",_xlfn.CONCAT("""",M2,"""")),",",
+IF(N2="","NULL",_xlfn.CONCAT("""",N2,"""")),",",
+IF(O2="","NULL",_xlfn.CONCAT("""",O2,"""")),",",
+IF(P2="","NULL",_xlfn.CONCAT("""",P2,"""")),",",
+IF(Q2="","NULL",_xlfn.CONCAT("""",Q2,"""")),",",
+IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")),",",
+IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")),"),")</f>
+        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","0","2017-12-01","2","1",NULL,"164519616","HOC sha","193563577","220698998","Black","sleeping pills","he can fly"),</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -1488,52 +1605,72 @@
       <c r="C3" t="s">
         <v>55</v>
       </c>
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
       <c r="E3" t="s">
         <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>154</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H8" ca="1" si="0">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
+      <c r="I3" s="1">
+        <v>43436</v>
+      </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:P8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
-        <v>242471416</v>
+        <v>161174992</v>
+      </c>
+      <c r="N3" t="s">
+        <v>147</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="2"/>
-        <v>284231022</v>
+        <v>312602124</v>
       </c>
       <c r="P3">
         <f t="shared" ca="1" si="2"/>
-        <v>205149893</v>
+        <v>223632487</v>
       </c>
       <c r="Q3" t="s">
         <v>64</v>
       </c>
+      <c r="S3" t="s">
+        <v>165</v>
+      </c>
       <c r="U3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A3, ",""",
-B3, """,""",
-F3, """,",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")), ",",
-IF(I3="","NULL",_xlfn.CONCAT("""",I3,"""")), ",""",
-H3, """,",
-J3, ",",
-K3, ",",
-M3, ",""",
-O3, """,""",
-P3, """,",
-IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")), ",""",
-Q3, """,",
-IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")), "),")</f>
-        <v>(2,"Ampersand","","Capuchin monkey",NULL,"0",2,2,242471416,"284231022","205149893",NULL,"Brown",NULL),</v>
+        <f t="shared" ref="U3:U8" ca="1" si="3">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
+IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
+IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),",",
+IF(I3="","NULL",_xlfn.CONCAT("""",TEXT(I3,"YYYY-MM-DD"),"""")),",",
+IF(J3="","NULL",_xlfn.CONCAT("""",J3,"""")),",",
+IF(K3="","NULL",_xlfn.CONCAT("""",K3,"""")),",",
+IF(L3="","NULL",_xlfn.CONCAT("""",L3,"""")),",",
+IF(M3="","NULL",_xlfn.CONCAT("""",M3,"""")),",",
+IF(N3="","NULL",_xlfn.CONCAT("""",N3,"""")),",",
+IF(O3="","NULL",_xlfn.CONCAT("""",O3,"""")),",",
+IF(P3="","NULL",_xlfn.CONCAT("""",P3,"""")),",",
+IF(Q3="","NULL",_xlfn.CONCAT("""",Q3,"""")),",",
+IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")),",",
+IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")),"),")</f>
+        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","0","2018-12-02","0","2",NULL,"161174992","ORE esd","312602124","223632487","Brown",NULL,"high jumps"),</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -1546,12 +1683,21 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
+      <c r="D4" t="s">
+        <v>162</v>
+      </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="G4" t="s">
+        <v>156</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>43924</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
@@ -1562,36 +1708,28 @@
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="2"/>
-        <v>342414252</v>
+        <v>168429354</v>
+      </c>
+      <c r="N4" t="s">
+        <v>148</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="2"/>
-        <v>283226903</v>
+        <v>260294146</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="2"/>
-        <v>162866305</v>
+        <v>137251498</v>
       </c>
       <c r="Q4" t="s">
         <v>71</v>
       </c>
+      <c r="S4" t="s">
+        <v>166</v>
+      </c>
       <c r="U4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A4, ",""",
-B4, """,""",
-F4, """,",
-IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")), ",",
-IF(I4="","NULL",_xlfn.CONCAT("""",I4,"""")), ",""",
-H4, """,",
-J4, ",",
-K4, ",",
-M4, ",""",
-O4, """,""",
-P4, """,",
-IF(S4="","NULL",_xlfn.CONCAT("""",S4,"""")), ",""",
-Q4, """,",
-IF(R4="","NULL",_xlfn.CONCAT("""",R4,"""")), "),")</f>
-        <v>(3,"Bat Cow","Dairy",NULL,NULL,"0",0,1,342414252,"283226903","162866305",NULL,"Brown, White",NULL),</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","1","2020-04-03","0","1",NULL,"168429354","NKN sds","260294146","137251498","Brown, White",NULL,"bat-shaped patch on face"),</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -1604,13 +1742,22 @@
       <c r="C5" t="s">
         <v>45</v>
       </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
       <c r="E5" t="s">
         <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
+      <c r="I5" s="1">
+        <v>43080</v>
+      </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
@@ -1620,36 +1767,28 @@
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="2"/>
-        <v>330261357</v>
+        <v>246700471</v>
+      </c>
+      <c r="N5" t="s">
+        <v>149</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="2"/>
-        <v>328276606</v>
+        <v>130273406</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="2"/>
-        <v>137148850</v>
+        <v>292675463</v>
       </c>
       <c r="Q5" t="s">
         <v>72</v>
       </c>
+      <c r="S5" t="s">
+        <v>167</v>
+      </c>
       <c r="U5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A5, ",""",
-B5, """,""",
-F5, """,",
-IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")), ",",
-IF(I5="","NULL",_xlfn.CONCAT("""",I5,"""")), ",""",
-H5, """,",
-J5, ",",
-K5, ",",
-M5, ",""",
-O5, """,""",
-P5, """,",
-IF(S5="","NULL",_xlfn.CONCAT("""",S5,"""")), ",""",
-Q5, """,",
-IF(R5="","NULL",_xlfn.CONCAT("""",R5,"""")), "),")</f>
-        <v>(4,"Comet","","Canadian horse",NULL,"0",3,3,330261357,"328276606","137148850",NULL,"White",NULL),</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","0","2017-12-11","3","3",NULL,"246700471","HIS sdm","130273406","292675463","White",NULL,"spotted"),</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -1662,52 +1801,50 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
+      <c r="D6" t="s">
+        <v>161</v>
+      </c>
       <c r="E6" t="s">
         <v>60</v>
       </c>
+      <c r="G6" t="s">
+        <v>157</v>
+      </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>43465</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="2"/>
-        <v>304150765</v>
+        <v>260642741</v>
+      </c>
+      <c r="N6" t="s">
+        <v>150</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="2"/>
-        <v>290197552</v>
+        <v>206528896</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="2"/>
-        <v>211837689</v>
+        <v>200050299</v>
       </c>
       <c r="Q6" t="s">
         <v>72</v>
       </c>
       <c r="U6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A6, ",""",
-B6, """,""",
-F6, """,",
-IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")), ",",
-IF(I6="","NULL",_xlfn.CONCAT("""",I6,"""")), ",""",
-H6, """,",
-J6, ",",
-K6, ",",
-M6, ",""",
-O6, """,""",
-P6, """,",
-IF(S6="","NULL",_xlfn.CONCAT("""",S6,"""")), ",""",
-Q6, """,",
-IF(R6="","NULL",_xlfn.CONCAT("""",R6,"""")), "),")</f>
-        <v>(5,"Krypto","","Labrador retriever",NULL,"0",2,3,304150765,"290197552","211837689",NULL,"White",NULL),</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","1","2018-12-31","0","3",NULL,"260642741","YSE mlc","206528896","200050299","White",NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1720,52 +1857,53 @@
       <c r="C7" t="s">
         <v>46</v>
       </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
       <c r="E7" t="s">
         <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>158</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
+      <c r="I7" s="1">
+        <v>43928</v>
+      </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K7">
         <v>4</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="2"/>
-        <v>327208653</v>
+        <v>127559683</v>
+      </c>
+      <c r="N7" t="s">
+        <v>151</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="2"/>
-        <v>258909036</v>
+        <v>310585598</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="2"/>
-        <v>288072947</v>
+        <v>287897166</v>
       </c>
       <c r="Q7" t="s">
         <v>72</v>
       </c>
+      <c r="S7" t="s">
+        <v>168</v>
+      </c>
       <c r="U7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A7, ",""",
-B7, """,""",
-F7, """,",
-IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")), ",",
-IF(I7="","NULL",_xlfn.CONCAT("""",I7,"""")), ",""",
-H7, """,",
-J7, ",",
-K7, ",",
-M7, ",""",
-O7, """,""",
-P7, """,",
-IF(S7="","NULL",_xlfn.CONCAT("""",S7,"""")), ",""",
-Q7, """,",
-IF(R7="","NULL",_xlfn.CONCAT("""",R7,"""")), "),")</f>
-        <v>(6,"Snowy","","Wire Fox Terrier",NULL,"0",0,4,327208653,"258909036","288072947",NULL,"White",NULL),</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","0","2020-04-07","3","4",NULL,"127559683","JSD sda","310585598","287897166","White",NULL,"long ears"),</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -1778,12 +1916,21 @@
       <c r="C8" t="s">
         <v>44</v>
       </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
       <c r="E8" t="s">
         <v>48</v>
       </c>
+      <c r="G8" t="s">
+        <v>159</v>
+      </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>44289</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
@@ -1794,36 +1941,44 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="2"/>
-        <v>312583075</v>
+        <v>229920898</v>
+      </c>
+      <c r="N8" t="s">
+        <v>152</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="2"/>
-        <v>196013643</v>
+        <v>311084059</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="2"/>
-        <v>156362035</v>
+        <v>176893198</v>
       </c>
       <c r="Q8" t="s">
         <v>73</v>
       </c>
       <c r="U8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A8, ",""",
-B8, """,""",
-F8, """,",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
-IF(I8="","NULL",_xlfn.CONCAT("""",I8,"""")), ",""",
-H8, """,",
-J8, ",",
-K8, ",",
-M8, ",""",
-O8, """,""",
-P8, """,",
-IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")), ",""",
-Q8, """,",
-IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")), ");")</f>
-        <v>(7,"Streaky","","Abyssinian",NULL,"0",0,3,312583075,"196013643","156362035",NULL,"Orange",NULL);</v>
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
+IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),",",
+IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),",",
+IF(I8="","NULL",_xlfn.CONCAT("""",TEXT(I8,"YYYY-MM-DD"),"""")),",",
+IF(J8="","NULL",_xlfn.CONCAT("""",J8,"""")),",",
+IF(K8="","NULL",_xlfn.CONCAT("""",K8,"""")),",",
+IF(L8="","NULL",_xlfn.CONCAT("""",L8,"""")),",",
+IF(M8="","NULL",_xlfn.CONCAT("""",M8,"""")),",",
+IF(N8="","NULL",_xlfn.CONCAT("""",N8,"""")),",",
+IF(O8="","NULL",_xlfn.CONCAT("""",O8,"""")),",",
+IF(P8="","NULL",_xlfn.CONCAT("""",P8,"""")),",",
+IF(Q8="","NULL",_xlfn.CONCAT("""",Q8,"""")),",",
+IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")),",",
+IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")),");")</f>
+        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","1","2021-04-03","0","3",NULL,"229920898","DLF kjs","311084059","176893198","Orange",NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -1868,7 +2023,14 @@
         <v>23</v>
       </c>
       <c r="I1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO owners (",A1,",",B1,",",C1,",",D1,",",E1,",",F1,",",G1,") VALUES ")</f>
+        <f>_xlfn.CONCAT("INSERT INTO owners (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,",",
+G1,") VALUES ")</f>
         <v xml:space="preserve">INSERT INTO owners (o_ownerid,o_firstname,o_middlename,o_lastname,o_contactnumber,o_emailid,o_address) VALUES </v>
       </c>
     </row>
@@ -1887,18 +2049,25 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4033889224</v>
+        <v>4038979328</v>
       </c>
       <c r="F2" t="str">
-        <f>_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
+        <f t="shared" ref="F2:F7" si="0">_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
         <v>damian.bruce.wayne@ucalgary.ca</v>
       </c>
       <c r="G2" t="s">
         <v>78</v>
       </c>
       <c r="I2" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A2,",""",B2,""",""",C2,""",""",D2,""",",",""",E2,""",""",F2,""",""",G2,"""),")</f>
-        <v>(1,"Damian","Bruce","Wayne",,"4033889224","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),"),")</f>
+        <v>("1","Damian","Bruce","Wayne","4038979328","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1912,16 +2081,23 @@
         <v>64</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E7" ca="1" si="0">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4036511734</v>
+        <f t="shared" ref="E3:E7" ca="1" si="1">RANDBETWEEN(4031111111,4039999999)</f>
+        <v>4037202675</v>
       </c>
       <c r="F3" t="str">
-        <f>_xlfn.CONCAT(LOWER(B3),IF(C3="","",_xlfn.CONCAT(".",LOWER(C3))),IF(D3="","",_xlfn.CONCAT(".",LOWER(D3))),"@ucalgary.ca")</f>
+        <f t="shared" si="0"/>
         <v>yorrick.brown@ucalgary.ca</v>
       </c>
       <c r="I3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A3,",""",B3,""",""",C3,""",""",D3,""",",",""",E3,""",""",F3,""",""",G3,"""),")</f>
-        <v>(2,"Yorrick","","Brown",,"4036511734","yorrick.brown@ucalgary.ca",""),</v>
+        <f t="shared" ref="I3:I7" ca="1" si="2">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
+IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),"),")</f>
+        <v>("2","Yorrick",NULL,"Brown","4037202675","yorrick.brown@ucalgary.ca",NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1938,19 +2114,19 @@
         <v>66</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>4031715373</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4031871083</v>
       </c>
       <c r="F4" t="str">
-        <f>_xlfn.CONCAT(LOWER(B4),IF(C4="","",_xlfn.CONCAT(".",LOWER(C4))),IF(D4="","",_xlfn.CONCAT(".",LOWER(D4))),"@ucalgary.ca")</f>
+        <f t="shared" si="0"/>
         <v>clark.joseph.kent@ucalgary.ca</v>
       </c>
       <c r="G4" t="s">
         <v>79</v>
       </c>
       <c r="I4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A4,",""",B4,""",""",C4,""",""",D4,""",",",""",E4,""",""",F4,""",""",G4,"""),")</f>
-        <v>(3,"Clark","Joseph","Kent",,"4031715373","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("3","Clark","Joseph","Kent","4031871083","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1961,19 +2137,19 @@
         <v>67</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4033987193</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4036739520</v>
       </c>
       <c r="F5" t="str">
-        <f>_xlfn.CONCAT(LOWER(B5),IF(C5="","",_xlfn.CONCAT(".",LOWER(C5))),IF(D5="","",_xlfn.CONCAT(".",LOWER(D5))),"@ucalgary.ca")</f>
+        <f t="shared" si="0"/>
         <v>tintin@ucalgary.ca</v>
       </c>
       <c r="G5" t="s">
         <v>82</v>
       </c>
       <c r="I5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A5,",""",B5,""",""",C5,""",""",D5,""",",",""",E5,""",""",F5,""",""",G5,"""),")</f>
-        <v>(4,"Tintin","","",,"4033987193","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("4","Tintin",NULL,NULL,"4036739520","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1984,19 +2160,19 @@
         <v>74</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="0"/>
-        <v>4031745433</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4035469416</v>
       </c>
       <c r="F6" t="str">
-        <f>_xlfn.CONCAT(LOWER(B6),IF(C6="","",_xlfn.CONCAT(".",LOWER(C6))),IF(D6="","",_xlfn.CONCAT(".",LOWER(D6))),"@ucalgary.ca")</f>
+        <f t="shared" si="0"/>
         <v>ucalgary@ucalgary.ca</v>
       </c>
       <c r="G6" t="s">
         <v>81</v>
       </c>
       <c r="I6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A6,",""",B6,""",""",C6,""",""",D6,""",",",""",E6,""",""",F6,""",""",G6,"""),")</f>
-        <v>(5,"UCalgary","","",,"4031745433","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("5","UCalgary",NULL,NULL,"4035469416","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2010,19 +2186,26 @@
         <v>76</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>4034877564</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4034784390</v>
       </c>
       <c r="F7" t="str">
-        <f>_xlfn.CONCAT(LOWER(B7),IF(C7="","",_xlfn.CONCAT(".",LOWER(C7))),IF(D7="","",_xlfn.CONCAT(".",LOWER(D7))),"@ucalgary.ca")</f>
+        <f t="shared" si="0"/>
         <v>james.gunn@ucalgary.ca</v>
       </c>
       <c r="G7" t="s">
         <v>80</v>
       </c>
       <c r="I7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",A7,",""",B7,""",""",C7,""",""",D7,""",",",""",E7,""",""",F7,""",""",G7,""");")</f>
-        <v>(6,"James","","Gunn",,"4034877564","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A7="","NULL",_xlfn.CONCAT("""",A7,"""")),",",
+IF(B7="","NULL",_xlfn.CONCAT("""",B7,"""")),",",
+IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),",",
+IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),",",
+IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
+IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),",",
+IF(G7="","NULL",_xlfn.CONCAT("""",G7,"""")),");")</f>
+        <v>("6","James",NULL,"Gunn","4034784390","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
       </c>
     </row>
   </sheetData>
@@ -2048,13 +2231,13 @@
         <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>30</v>
@@ -2069,26 +2252,46 @@
         <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="N1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO users (",A1,",",E1,",",F1,",",G1,",",H1,",",I1,",",J1,",",L1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO users (u_userid,u_firstname,u_middlename,u_lastname,u_role,u_email,u_passwordhash,u_status) VALUES </v>
+        <f>_xlfn.CONCAT("INSERT INTO users (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,",",
+G1,",",
+H1,",",
+I1,",",
+J1,",",
+K1,",",
+L1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO users (u_userid,u_joiningdate,u_activationdate,u_terminationdate,u_firstname,u_middlename,u_lastname,u_role,u_emailid,u_passwordhash,u_passwordsalt,u_status) VALUES </v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="1">
+        <v>43070</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2+1</f>
+        <v>43071</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>106</v>
       </c>
@@ -2110,21 +2313,33 @@
       </c>
       <c r="N2" t="str">
         <f>_xlfn.CONCAT("(",
-A2,",""",
-E2,""",",
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",TEXT(B2,"YYYY-MM-DD"),"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
-H2,",""",
-I2,""",""",
-J2,""",",
-L2,"),")</f>
-        <v>(1,"Greg",NULL,"Boorman",0,"greg.boorman@ucalgary.ca","passw0rd",1),</v>
+IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),",",
+IF(I2="","NULL",_xlfn.CONCAT("""",TEXT(I2,"YYYY-MM-DD"),"""")),",",
+IF(J2="","NULL",_xlfn.CONCAT("""",J2,"""")),",",
+IF(K2="","NULL",_xlfn.CONCAT("""",K2,"""")),",",
+IF(L2="","NULL",_xlfn.CONCAT("""",L2,"""")),"),")</f>
+        <v>("1","2017-12-01","2017-12-02",NULL,"Greg",NULL,"Boorman","0","greg.boorman@ucalgary.ca","passw0rd",NULL,"1"),</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>43436</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C8" si="0">B3+1</f>
+        <v>43437</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>108</v>
       </c>
@@ -2135,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I8" si="0">_xlfn.CONCAT(LOWER(E3),IF(F3="","",_xlfn.CONCAT(".",LOWER(F3))),IF(G3="","",_xlfn.CONCAT(".",LOWER(G3))),"@ucalgary.ca")</f>
+        <f t="shared" ref="I3:I8" si="1">_xlfn.CONCAT(LOWER(E3),IF(F3="","",_xlfn.CONCAT(".",LOWER(F3))),IF(G3="","",_xlfn.CONCAT(".",LOWER(G3))),"@ucalgary.ca")</f>
         <v>teacher.admin@ucalgary.ca</v>
       </c>
       <c r="J3" t="s">
@@ -2145,22 +2360,34 @@
         <v>0</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N7" si="1">_xlfn.CONCAT("(",
-A3,",""",
-E3,""",",
+        <f t="shared" ref="N3:N8" si="2">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",TEXT(B3,"YYYY-MM-DD"),"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
-H3,",""",
-I3,""",""",
-J3,""",",
-L3,"),")</f>
-        <v>(2,"Teacher",NULL,"Admin",0,"teacher.admin@ucalgary.ca","passw0rd",0),</v>
+IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),",",
+IF(I3="","NULL",_xlfn.CONCAT("""",TEXT(I3,"YYYY-MM-DD"),"""")),",",
+IF(J3="","NULL",_xlfn.CONCAT("""",J3,"""")),",",
+IF(K3="","NULL",_xlfn.CONCAT("""",K3,"""")),",",
+IF(L3="","NULL",_xlfn.CONCAT("""",L3,"""")),"),")</f>
+        <v>("2","2018-12-02","2018-12-03",NULL,"Teacher",NULL,"Admin","0","teacher.admin@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <v>43924</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>43925</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" t="s">
         <v>111</v>
       </c>
@@ -2171,7 +2398,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>technician.a@ucalgary.ca</v>
       </c>
       <c r="J4" t="s">
@@ -2181,14 +2408,22 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="1"/>
-        <v>(3,"Technician",NULL,"A",2,"technician.a@ucalgary.ca","passw0rd",0),</v>
+        <f t="shared" si="2"/>
+        <v>("3","2020-04-03","2020-04-04",NULL,"Technician",NULL,"A","2","technician.a@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="1">
+        <v>43080</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>43081</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" t="s">
         <v>113</v>
       </c>
@@ -2199,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>attendant.b@ucalgary.ca</v>
       </c>
       <c r="J5" t="s">
@@ -2209,14 +2444,25 @@
         <v>0</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="1"/>
-        <v>(4,"Attendant",NULL,"B",1,"attendant.b@ucalgary.ca","passw0rd",0),</v>
+        <f t="shared" si="2"/>
+        <v>("4","2017-12-11","2017-12-12",NULL,"Attendant",NULL,"B","1","attendant.b@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>43465</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>43466</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D3:D8" si="3">C6+1000</f>
+        <v>44466</v>
+      </c>
       <c r="E6" t="s">
         <v>108</v>
       </c>
@@ -2227,7 +2473,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>teacher.c@ucalgary.ca</v>
       </c>
       <c r="J6" t="s">
@@ -2237,14 +2483,25 @@
         <v>0</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="1"/>
-        <v>(5,"Teacher",NULL,"C",3,"teacher.c@ucalgary.ca","passw0rd",0),</v>
+        <f t="shared" si="2"/>
+        <v>("5","2018-12-31","2019-01-01","2021-09-27","Teacher",NULL,"C","3","teacher.c@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" s="1">
+        <v>43928</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>43929</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="3"/>
+        <v>44929</v>
+      </c>
       <c r="E7" t="s">
         <v>115</v>
       </c>
@@ -2255,7 +2512,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>student.d@ucalgary.ca</v>
       </c>
       <c r="J7" t="s">
@@ -2265,14 +2522,25 @@
         <v>0</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="1"/>
-        <v>(6,"Student",NULL,"D",4,"student.d@ucalgary.ca","passw0rd",0),</v>
+        <f t="shared" si="2"/>
+        <v>("6","2020-04-07","2020-04-08","2023-01-03","Student",NULL,"D","4","student.d@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>44290</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="3"/>
+        <v>45290</v>
+      </c>
       <c r="E8" t="s">
         <v>115</v>
       </c>
@@ -2283,7 +2551,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>student.e@ucalgary.ca</v>
       </c>
       <c r="J8" t="s">
@@ -2294,15 +2562,19 @@
       </c>
       <c r="N8" t="str">
         <f>_xlfn.CONCAT("(",
-A8,",""",
-E8,""",",
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",TEXT(B8,"YYYY-MM-DD"),"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",TEXT(D8,"YYYY-MM-DD"),"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),",",
-H8,",""",
-I8,""",""",
-J8,""",",
-L8,");")</f>
-        <v>(7,"Student",NULL,"E",4,"student.e@ucalgary.ca","passw0rd",0);</v>
+IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),",",
+IF(I8="","NULL",_xlfn.CONCAT("""",TEXT(I8,"YYYY-MM-DD"),"""")),",",
+IF(J8="","NULL",_xlfn.CONCAT("""",J8,"""")),",",
+IF(K8="","NULL",_xlfn.CONCAT("""",K8,"""")),",",
+IF(L8="","NULL",_xlfn.CONCAT("""",L8,"""")),");")</f>
+        <v>("7","2021-04-03","2021-04-04","2023-12-30","Student",NULL,"E","4","student.e@ucalgary.ca","passw0rd",NULL,"0");</v>
       </c>
     </row>
   </sheetData>
@@ -2327,23 +2599,28 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="G1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO photos (",A1,",",E1,",",C1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO photos (w_weightid,w_animalid,w_recorddate) VALUES </v>
+        <f>_xlfn.CONCAT("INSERT INTO weights (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO weights (w_weightid,w_massinkg,w_recorddate,w_recordedby,w_animalid) VALUES </v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2352,14 +2629,16 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A2,",",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
-IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),"","),")</f>
-        <v>(1,"5",NULL),</v>
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
+        <v>("1",NULL,NULL,NULL,"7"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2368,30 +2647,30 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A3,",",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
-IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),"","),")</f>
-        <v>(2,"1",NULL),</v>
+        <f t="shared" ref="G3:G8" ca="1" si="1">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
+        <v>("2",NULL,NULL,NULL,"6"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4" s="1"/>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A4,",",
-IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")),",",
-IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),"","),")</f>
-        <v>(3,"3",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("3",NULL,NULL,NULL,"5"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2400,14 +2679,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A5,",",
-IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")),",",
-IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),"","),")</f>
-        <v>(4,"5",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("4",NULL,NULL,NULL,"6"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2416,14 +2692,11 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A6,",",
-IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")),",",
-IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),"","),")</f>
-        <v>(5,"3",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("5",NULL,NULL,NULL,"1"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2432,14 +2705,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A7,",",
-IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
-IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),"","),")</f>
-        <v>(6,"7",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("6",NULL,NULL,NULL,"5"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2448,14 +2718,16 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A8,",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
-IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),"",")",";")</f>
-        <v>(7,"1",NULL);</v>
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),");")</f>
+        <v>("7",NULL,NULL,NULL,"4");</v>
       </c>
     </row>
   </sheetData>
@@ -2480,7 +2752,7 @@
         <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>42</v>
@@ -2489,17 +2761,24 @@
         <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="I1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO photos (",A1,",",C1,",",D1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO photos (p_photoid,p_animalid,p_photolink) VALUES </v>
+        <f>_xlfn.CONCAT("INSERT INTO photos (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,",",
+G1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO photos (p_photoid,p_photodesc,p_animalid,p_photolink,p_alttext,p_uploader,p_uploaddate) VALUES </v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2508,17 +2787,21 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
       </c>
       <c r="I2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A2,",",
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
-IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),"","),")</f>
-        <v>(1,"7","image1.png"),</v>
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),"),")</f>
+        <v>("1",NULL,"4","image1.png",NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2527,17 +2810,21 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
       </c>
       <c r="I3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A3,",",
+        <f t="shared" ref="I3:I8" ca="1" si="1">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),"","),")</f>
-        <v>(2,"1","image2.png"),</v>
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
+IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),"),")</f>
+        <v>("2",NULL,"3","image2.png",NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2546,17 +2833,14 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>102</v>
       </c>
       <c r="I4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A4,",",
-IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),",",
-IF(D4="","NULL",_xlfn.CONCAT("""",D4,"""")),"","),")</f>
-        <v>(3,"3","image4.png"),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("3",NULL,"1","image4.png",NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2565,14 +2849,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A5,",",
-IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),",",
-IF(D5="","NULL",_xlfn.CONCAT("""",D5,"""")),"","),")</f>
-        <v>(4,"4",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("4",NULL,"5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2581,17 +2862,14 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>103</v>
       </c>
       <c r="I6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A6,",",
-IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),",",
-IF(D6="","NULL",_xlfn.CONCAT("""",D6,"""")),"","),")</f>
-        <v>(5,"3","image7.png"),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("5",NULL,"7","image7.png",NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2600,17 +2878,14 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
       </c>
       <c r="I7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A7,",",
-IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),",",
-IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),"","),")</f>
-        <v>(6,"2","image6.png"),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("6",NULL,"5","image6.png",NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2619,17 +2894,21 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>105</v>
       </c>
       <c r="I8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A8,",",
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
 IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),"",")",";")</f>
-        <v>(7,"3","image5.png");</v>
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
+IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),");")</f>
+        <v>("7",NULL,"5","image5.png",NULL,NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -2667,7 +2946,12 @@
         <v>15</v>
       </c>
       <c r="G1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO comments (",A1,",",B1,",",C1,",",D1,",",E1,") VALUES ")</f>
+        <f>_xlfn.CONCAT("INSERT INTO comments (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,") VALUES ")</f>
         <v xml:space="preserve">INSERT INTO comments (c_commentid,c_commentdesc,c_animalid,c_commentdate,c_commenter) VALUES </v>
       </c>
     </row>
@@ -2680,23 +2964,23 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A2,",",
-IF(B2="","""No Comment Provided""",_xlfn.CONCAT("""",B2,"""")), ",""",
-C2,""",",
-IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
-IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"","),")</f>
-        <v>(1,"Nighttime terror","5","44538","2"),</v>
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
+        <v>("1","Nighttime terror","4","2021-12-08","6"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2708,23 +2992,23 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <v>44539</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
-A3,",",
-IF(B3="","""No Comment Provided""",_xlfn.CONCAT("""",B3,"""")), ",""",
-C3,""",",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
-IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"","),")</f>
-        <v>(2,"Howling ","3","44539","7"),</v>
+        <f t="shared" ref="G3:G8" ca="1" si="2">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
+        <v>("2","Howling ","1","2021-12-09","6"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2736,18 +3020,18 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(3,"Pregnant ","6","44540","2"),</v>
+        <v>("3","Pregnant ","4","2021-12-10","4"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2756,18 +3040,18 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(4,"No Comment Provided","1","44538","5"),</v>
+        <v>("4",NULL,"7","2021-12-08","7"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2776,18 +3060,18 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(5,"No Comment Provided","7","44539","5"),</v>
+        <v>("5",NULL,"5","2021-12-09","6"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2796,18 +3080,18 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>(6,"No Comment Provided","2","44540","5"),</v>
+        <v>("6",NULL,"7","2021-12-10","2"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2819,23 +3103,23 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A8,",",
-IF(B8="","""No Comment Provided""",_xlfn.CONCAT("""",B8,"""")), ",""",
-C8,""",",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"",")",";")</f>
-        <v>(7,"Not sleeping","2","44538","2");</v>
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",TEXT(D8,"YYYY-MM-DD"),"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),");")</f>
+        <v>("7","Not sleeping","5","2021-12-08","3");</v>
       </c>
     </row>
   </sheetData>
@@ -2847,9 +3131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E769BC6-8AA4-47AC-8CDF-52C74C698B1A}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2879,8 +3161,14 @@
         <v>19</v>
       </c>
       <c r="H1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO issues (",A1,",",B1,",",D1,",",C1,",",E1,",",F1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_animalid,i_detecteddate,i_raisedby,i_isresolved) VALUES </v>
+        <f>_xlfn.CONCAT("INSERT INTO issues (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_detecteddate,i_animalid,i_raisedby,i_isresolved) VALUES </v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2895,7 +3183,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2905,13 +3193,13 @@
       </c>
       <c r="H2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A2,",",
-IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")), ",""",
-D2,""",",
-IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
-IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),"","),")</f>
-        <v>(1,"Limp Walk","1","44538","1","1"),</v>
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),"),")</f>
+        <v>("1","Limp Walk","2021-12-08","4","1","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2923,7 +3211,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2932,14 +3220,14 @@
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A3,",",
-IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")), ",""",
-D3,""",",
-IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+        <f t="shared" ref="H3:H8" ca="1" si="1">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
-IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"","),")</f>
-        <v>(2,NULL,"7","44177","1","1"),</v>
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"),")</f>
+        <v>("2",NULL,"2020-12-12","2","1","1"),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2954,7 +3242,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2963,14 +3251,8 @@
         <v>0</v>
       </c>
       <c r="H4" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A4,",",
-IF(B4="","NULL",_xlfn.CONCAT("""",B4,"""")), ",""",
-D4,""",",
-IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),",",
-IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")),",",
-IF(F4="","NULL",_xlfn.CONCAT("""",F4,"""")),"","),")</f>
-        <v>(3,"Diabetes","3","44332","2","0"),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("3","Diabetes","2021-05-16","2","2","0"),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2985,20 +3267,14 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="H5" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A5,",",
-IF(B5="","NULL",_xlfn.CONCAT("""",B5,"""")), ",""",
-D5,""",",
-IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),",",
-IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")),",",
-IF(F5="","NULL",_xlfn.CONCAT("""",F5,"""")),"","),")</f>
-        <v>(4,"Inflammed limb","6","44345","1",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("4","Inflammed limb","2021-05-29","2","1",NULL),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3011,20 +3287,14 @@
       <c r="C6" s="1"/>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="H6" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A6,",",
-IF(B6="","NULL",_xlfn.CONCAT("""",B6,"""")), ",""",
-D6,""",",
-IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),",",
-IF(E6="","NULL",_xlfn.CONCAT("""",E6,"""")),",",
-IF(F6="","NULL",_xlfn.CONCAT("""",F6,"""")),"","),")</f>
-        <v>(5,"Bladder Infection","6",NULL,"5",NULL),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("5","Bladder Infection",NULL,"7","5",NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3039,7 +3309,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -3048,14 +3318,8 @@
         <v>0</v>
       </c>
       <c r="H7" t="str">
-        <f ca="1">_xlfn.CONCAT("(",
-A7,",",
-IF(B7="","NULL",_xlfn.CONCAT("""",B7,"""")), ",""",
-D7,""",",
-IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),",",
-IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
-IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),"","),")</f>
-        <v>(6,"chronic kidney disease","3","44517","3","0"),</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>("6","chronic kidney disease","2021-11-17","6","3","0"),</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3077,13 +3341,13 @@
       </c>
       <c r="H8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A8, ",",
-IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")), ",""",
-D8, """,",
-IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")), ",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")), ",",
-IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),"",")",";")</f>
-        <v>(7,"Upset Stomach","3","44517","2",NULL);</v>
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),");")</f>
+        <v>("7","Upset Stomach","2021-11-17","3","2",NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -3114,13 +3378,13 @@
         <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>35</v>
@@ -3132,8 +3396,16 @@
         <v>36</v>
       </c>
       <c r="J1" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO treatments (",A1,",",B1,",",F1,",",G1,",",H1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
+        <f>_xlfn.CONCAT("INSERT INTO treatments (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,",",
+G1,",",
+H1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_drugname,t_drugdose,t_deliverymethod,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -3145,7 +3417,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>44538</v>
@@ -3155,12 +3427,15 @@
       </c>
       <c r="J2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A2,",""",
-B2,""",""",
-F2,""",",
-IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
-IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"","),")</f>
-        <v>(1,"Physical exam","7","44538","1"),</v>
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),",",
+IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
+        <v>("1","Physical exam",NULL,NULL,NULL,"5","2021-12-08","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -3172,7 +3447,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>44539</v>
@@ -3181,13 +3456,16 @@
         <v>2</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J7" ca="1" si="1">_xlfn.CONCAT("(",
-A3,",""",
-B3,""",""",
-F3,""",",
-IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
-IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"","),")</f>
-        <v>(2,"Blood work","5","44539","2"),</v>
+        <f t="shared" ref="J3:J8" ca="1" si="1">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
+IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),",",
+IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
+        <v>("2","Blood work",NULL,NULL,NULL,"1","2021-12-09","2"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -3199,7 +3477,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <v>44540</v>
@@ -3209,7 +3487,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(3,"Da2pp","1","44540","5"),</v>
+        <v>("3","Da2pp",NULL,NULL,NULL,"2","2021-12-10","5"),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -3221,7 +3499,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1">
         <v>44538</v>
@@ -3231,7 +3509,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(4,"dental cleaning","4","44538","3"),</v>
+        <v>("4","dental cleaning",NULL,NULL,NULL,"6","2021-12-08","3"),</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -3243,7 +3521,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>44539</v>
@@ -3253,7 +3531,7 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(5,"drontal deworm","1","44539","4"),</v>
+        <v>("5","drontal deworm",NULL,NULL,NULL,"4","2021-12-09","4"),</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -3265,7 +3543,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>44540</v>
@@ -3275,7 +3553,7 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>(6,"rabies vaccination","4","44540","2"),</v>
+        <v>("6","rabies vaccination",NULL,NULL,NULL,"3","2021-12-10","2"),</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -3287,7 +3565,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <v>44538</v>
@@ -3297,12 +3575,15 @@
       </c>
       <c r="J8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
-A8,",""",
-B8,""",""",
-F8,""",",
-IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),",",
-IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),"",")",";")</f>
-        <v>(7,"Revolution treatment","7","44538","4");</v>
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
+IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),",",
+IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),");")</f>
+        <v>("7","Revolution treatment",NULL,NULL,NULL,"2","2021-12-08","4");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build: [U888-62] created views and more dummy data
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9F67C6-8C9F-4984-ADEC-167AB72A1127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36941F2D-4EFD-49D2-96E4-AD7AC19D9B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="172">
   <si>
     <t>a_animalid</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>u_emailid</t>
+  </si>
+  <si>
+    <t>leg broken</t>
+  </si>
+  <si>
+    <t>neck</t>
   </si>
 </sst>
 </file>
@@ -1542,25 +1548,25 @@
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="M2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>164519616</v>
+        <v>254096526</v>
       </c>
       <c r="N2" t="s">
         <v>146</v>
       </c>
       <c r="O2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>193563577</v>
+        <v>325947707</v>
       </c>
       <c r="P2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>220698998</v>
+        <v>252688474</v>
       </c>
       <c r="Q2" t="s">
         <v>70</v>
@@ -1592,7 +1598,7 @@
 IF(Q2="","NULL",_xlfn.CONCAT("""",Q2,"""")),",",
 IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")),",",
 IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")),"),")</f>
-        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","0","2017-12-01","2","1",NULL,"164519616","HOC sha","193563577","220698998","Black","sleeping pills","he can fly"),</v>
+        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","0","2017-12-01","1","1",NULL,"254096526","HOC sha","325947707","252688474","Black","sleeping pills","he can fly"),</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -1623,25 +1629,25 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:P8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
-        <v>161174992</v>
+        <v>257238887</v>
       </c>
       <c r="N3" t="s">
         <v>147</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="2"/>
-        <v>312602124</v>
+        <v>337372126</v>
       </c>
       <c r="P3">
         <f t="shared" ca="1" si="2"/>
-        <v>223632487</v>
+        <v>150999162</v>
       </c>
       <c r="Q3" t="s">
         <v>64</v>
@@ -1650,7 +1656,7 @@
         <v>165</v>
       </c>
       <c r="U3" t="str">
-        <f t="shared" ref="U3:U8" ca="1" si="3">_xlfn.CONCAT("(",
+        <f t="shared" ref="U3:U7" ca="1" si="3">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
@@ -1670,7 +1676,7 @@
 IF(Q3="","NULL",_xlfn.CONCAT("""",Q3,"""")),",",
 IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")),",",
 IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")),"),")</f>
-        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","0","2018-12-02","0","2",NULL,"161174992","ORE esd","312602124","223632487","Brown",NULL,"high jumps"),</v>
+        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","0","2018-12-02","1","2",NULL,"257238887","ORE esd","337372126","150999162","Brown",NULL,"high jumps"),</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -1694,32 +1700,32 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>43924</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="2"/>
-        <v>168429354</v>
+        <v>266851685</v>
       </c>
       <c r="N4" t="s">
         <v>148</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="2"/>
-        <v>260294146</v>
+        <v>141801485</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="2"/>
-        <v>137251498</v>
+        <v>229161701</v>
       </c>
       <c r="Q4" t="s">
         <v>71</v>
@@ -1729,7 +1735,7 @@
       </c>
       <c r="U4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","1","2020-04-03","0","1",NULL,"168429354","NKN sds","260294146","137251498","Brown, White",NULL,"bat-shaped patch on face"),</v>
+        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","0","2020-04-03","3","1",NULL,"266851685","NKN sds","141801485","229161701","Brown, White",NULL,"bat-shaped patch on face"),</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -1753,32 +1759,32 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>43080</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="2"/>
-        <v>246700471</v>
+        <v>220216471</v>
       </c>
       <c r="N5" t="s">
         <v>149</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="2"/>
-        <v>130273406</v>
+        <v>151163228</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="2"/>
-        <v>292675463</v>
+        <v>189812256</v>
       </c>
       <c r="Q5" t="s">
         <v>72</v>
@@ -1788,7 +1794,7 @@
       </c>
       <c r="U5" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","0","2017-12-11","3","3",NULL,"246700471","HIS sdm","130273406","292675463","White",NULL,"spotted"),</v>
+        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","1","2017-12-11","2","3",NULL,"220216471","HIS sdm","151163228","189812256","White",NULL,"spotted"),</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -1812,7 +1818,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>43465</v>
@@ -1826,25 +1832,25 @@
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="2"/>
-        <v>260642741</v>
+        <v>243701521</v>
       </c>
       <c r="N6" t="s">
         <v>150</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="2"/>
-        <v>206528896</v>
+        <v>168003214</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="2"/>
-        <v>200050299</v>
+        <v>210776146</v>
       </c>
       <c r="Q6" t="s">
         <v>72</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","1","2018-12-31","0","3",NULL,"260642741","YSE mlc","206528896","200050299","White",NULL,NULL),</v>
+        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","0","2018-12-31","0","3",NULL,"243701521","YSE mlc","168003214","210776146","White",NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1875,25 +1881,25 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>4</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="2"/>
-        <v>127559683</v>
+        <v>308818670</v>
       </c>
       <c r="N7" t="s">
         <v>151</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="2"/>
-        <v>310585598</v>
+        <v>129775445</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="2"/>
-        <v>287897166</v>
+        <v>329563799</v>
       </c>
       <c r="Q7" t="s">
         <v>72</v>
@@ -1903,7 +1909,7 @@
       </c>
       <c r="U7" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","0","2020-04-07","3","4",NULL,"127559683","JSD sda","310585598","287897166","White",NULL,"long ears"),</v>
+        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","0","2020-04-07","2","4",NULL,"308818670","JSD sda","129775445","329563799","White",NULL,"long ears"),</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -1927,32 +1933,32 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
         <v>44289</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <v>3</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="2"/>
-        <v>229920898</v>
+        <v>144541305</v>
       </c>
       <c r="N8" t="s">
         <v>152</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="2"/>
-        <v>311084059</v>
+        <v>238484846</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="2"/>
-        <v>176893198</v>
+        <v>227949821</v>
       </c>
       <c r="Q8" t="s">
         <v>73</v>
@@ -1978,7 +1984,7 @@
 IF(Q8="","NULL",_xlfn.CONCAT("""",Q8,"""")),",",
 IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")),",",
 IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")),");")</f>
-        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","1","2021-04-03","0","3",NULL,"229920898","DLF kjs","311084059","176893198","Orange",NULL,NULL);</v>
+        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","0","2021-04-03","2","3",NULL,"144541305","DLF kjs","238484846","227949821","Orange",NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -2049,7 +2055,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4038979328</v>
+        <v>4039774023</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F7" si="0">_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
@@ -2067,7 +2073,7 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),"),")</f>
-        <v>("1","Damian","Bruce","Wayne","4038979328","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+        <v>("1","Damian","Bruce","Wayne","4039774023","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2082,14 +2088,14 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E7" ca="1" si="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4037202675</v>
+        <v>4039397251</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>yorrick.brown@ucalgary.ca</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I7" ca="1" si="2">_xlfn.CONCAT("(",
+        <f t="shared" ref="I3:I6" ca="1" si="2">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
@@ -2097,7 +2103,7 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),"),")</f>
-        <v>("2","Yorrick",NULL,"Brown","4037202675","yorrick.brown@ucalgary.ca",NULL),</v>
+        <v>("2","Yorrick",NULL,"Brown","4039397251","yorrick.brown@ucalgary.ca",NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2115,7 +2121,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4031871083</v>
+        <v>4031810495</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -2126,7 +2132,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Clark","Joseph","Kent","4031871083","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+        <v>("3","Clark","Joseph","Kent","4031810495","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2138,7 +2144,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>4036739520</v>
+        <v>4036232718</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -2149,7 +2155,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","Tintin",NULL,NULL,"4036739520","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+        <v>("4","Tintin",NULL,NULL,"4036232718","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2161,7 +2167,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>4035469416</v>
+        <v>4037061417</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -2172,7 +2178,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5","UCalgary",NULL,NULL,"4035469416","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+        <v>("5","UCalgary",NULL,NULL,"4037061417","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2187,7 +2193,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4034784390</v>
+        <v>4033313504</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -2205,7 +2211,7 @@
 IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
 IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),",",
 IF(G7="","NULL",_xlfn.CONCAT("""",G7,"""")),");")</f>
-        <v>("6","James",NULL,"Gunn","4034784390","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+        <v>("6","James",NULL,"Gunn","4033313504","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N8" si="2">_xlfn.CONCAT("(",
+        <f t="shared" ref="N3:N7" si="2">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",TEXT(B3,"YYYY-MM-DD"),"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
@@ -2460,7 +2466,7 @@
         <v>43466</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D3:D8" si="3">C6+1000</f>
+        <f t="shared" ref="D6:D8" si="3">C6+1000</f>
         <v>44466</v>
       </c>
       <c r="E6" t="s">
@@ -2584,7 +2590,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3D06D0-BF1F-4225-AF4B-50DA628F29F9}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2627,9 +2633,18 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
       <c r="E2">
-        <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2638,87 +2653,140 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1",NULL,NULL,NULL,"7"),</v>
+        <v>("1","5","2020-10-01","4","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D29" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>7</v>
+      </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G8" ca="1" si="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="G3:G7" ca="1" si="1">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2",NULL,NULL,NULL,"6"),</v>
+        <v>("2","4","2020-10-01","7","2"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
       <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3",NULL,NULL,NULL,"5"),</v>
+        <v>("3","30","2020-10-01","6","3"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
       <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4",NULL,NULL,NULL,"6"),</v>
+        <v>("4","40","2020-10-01","6","4"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5",NULL,NULL,NULL,"1"),</v>
+        <v>("5","3","2020-10-01","2","5"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
       <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6",NULL,NULL,NULL,"5"),</v>
+        <v>("6","3","2020-10-01","3","6"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44105</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2726,8 +2794,500 @@
 IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
 IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
-IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),");")</f>
-        <v>("7",NULL,NULL,NULL,"4");</v>
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"),")</f>
+        <v>("7","1","2020-10-01","1","7"),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" ref="G9:G28" ca="1" si="2">_xlfn.CONCAT("(",
+IF(A9="","NULL",_xlfn.CONCAT("""",A9,"""")),",",
+IF(B9="","NULL",_xlfn.CONCAT("""",B9,"""")),",",
+IF(C9="","NULL",_xlfn.CONCAT("""",TEXT(C9,"YYYY-MM-DD"),"""")),",",
+IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),",",
+IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),"),")</f>
+        <v>("8","4","2020-11-03","7","1"),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>B2+0.2</f>
+        <v>5.2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("9","5.2","2020-11-03","1","2"),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:B15" si="3">B3+0.2</f>
+        <v>4.2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("10","4.2","2020-11-03","3","3"),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="3"/>
+        <v>30.2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("11","30.2","2020-11-03","6","4"),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="3"/>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("12","40.2","2020-11-03","3","5"),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("13","3.2","2020-11-03","6","6"),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44138</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("14","3.2","2020-11-03","1","7"),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f>B8-0.4</f>
+        <v>0.6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("15","0.6","2020-11-29","1","1"),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:B22" si="4">B9-0.4</f>
+        <v>3.6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("16","3.6","2020-11-29","3","2"),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="4"/>
+        <v>4.8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("17","4.8","2020-11-29","3","3"),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="4"/>
+        <v>3.8000000000000003</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("18","3.8","2020-11-29","3","4"),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="4"/>
+        <v>29.8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("19","29.8","2020-11-29","3","5"),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="4"/>
+        <v>39.800000000000004</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("20","39.8","2020-11-29","3","6"),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="4"/>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44164</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("21","2.8","2020-11-29","4","7"),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f>B15+0.6</f>
+        <v>3.8000000000000003</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("22","3.8","2021-02-28","1","1"),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:B29" si="5">B16+0.6</f>
+        <v>1.2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("23","1.2","2021-02-28","3","2"),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="5"/>
+        <v>4.2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("24","4.2","2021-02-28","1","3"),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="5"/>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="C26" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("25","5.4","2021-02-28","6","4"),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="5"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C27" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("26","4.4","2021-02-28","1","5"),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="5"/>
+        <v>30.400000000000002</v>
+      </c>
+      <c r="C28" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("27","30.4","2021-02-28","2","6"),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="5"/>
+        <v>40.400000000000006</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44255</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="G29" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A29="","NULL",_xlfn.CONCAT("""",A29,"""")),",",
+IF(B29="","NULL",_xlfn.CONCAT("""",B29,"""")),",",
+IF(C29="","NULL",_xlfn.CONCAT("""",TEXT(C29,"YYYY-MM-DD"),"""")),",",
+IF(D29="","NULL",_xlfn.CONCAT("""",D29,"""")),",",
+IF(E29="","NULL",_xlfn.CONCAT("""",E29,"""")),");")</f>
+        <v>("28","40.4","2021-02-28","2","7");</v>
       </c>
     </row>
   </sheetData>
@@ -2787,10 +3347,20 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44105</v>
       </c>
       <c r="I2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2801,7 +3371,7 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1",NULL,"4","image1.png",NULL,NULL,NULL),</v>
+        <v>("1",NULL,"2","image1.png","neck","3","2020-10-01"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2810,13 +3380,20 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(1,7)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44105</v>
+      </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I8" ca="1" si="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="I3:I7" ca="1" si="2">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
@@ -2824,7 +3401,7 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2",NULL,"3","image2.png",NULL,NULL,NULL),</v>
+        <v>("2",NULL,"5","image2.png",NULL,"2","2020-10-01"),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2833,27 +3410,44 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>102</v>
       </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44105</v>
+      </c>
       <c r="I4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>("3",NULL,"1","image4.png",NULL,NULL,NULL),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("3",NULL,"4","image4.png",NULL,"1","2020-10-01"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44105</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>("4",NULL,"5",NULL,NULL,NULL,NULL),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("4","leg broken","1",NULL,NULL,"6","2020-10-01"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2862,14 +3456,21 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>103</v>
       </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44105</v>
+      </c>
       <c r="I6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>("5",NULL,"7","image7.png",NULL,NULL,NULL),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("5",NULL,"3","image7.png",NULL,"4","2020-10-01"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2878,14 +3479,21 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
       </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44105</v>
+      </c>
       <c r="I7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>("6",NULL,"5","image6.png",NULL,NULL,NULL),</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>("6",NULL,"7","image6.png",NULL,"7","2020-10-01"),</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2894,10 +3502,17 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>105</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44105</v>
       </c>
       <c r="I8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -2908,7 +3523,7 @@
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),");")</f>
-        <v>("7",NULL,"5","image5.png",NULL,NULL,NULL);</v>
+        <v>("7",NULL,"7","image5.png",NULL,"7","2020-10-01");</v>
       </c>
     </row>
   </sheetData>
@@ -2964,7 +3579,7 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
@@ -2980,7 +3595,7 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","Nighttime terror","4","2021-12-08","6"),</v>
+        <v>("1","Nighttime terror","1","2021-12-08","6"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2992,7 +3607,7 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>44539</v>
@@ -3002,13 +3617,13 @@
         <v>6</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G8" ca="1" si="2">_xlfn.CONCAT("(",
+        <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","Howling ","1","2021-12-09","6"),</v>
+        <v>("2","Howling ","3","2021-12-09","6"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3020,18 +3635,18 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Pregnant ","4","2021-12-10","4"),</v>
+        <v>("3","Pregnant ","6","2021-12-10","1"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3040,7 +3655,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
@@ -3051,7 +3666,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4",NULL,"7","2021-12-08","7"),</v>
+        <v>("4",NULL,"5","2021-12-08","7"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3060,18 +3675,18 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"5","2021-12-09","6"),</v>
+        <v>("5",NULL,"4","2021-12-09","2"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3080,18 +3695,18 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"7","2021-12-10","2"),</v>
+        <v>("6",NULL,"6","2021-12-10","4"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3103,14 +3718,14 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -3119,7 +3734,7 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",TEXT(D8,"YYYY-MM-DD"),"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),");")</f>
-        <v>("7","Not sleeping","5","2021-12-08","3");</v>
+        <v>("7","Not sleeping","4","2021-12-08","7");</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3798,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3198,8 +3813,8 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
-IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),"),")</f>
-        <v>("1","Limp Walk","2021-12-08","4","1","1"),</v>
+IF(F2="","NULL",_xlfn.CONCAT("",F2,"")),"),")</f>
+        <v>("1","Limp Walk","2021-12-08","1","1",1),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -3211,7 +3826,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3226,8 +3841,8 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
-IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),"),")</f>
-        <v>("2",NULL,"2020-12-12","2","1","1"),</v>
+IF(F3="","NULL",_xlfn.CONCAT("",F3,"")),"),")</f>
+        <v>("2",NULL,"2020-12-12","1","1",1),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3242,7 +3857,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -3252,7 +3867,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Diabetes","2021-05-16","2","2","0"),</v>
+        <v>("3","Diabetes","2021-05-16","6","2",0),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3267,14 +3882,17 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","Inflammed limb","2021-05-29","2","1",NULL),</v>
+        <v>("4","Inflammed limb","2021-05-29","5","1",0),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3284,17 +3902,22 @@
       <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>44332</v>
+      </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","Bladder Infection",NULL,"7","5",NULL),</v>
+        <v>("5","Bladder Infection","2021-05-16","5","5",0),</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3309,7 +3932,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -3319,7 +3942,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","chronic kidney disease","2021-11-17","6","3","0"),</v>
+        <v>("6","chronic kidney disease","2021-11-17","5","3",0),</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3334,10 +3957,13 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
       <c r="H8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -3346,8 +3972,8 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
-IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),");")</f>
-        <v>("7","Upset Stomach","2021-11-17","3","2",NULL);</v>
+IF(F8="","NULL",_xlfn.CONCAT("",F8,"")),");")</f>
+        <v>("7","Upset Stomach","2021-11-17","4","2",0);</v>
       </c>
     </row>
   </sheetData>
@@ -3417,7 +4043,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1">
         <v>44538</v>
@@ -3435,7 +4061,7 @@
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),",",
 IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
-        <v>("1","Physical exam",NULL,NULL,NULL,"5","2021-12-08","1"),</v>
+        <v>("1","Physical exam",NULL,NULL,NULL,"3","2021-12-08","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -3447,7 +4073,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
         <v>44539</v>
@@ -3456,7 +4082,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J8" ca="1" si="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="J3:J7" ca="1" si="1">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
@@ -3465,7 +4091,7 @@
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),",",
 IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
-        <v>("2","Blood work",NULL,NULL,NULL,"1","2021-12-09","2"),</v>
+        <v>("2","Blood work",NULL,NULL,NULL,"3","2021-12-09","2"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -3477,7 +4103,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1">
         <v>44540</v>
@@ -3487,7 +4113,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Da2pp",NULL,NULL,NULL,"2","2021-12-10","5"),</v>
+        <v>("3","Da2pp",NULL,NULL,NULL,"4","2021-12-10","5"),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -3499,7 +4125,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>44538</v>
@@ -3509,7 +4135,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","dental cleaning",NULL,NULL,NULL,"6","2021-12-08","3"),</v>
+        <v>("4","dental cleaning",NULL,NULL,NULL,"1","2021-12-08","3"),</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -3543,7 +4169,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>44540</v>
@@ -3553,7 +4179,7 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","rabies vaccination",NULL,NULL,NULL,"3","2021-12-10","2"),</v>
+        <v>("6","rabies vaccination",NULL,NULL,NULL,"1","2021-12-10","2"),</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -3565,7 +4191,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1">
         <v>44538</v>
@@ -3583,7 +4209,7 @@
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),",",
 IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),");")</f>
-        <v>("7","Revolution treatment",NULL,NULL,NULL,"2","2021-12-08","4");</v>
+        <v>("7","Revolution treatment",NULL,NULL,NULL,"7","2021-12-08","4");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build: [U888-63] assimilating assignment 6 build to the project
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36941F2D-4EFD-49D2-96E4-AD7AC19D9B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F6858C-DC3F-4D98-B410-7CC0D0474C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,10 @@
     <sheet name="comments" sheetId="2" r:id="rId6"/>
     <sheet name="issues" sheetId="3" r:id="rId7"/>
     <sheet name="treatments" sheetId="4" r:id="rId8"/>
+    <sheet name="requests" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">animals!$A$1:$S$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">animals!$A$1:$T$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="183">
   <si>
     <t>a_animalid</t>
   </si>
@@ -557,6 +558,39 @@
   </si>
   <si>
     <t>neck</t>
+  </si>
+  <si>
+    <t>r_requestid</t>
+  </si>
+  <si>
+    <t>r_animalid</t>
+  </si>
+  <si>
+    <t>r_requester</t>
+  </si>
+  <si>
+    <t>r_requestdate</t>
+  </si>
+  <si>
+    <t>r_requeststatus</t>
+  </si>
+  <si>
+    <t>r_acceptadmindate</t>
+  </si>
+  <si>
+    <t>r_approvedate</t>
+  </si>
+  <si>
+    <t>r_canceldate</t>
+  </si>
+  <si>
+    <t>r_rejectdate</t>
+  </si>
+  <si>
+    <t>r_requestdesc</t>
+  </si>
+  <si>
+    <t>a_requeststatus</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1427,18 +1461,19 @@
     <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1470,33 +1505,36 @@
         <v>10</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="U1" t="str">
+      <c r="V1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO animals (",
 A1,",",
 B1,",",
@@ -1515,12 +1553,13 @@
 O1,",",
 P1,",",
 Q1,",",
-S1,",",
-R1,") VALUES ")</f>
-        <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_species,a_subspecies,a_breed,a_type,a_region,a_sex,a_birthdate,a_status,a_ownerid,a_profilepic,a_tattoonum,a_citytattoo,a_rfidnumber,a_microchipnumber,a_coatcolor,a_distinctfeature,a_continuousmedication) VALUES </v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+R1,",",
+T1,",",
+S1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_species,a_subspecies,a_breed,a_type,a_region,a_sex,a_birthdate,a_status,a_requeststatus,a_ownerid,a_profilepic,a_tattoonum,a_citytattoo,a_rfidnumber,a_microchipnumber,a_coatcolor,a_distinctfeature,a_continuousmedication) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1541,43 +1580,46 @@
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
         <v>43070</v>
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(0,3)</f>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="M2">
+      <c r="N2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>254096526</v>
-      </c>
-      <c r="N2" t="s">
+        <v>286704680</v>
+      </c>
+      <c r="O2" t="s">
         <v>146</v>
-      </c>
-      <c r="O2">
-        <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>325947707</v>
       </c>
       <c r="P2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>252688474</v>
-      </c>
-      <c r="Q2" t="s">
+        <v>200779867</v>
+      </c>
+      <c r="Q2">
+        <f ca="1">RANDBETWEEN(123456789,345678912)</f>
+        <v>300212935</v>
+      </c>
+      <c r="R2" t="s">
         <v>70</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>144</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>145</v>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
 IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
 IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
@@ -1597,11 +1639,12 @@
 IF(P2="","NULL",_xlfn.CONCAT("""",P2,"""")),",",
 IF(Q2="","NULL",_xlfn.CONCAT("""",Q2,"""")),",",
 IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")),",",
-IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")),"),")</f>
-        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","0","2017-12-01","1","1",NULL,"254096526","HOC sha","325947707","252688474","Black","sleeping pills","he can fly"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")),",",
+IF(T2="","NULL",_xlfn.CONCAT("""",T2,"""")),"),")</f>
+        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","1","2017-12-01","2","0","1",NULL,"286704680","HOC sha","200779867","300212935","Black","sleeping pills","he can fly"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1622,41 +1665,44 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H8" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
         <v>43436</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:P8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
-        <v>257238887</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="N3">
+        <f t="shared" ref="N3:Q8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
+        <v>224037195</v>
+      </c>
+      <c r="O3" t="s">
         <v>147</v>
       </c>
-      <c r="O3">
-        <f t="shared" ca="1" si="2"/>
-        <v>337372126</v>
-      </c>
       <c r="P3">
         <f t="shared" ca="1" si="2"/>
-        <v>150999162</v>
-      </c>
-      <c r="Q3" t="s">
+        <v>270458816</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ca="1" si="2"/>
+        <v>219009740</v>
+      </c>
+      <c r="R3" t="s">
         <v>64</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>165</v>
       </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3:U7" ca="1" si="3">_xlfn.CONCAT("(",
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V7" ca="1" si="3">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
@@ -1675,11 +1721,12 @@
 IF(P3="","NULL",_xlfn.CONCAT("""",P3,"""")),",",
 IF(Q3="","NULL",_xlfn.CONCAT("""",Q3,"""")),",",
 IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")),",",
-IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")),"),")</f>
-        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","0","2018-12-02","1","2",NULL,"257238887","ORE esd","337372126","150999162","Brown",NULL,"high jumps"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")),",",
+IF(T3="","NULL",_xlfn.CONCAT("""",T3,"""")),"),")</f>
+        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","1","2018-12-02","3","0","2",NULL,"224037195","ORE esd","270458816","219009740","Brown",NULL,"high jumps"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1707,38 +1754,41 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <f t="shared" ca="1" si="2"/>
-        <v>266851685</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="N4">
+        <f t="shared" ca="1" si="2"/>
+        <v>227479807</v>
+      </c>
+      <c r="O4" t="s">
         <v>148</v>
       </c>
-      <c r="O4">
-        <f t="shared" ca="1" si="2"/>
-        <v>141801485</v>
-      </c>
       <c r="P4">
         <f t="shared" ca="1" si="2"/>
-        <v>229161701</v>
-      </c>
-      <c r="Q4" t="s">
+        <v>271415667</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ca="1" si="2"/>
+        <v>270705876</v>
+      </c>
+      <c r="R4" t="s">
         <v>71</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>166</v>
       </c>
-      <c r="U4" t="str">
+      <c r="V4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","0","2020-04-03","3","1",NULL,"266851685","NKN sds","141801485","229161701","Brown, White",NULL,"bat-shaped patch on face"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","0","2020-04-03","1","0","1",NULL,"227479807","NKN sds","271415667","270705876","Brown, White",NULL,"bat-shaped patch on face"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1759,45 +1809,48 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>43080</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>3</v>
       </c>
-      <c r="M5">
-        <f t="shared" ca="1" si="2"/>
-        <v>220216471</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="N5">
+        <f t="shared" ca="1" si="2"/>
+        <v>232141799</v>
+      </c>
+      <c r="O5" t="s">
         <v>149</v>
       </c>
-      <c r="O5">
-        <f t="shared" ca="1" si="2"/>
-        <v>151163228</v>
-      </c>
       <c r="P5">
         <f t="shared" ca="1" si="2"/>
-        <v>189812256</v>
-      </c>
-      <c r="Q5" t="s">
+        <v>215373589</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ca="1" si="2"/>
+        <v>160639011</v>
+      </c>
+      <c r="R5" t="s">
         <v>72</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>167</v>
       </c>
-      <c r="U5" t="str">
+      <c r="V5" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","1","2017-12-11","2","3",NULL,"220216471","HIS sdm","151163228","189812256","White",NULL,"spotted"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","0","2017-12-11","3","0","3",NULL,"232141799","HIS sdm","215373589","160639011","White",NULL,"spotted"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1818,42 +1871,45 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
         <v>43465</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3</v>
       </c>
-      <c r="M6">
-        <f t="shared" ca="1" si="2"/>
-        <v>243701521</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="N6">
+        <f t="shared" ca="1" si="2"/>
+        <v>126325196</v>
+      </c>
+      <c r="O6" t="s">
         <v>150</v>
       </c>
-      <c r="O6">
-        <f t="shared" ca="1" si="2"/>
-        <v>168003214</v>
-      </c>
       <c r="P6">
         <f t="shared" ca="1" si="2"/>
-        <v>210776146</v>
-      </c>
-      <c r="Q6" t="s">
+        <v>300139197</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ca="1" si="2"/>
+        <v>169573012</v>
+      </c>
+      <c r="R6" t="s">
         <v>72</v>
       </c>
-      <c r="U6" t="str">
+      <c r="V6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","0","2018-12-31","0","3",NULL,"243701521","YSE mlc","168003214","210776146","White",NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","1","2018-12-31","1","0","3",NULL,"126325196","YSE mlc","300139197","169573012","White",NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1874,45 +1930,48 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
         <v>43928</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>4</v>
       </c>
-      <c r="M7">
-        <f t="shared" ca="1" si="2"/>
-        <v>308818670</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="N7">
+        <f t="shared" ca="1" si="2"/>
+        <v>171153107</v>
+      </c>
+      <c r="O7" t="s">
         <v>151</v>
       </c>
-      <c r="O7">
-        <f t="shared" ca="1" si="2"/>
-        <v>129775445</v>
-      </c>
       <c r="P7">
         <f t="shared" ca="1" si="2"/>
-        <v>329563799</v>
-      </c>
-      <c r="Q7" t="s">
+        <v>174511649</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ca="1" si="2"/>
+        <v>295539895</v>
+      </c>
+      <c r="R7" t="s">
         <v>72</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>168</v>
       </c>
-      <c r="U7" t="str">
+      <c r="V7" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","0","2020-04-07","2","4",NULL,"308818670","JSD sda","129775445","329563799","White",NULL,"long ears"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","1","2020-04-07","3","0","4",NULL,"171153107","JSD sda","174511649","295539895","White",NULL,"long ears"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1943,27 +2002,30 @@
         <v>2</v>
       </c>
       <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>3</v>
       </c>
-      <c r="M8">
-        <f t="shared" ca="1" si="2"/>
-        <v>144541305</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="N8">
+        <f t="shared" ca="1" si="2"/>
+        <v>137582509</v>
+      </c>
+      <c r="O8" t="s">
         <v>152</v>
       </c>
-      <c r="O8">
-        <f t="shared" ca="1" si="2"/>
-        <v>238484846</v>
-      </c>
       <c r="P8">
         <f t="shared" ca="1" si="2"/>
-        <v>227949821</v>
-      </c>
-      <c r="Q8" t="s">
+        <v>185233095</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ca="1" si="2"/>
+        <v>188980246</v>
+      </c>
+      <c r="R8" t="s">
         <v>73</v>
       </c>
-      <c r="U8" t="str">
+      <c r="V8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
 IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
 IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
@@ -1983,8 +2045,9 @@
 IF(P8="","NULL",_xlfn.CONCAT("""",P8,"""")),",",
 IF(Q8="","NULL",_xlfn.CONCAT("""",Q8,"""")),",",
 IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")),",",
-IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")),");")</f>
-        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","0","2021-04-03","2","3",NULL,"144541305","DLF kjs","238484846","227949821","Orange",NULL,NULL);</v>
+IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")),",",
+IF(T8="","NULL",_xlfn.CONCAT("""",T8,"""")),");")</f>
+        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","0","2021-04-03","2","0","3",NULL,"137582509","DLF kjs","185233095","188980246","Orange",NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2118,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4039774023</v>
+        <v>4038760918</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F7" si="0">_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
@@ -2073,7 +2136,7 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),"),")</f>
-        <v>("1","Damian","Bruce","Wayne","4039774023","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+        <v>("1","Damian","Bruce","Wayne","4038760918","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2088,7 +2151,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E7" ca="1" si="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4039397251</v>
+        <v>4036743199</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
@@ -2103,7 +2166,7 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),"),")</f>
-        <v>("2","Yorrick",NULL,"Brown","4039397251","yorrick.brown@ucalgary.ca",NULL),</v>
+        <v>("2","Yorrick",NULL,"Brown","4036743199","yorrick.brown@ucalgary.ca",NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2121,7 +2184,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4031810495</v>
+        <v>4036667207</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -2132,7 +2195,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Clark","Joseph","Kent","4031810495","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+        <v>("3","Clark","Joseph","Kent","4036667207","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2144,7 +2207,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>4036232718</v>
+        <v>4039583644</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -2155,7 +2218,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","Tintin",NULL,NULL,"4036232718","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+        <v>("4","Tintin",NULL,NULL,"4039583644","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2167,7 +2230,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>4037061417</v>
+        <v>4032258209</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -2178,7 +2241,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5","UCalgary",NULL,NULL,"4037061417","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+        <v>("5","UCalgary",NULL,NULL,"4032258209","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2193,7 +2256,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4033313504</v>
+        <v>4032375907</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -2211,7 +2274,7 @@
 IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
 IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),",",
 IF(G7="","NULL",_xlfn.CONCAT("""",G7,"""")),");")</f>
-        <v>("6","James",NULL,"Gunn","4033313504","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+        <v>("6","James",NULL,"Gunn","4032375907","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
       </c>
     </row>
   </sheetData>
@@ -2641,7 +2704,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2653,7 +2716,7 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","5","2020-10-01","4","1"),</v>
+        <v>("1","5","2020-10-01","5","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2668,7 +2731,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D29" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2680,7 +2743,7 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","4","2020-10-01","7","2"),</v>
+        <v>("2","4","2020-10-01","5","2"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2695,14 +2758,14 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","30","2020-10-01","6","3"),</v>
+        <v>("3","30","2020-10-01","7","3"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2739,14 +2802,14 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","3","2020-10-01","2","5"),</v>
+        <v>("5","3","2020-10-01","4","5"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2761,14 +2824,14 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","3","2020-10-01","3","6"),</v>
+        <v>("6","3","2020-10-01","7","6"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2810,7 +2873,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2822,7 +2885,7 @@
 IF(C9="","NULL",_xlfn.CONCAT("""",TEXT(C9,"YYYY-MM-DD"),"""")),",",
 IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),",",
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),"),")</f>
-        <v>("8","4","2020-11-03","7","1"),</v>
+        <v>("8","4","2020-11-03","4","1"),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2838,14 +2901,14 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("9","5.2","2020-11-03","1","2"),</v>
+        <v>("9","5.2","2020-11-03","4","2"),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2907,14 +2970,14 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>5</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("12","40.2","2020-11-03","3","5"),</v>
+        <v>("12","40.2","2020-11-03","1","5"),</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2930,14 +2993,14 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>6</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("13","3.2","2020-11-03","6","6"),</v>
+        <v>("13","3.2","2020-11-03","7","6"),</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2953,14 +3016,14 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("14","3.2","2020-11-03","1","7"),</v>
+        <v>("14","3.2","2020-11-03","4","7"),</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2976,14 +3039,14 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("15","0.6","2020-11-29","1","1"),</v>
+        <v>("15","0.6","2020-11-29","5","1"),</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3045,14 +3108,14 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("18","3.8","2020-11-29","3","4"),</v>
+        <v>("18","3.8","2020-11-29","6","4"),</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3091,14 +3154,14 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <v>6</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("20","39.8","2020-11-29","3","6"),</v>
+        <v>("20","39.8","2020-11-29","4","6"),</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3114,14 +3177,14 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>7</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("21","2.8","2020-11-29","4","7"),</v>
+        <v>("21","2.8","2020-11-29","2","7"),</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3137,14 +3200,14 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("22","3.8","2021-02-28","1","1"),</v>
+        <v>("22","3.8","2021-02-28","7","1"),</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3160,14 +3223,14 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("23","1.2","2021-02-28","3","2"),</v>
+        <v>("23","1.2","2021-02-28","7","2"),</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3183,14 +3246,14 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>3</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("24","4.2","2021-02-28","1","3"),</v>
+        <v>("24","4.2","2021-02-28","4","3"),</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3206,14 +3269,14 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("25","5.4","2021-02-28","6","4"),</v>
+        <v>("25","5.4","2021-02-28","5","4"),</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3252,14 +3315,14 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E28">
         <v>6</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("27","30.4","2021-02-28","2","6"),</v>
+        <v>("27","30.4","2021-02-28","5","6"),</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3275,7 +3338,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -3287,7 +3350,7 @@
 IF(C29="","NULL",_xlfn.CONCAT("""",TEXT(C29,"YYYY-MM-DD"),"""")),",",
 IF(D29="","NULL",_xlfn.CONCAT("""",D29,"""")),",",
 IF(E29="","NULL",_xlfn.CONCAT("""",E29,"""")),");")</f>
-        <v>("28","40.4","2021-02-28","2","7");</v>
+        <v>("28","40.4","2021-02-28","7","7");</v>
       </c>
     </row>
   </sheetData>
@@ -3347,7 +3410,7 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
@@ -3371,7 +3434,7 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1",NULL,"2","image1.png","neck","3","2020-10-01"),</v>
+        <v>("1",NULL,"3","image1.png","neck","3","2020-10-01"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3380,14 +3443,14 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>44105</v>
@@ -3401,7 +3464,7 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2",NULL,"5","image2.png",NULL,"2","2020-10-01"),</v>
+        <v>("2",NULL,"6","image2.png",NULL,"1","2020-10-01"),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3410,21 +3473,21 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>102</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <v>44105</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3",NULL,"4","image4.png",NULL,"1","2020-10-01"),</v>
+        <v>("3",NULL,"1","image4.png",NULL,"2","2020-10-01"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3436,18 +3499,18 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
         <v>44105</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","leg broken","1",NULL,NULL,"6","2020-10-01"),</v>
+        <v>("4","leg broken","3",NULL,NULL,"3","2020-10-01"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3456,7 +3519,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>103</v>
@@ -3470,7 +3533,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"3","image7.png",NULL,"4","2020-10-01"),</v>
+        <v>("5",NULL,"1","image7.png",NULL,"4","2020-10-01"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3479,21 +3542,21 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1">
         <v>44105</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"7","image6.png",NULL,"7","2020-10-01"),</v>
+        <v>("6",NULL,"2","image6.png",NULL,"5","2020-10-01"),</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -3502,7 +3565,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>105</v>
@@ -3523,7 +3586,7 @@
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),");")</f>
-        <v>("7",NULL,"7","image5.png",NULL,"7","2020-10-01");</v>
+        <v>("7",NULL,"2","image5.png",NULL,"7","2020-10-01");</v>
       </c>
     </row>
   </sheetData>
@@ -3579,14 +3642,14 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -3595,7 +3658,7 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","Nighttime terror","1","2021-12-08","6"),</v>
+        <v>("1","Nighttime terror","4","2021-12-08","4"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3607,14 +3670,14 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1">
         <v>44539</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
@@ -3623,7 +3686,7 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","Howling ","3","2021-12-09","6"),</v>
+        <v>("2","Howling ","6","2021-12-09","4"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3635,18 +3698,18 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Pregnant ","6","2021-12-10","1"),</v>
+        <v>("3","Pregnant ","7","2021-12-10","6"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3655,18 +3718,18 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4",NULL,"5","2021-12-08","7"),</v>
+        <v>("4",NULL,"2","2021-12-08","1"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3675,18 +3738,18 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"4","2021-12-09","2"),</v>
+        <v>("5",NULL,"6","2021-12-09","3"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3695,18 +3758,18 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"6","2021-12-10","4"),</v>
+        <v>("6",NULL,"7","2021-12-10","3"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3718,7 +3781,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
@@ -3734,7 +3797,7 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",TEXT(D8,"YYYY-MM-DD"),"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),");")</f>
-        <v>("7","Not sleeping","4","2021-12-08","7");</v>
+        <v>("7","Not sleeping","2","2021-12-08","7");</v>
       </c>
     </row>
   </sheetData>
@@ -3798,7 +3861,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3814,7 +3877,7 @@
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("",F2,"")),"),")</f>
-        <v>("1","Limp Walk","2021-12-08","1","1",1),</v>
+        <v>("1","Limp Walk","2021-12-08","2","1",1),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -3826,7 +3889,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3835,14 +3898,14 @@
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H8" ca="1" si="1">_xlfn.CONCAT("(",
+        <f t="shared" ref="H3:H7" ca="1" si="1">_xlfn.CONCAT("(",
 IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
 IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("",F3,"")),"),")</f>
-        <v>("2",NULL,"2020-12-12","1","1",1),</v>
+        <v>("2",NULL,"2020-12-12","4","1",1),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3857,7 +3920,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -3867,7 +3930,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Diabetes","2021-05-16","6","2",0),</v>
+        <v>("3","Diabetes","2021-05-16","3","2",0),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3882,7 +3945,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3892,7 +3955,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","Inflammed limb","2021-05-29","5","1",0),</v>
+        <v>("4","Inflammed limb","2021-05-29","1","1",0),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3907,7 +3970,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -3917,7 +3980,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","Bladder Infection","2021-05-16","5","5",0),</v>
+        <v>("5","Bladder Infection","2021-05-16","2","5",0),</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3957,7 +4020,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -3973,7 +4036,7 @@
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("",F8,"")),");")</f>
-        <v>("7","Upset Stomach","2021-11-17","4","2",0);</v>
+        <v>("7","Upset Stomach","2021-11-17","7","2",0);</v>
       </c>
     </row>
   </sheetData>
@@ -4073,7 +4136,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1">
         <v>44539</v>
@@ -4091,7 +4154,7 @@
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),",",
 IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
-        <v>("2","Blood work",NULL,NULL,NULL,"3","2021-12-09","2"),</v>
+        <v>("2","Blood work",NULL,NULL,NULL,"7","2021-12-09","2"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4103,7 +4166,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1">
         <v>44540</v>
@@ -4113,7 +4176,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Da2pp",NULL,NULL,NULL,"4","2021-12-10","5"),</v>
+        <v>("3","Da2pp",NULL,NULL,NULL,"6","2021-12-10","5"),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4125,7 +4188,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1">
         <v>44538</v>
@@ -4135,7 +4198,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","dental cleaning",NULL,NULL,NULL,"1","2021-12-08","3"),</v>
+        <v>("4","dental cleaning",NULL,NULL,NULL,"6","2021-12-08","3"),</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4147,7 +4210,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
         <v>44539</v>
@@ -4157,7 +4220,7 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","drontal deworm",NULL,NULL,NULL,"4","2021-12-09","4"),</v>
+        <v>("5","drontal deworm",NULL,NULL,NULL,"7","2021-12-09","4"),</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -4169,7 +4232,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>44540</v>
@@ -4179,7 +4242,7 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","rabies vaccination",NULL,NULL,NULL,"1","2021-12-10","2"),</v>
+        <v>("6","rabies vaccination",NULL,NULL,NULL,"3","2021-12-10","2"),</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -4191,7 +4254,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <v>44538</v>
@@ -4209,11 +4272,272 @@
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),",",
 IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),");")</f>
-        <v>("7","Revolution treatment",NULL,NULL,NULL,"7","2021-12-08","4");</v>
+        <v>("7","Revolution treatment",NULL,NULL,NULL,"2","2021-12-08","4");</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F1D254-DAA5-4C45-81E9-439CA656FE0D}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="10" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO requests (",
+A1,",",
+B1,",",
+C1,",",
+D1,",",
+E1,",",
+F1,",",
+G1,",",
+H1,",",
+I1,",",
+J1,") VALUES ")</f>
+        <v xml:space="preserve">INSERT INTO requests (r_requestid,r_requestdesc,r_requeststatus,r_animalid,r_requester,r_requestdate,r_acceptadmindate,r_approvedate,r_canceldate,r_rejectdate) VALUES </v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f ca="1">RANDBETWEEN(1,7)</f>
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="L2" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A2="","NULL",_xlfn.CONCAT("""",A2,"""")),",",
+IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
+IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
+IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
+IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
+IF(F2="","NULL",_xlfn.CONCAT("""",TEXT(F2,"YYYY-MM-DD"),"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),",",
+IF(H2="","NULL",_xlfn.CONCAT("""",TEXT(H2,"YYYY-MM-DD"),"""")),",",
+IF(I2="","NULL",_xlfn.CONCAT("""",TEXT(I2,"YYYY-MM-DD"),"""")),",",
+IF(J2="","NULL",_xlfn.CONCAT("""",TEXT(J2,"YYYY-MM-DD"),"""")),"),")</f>
+        <v>("1",NULL,NULL,"1","3","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" ca="1" si="0">RANDBETWEEN(1,7)</f>
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L7" ca="1" si="2">_xlfn.CONCAT("(",
+IF(A3="","NULL",_xlfn.CONCAT("""",A3,"""")),",",
+IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
+IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
+IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
+IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
+IF(F3="","NULL",_xlfn.CONCAT("""",TEXT(F3,"YYYY-MM-DD"),"""")),",",
+IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),",",
+IF(H3="","NULL",_xlfn.CONCAT("""",TEXT(H3,"YYYY-MM-DD"),"""")),",",
+IF(I3="","NULL",_xlfn.CONCAT("""",TEXT(I3,"YYYY-MM-DD"),"""")),",",
+IF(J3="","NULL",_xlfn.CONCAT("""",TEXT(J3,"YYYY-MM-DD"),"""")),"),")</f>
+        <v>("2",NULL,NULL,"5","4","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="L4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("3",NULL,NULL,"2","2","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("4",NULL,NULL,"1","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("5",NULL,NULL,"4","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>("6",NULL,NULL,"5","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44105</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="L8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(F8="","NULL",_xlfn.CONCAT("""",TEXT(F8,"YYYY-MM-DD"),"""")),",",
+IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),",",
+IF(H8="","NULL",_xlfn.CONCAT("""",TEXT(H8,"YYYY-MM-DD"),"""")),",",
+IF(I8="","NULL",_xlfn.CONCAT("""",TEXT(I8,"YYYY-MM-DD"),"""")),",",
+IF(J8="","NULL",_xlfn.CONCAT("""",TEXT(J8,"YYYY-MM-DD"),"""")),");")</f>
+        <v>("7",NULL,NULL,"7","7","2020-10-01",NULL,NULL,NULL,NULL);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
owner table values added
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-607-608-project\sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarangkumar/Documents/Software/Fall 2021/ENSF607/final-project-uofeng607-888/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F6858C-DC3F-4D98-B410-7CC0D0474C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB417C0-DB3C-C643-8B37-34FAF21F837C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="35540" windowHeight="17360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animals" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="227">
   <si>
     <t>a_animalid</t>
   </si>
@@ -591,6 +589,138 @@
   </si>
   <si>
     <t>a_requeststatus</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Marasco</t>
+  </si>
+  <si>
+    <t>1042 Hope Street, Edmonton AB</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Durant</t>
+  </si>
+  <si>
+    <t>5463 Wallflower Road, San Francisco, CA 90315, USA</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Kyrie</t>
+  </si>
+  <si>
+    <t>Irving</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t>Kailey</t>
+  </si>
+  <si>
+    <t>Camen</t>
+  </si>
+  <si>
+    <t>Hoeld</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Dillon</t>
+  </si>
+  <si>
+    <t>Amber</t>
+  </si>
+  <si>
+    <t>Fair</t>
+  </si>
+  <si>
+    <t>Polinski</t>
+  </si>
+  <si>
+    <t>Gurneet</t>
+  </si>
+  <si>
+    <t>Dhillon</t>
+  </si>
+  <si>
+    <t>Kaur</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Teja</t>
+  </si>
+  <si>
+    <t>Challa</t>
+  </si>
+  <si>
+    <t>Kamika</t>
+  </si>
+  <si>
+    <t>Fukuda</t>
+  </si>
+  <si>
+    <t>Kong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1354 Douglasdale Blvd, Calgary,AB </t>
+  </si>
+  <si>
+    <t>30 Building Way, San Francisco, CA 90315, USA</t>
+  </si>
+  <si>
+    <t>6401 Jasper Ave, Edmonton AB</t>
+  </si>
+  <si>
+    <t>93 Essense Hall, Crawley, London</t>
+  </si>
+  <si>
+    <t>10 Guardian Manor, Fort McMurray, AB</t>
+  </si>
+  <si>
+    <t>172 Silin Forest Road, Fort McMurray, AB</t>
+  </si>
+  <si>
+    <t>2850 Delancey Crescent, San Francisco, CA 904361, USA</t>
+  </si>
+  <si>
+    <t>#401 Arera Colony, Bhopal, MP, India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">326 Ricardo Road, Bogota, Colombia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1792 Camille Street, Medellin, Colombia </t>
+  </si>
+  <si>
+    <t>326 Hamptons Way, Calgary, AB</t>
+  </si>
+  <si>
+    <t>564 Embarcodero Road, San Francisco, CA 953019, USA</t>
   </si>
 </sst>
 </file>
@@ -1447,33 +1577,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1691,7 @@
         <v xml:space="preserve">INSERT INTO animals (a_animalid,a_name,a_species,a_subspecies,a_breed,a_type,a_region,a_sex,a_birthdate,a_status,a_requeststatus,a_ownerid,a_profilepic,a_tattoonum,a_citytattoo,a_rfidnumber,a_microchipnumber,a_coatcolor,a_distinctfeature,a_continuousmedication) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1587,7 +1719,7 @@
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1597,18 +1729,18 @@
       </c>
       <c r="N2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>286704680</v>
+        <v>267709606</v>
       </c>
       <c r="O2" t="s">
         <v>146</v>
       </c>
       <c r="P2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>200779867</v>
+        <v>198386680</v>
       </c>
       <c r="Q2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>300212935</v>
+        <v>140268702</v>
       </c>
       <c r="R2" t="s">
         <v>70</v>
@@ -1641,10 +1773,10 @@
 IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")),",",
 IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")),",",
 IF(T2="","NULL",_xlfn.CONCAT("""",T2,"""")),"),")</f>
-        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","1","2017-12-01","2","0","1",NULL,"286704680","HOC sha","200779867","300212935","Black","sleeping pills","he can fly"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","1","2017-12-01","3","0","1",NULL,"267709606","HOC sha","198386680","140268702","Black","sleeping pills","he can fly"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1672,7 +1804,7 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1682,18 +1814,18 @@
       </c>
       <c r="N3">
         <f t="shared" ref="N3:Q8" ca="1" si="2">RANDBETWEEN(123456789,345678912)</f>
-        <v>224037195</v>
+        <v>160806280</v>
       </c>
       <c r="O3" t="s">
         <v>147</v>
       </c>
       <c r="P3">
         <f t="shared" ca="1" si="2"/>
-        <v>270458816</v>
+        <v>178192806</v>
       </c>
       <c r="Q3">
         <f t="shared" ca="1" si="2"/>
-        <v>219009740</v>
+        <v>307378245</v>
       </c>
       <c r="R3" t="s">
         <v>64</v>
@@ -1723,10 +1855,10 @@
 IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")),",",
 IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")),",",
 IF(T3="","NULL",_xlfn.CONCAT("""",T3,"""")),"),")</f>
-        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","1","2018-12-02","3","0","2",NULL,"224037195","ORE esd","270458816","219009740","Brown",NULL,"high jumps"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","1","2018-12-02","2","0","2",NULL,"160806280","ORE esd","178192806","307378245","Brown",NULL,"high jumps"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1747,14 +1879,14 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1">
         <v>43924</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1764,18 +1896,18 @@
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="2"/>
-        <v>227479807</v>
+        <v>203668024</v>
       </c>
       <c r="O4" t="s">
         <v>148</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="2"/>
-        <v>271415667</v>
+        <v>168908815</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="2"/>
-        <v>270705876</v>
+        <v>163009282</v>
       </c>
       <c r="R4" t="s">
         <v>71</v>
@@ -1785,10 +1917,10 @@
       </c>
       <c r="V4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","0","2020-04-03","1","0","1",NULL,"227479807","NKN sds","271415667","270705876","Brown, White",NULL,"bat-shaped patch on face"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","1","2020-04-03","0","0","1",NULL,"203668024","NKN sds","168908815","163009282","Brown, White",NULL,"bat-shaped patch on face"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1809,14 +1941,14 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>43080</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1826,18 +1958,18 @@
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="2"/>
-        <v>232141799</v>
+        <v>333399701</v>
       </c>
       <c r="O5" t="s">
         <v>149</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="2"/>
-        <v>215373589</v>
+        <v>292993719</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="2"/>
-        <v>160639011</v>
+        <v>150604516</v>
       </c>
       <c r="R5" t="s">
         <v>72</v>
@@ -1847,10 +1979,10 @@
       </c>
       <c r="V5" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","0","2017-12-11","3","0","3",NULL,"232141799","HIS sdm","215373589","160639011","White",NULL,"spotted"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","1","2017-12-11","1","0","3",NULL,"333399701","HIS sdm","292993719","150604516","White",NULL,"spotted"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1878,7 +2010,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1888,28 +2020,28 @@
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="2"/>
-        <v>126325196</v>
+        <v>342080231</v>
       </c>
       <c r="O6" t="s">
         <v>150</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="2"/>
-        <v>300139197</v>
+        <v>334313560</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="2"/>
-        <v>169573012</v>
+        <v>344555022</v>
       </c>
       <c r="R6" t="s">
         <v>72</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","1","2018-12-31","1","0","3",NULL,"126325196","YSE mlc","300139197","169573012","White",NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","1","2018-12-31","2","0","3",NULL,"342080231","YSE mlc","334313560","344555022","White",NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1930,14 +2062,14 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
         <v>43928</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1947,18 +2079,18 @@
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="2"/>
-        <v>171153107</v>
+        <v>335518029</v>
       </c>
       <c r="O7" t="s">
         <v>151</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="2"/>
-        <v>174511649</v>
+        <v>162582635</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="2"/>
-        <v>295539895</v>
+        <v>126720526</v>
       </c>
       <c r="R7" t="s">
         <v>72</v>
@@ -1968,10 +2100,10 @@
       </c>
       <c r="V7" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","1","2020-04-07","3","0","4",NULL,"171153107","JSD sda","174511649","295539895","White",NULL,"long ears"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","0","2020-04-07","2","0","4",NULL,"335518029","JSD sda","162582635","126720526","White",NULL,"long ears"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1992,14 +2124,14 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
         <v>44289</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2009,18 +2141,18 @@
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="2"/>
-        <v>137582509</v>
+        <v>201062209</v>
       </c>
       <c r="O8" t="s">
         <v>152</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="2"/>
-        <v>185233095</v>
+        <v>127757459</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="2"/>
-        <v>188980246</v>
+        <v>259345272</v>
       </c>
       <c r="R8" t="s">
         <v>73</v>
@@ -2047,7 +2179,7 @@
 IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")),",",
 IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")),",",
 IF(T8="","NULL",_xlfn.CONCAT("""",T8,"""")),");")</f>
-        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","0","2021-04-03","2","0","3",NULL,"137582509","DLF kjs","185233095","188980246","Orange",NULL,NULL);</v>
+        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","1","2021-04-03","1","0","3",NULL,"201062209","DLF kjs","127757459","259345272","Orange",NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -2058,18 +2190,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B2892-340A-4DA8-A00C-A7D7ACDCDE8B}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="1" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2103,7 +2237,7 @@
         <v xml:space="preserve">INSERT INTO owners (o_ownerid,o_firstname,o_middlename,o_lastname,o_contactnumber,o_emailid,o_address) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2118,7 +2252,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4038760918</v>
+        <v>4034340123</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F7" si="0">_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
@@ -2136,10 +2270,10 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),"),")</f>
-        <v>("1","Damian","Bruce","Wayne","4038760918","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("1","Damian","Bruce","Wayne","4034340123","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2150,8 +2284,8 @@
         <v>64</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E7" ca="1" si="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4036743199</v>
+        <f t="shared" ref="E3:E20" ca="1" si="1">RANDBETWEEN(4031111111,4039999999)</f>
+        <v>4038832120</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
@@ -2166,10 +2300,10 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),"),")</f>
-        <v>("2","Yorrick",NULL,"Brown","4036743199","yorrick.brown@ucalgary.ca",NULL),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("2","Yorrick",NULL,"Brown","4038832120","yorrick.brown@ucalgary.ca",NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2184,7 +2318,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4036667207</v>
+        <v>4036803045</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -2195,10 +2329,10 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Clark","Joseph","Kent","4036667207","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("3","Clark","Joseph","Kent","4036803045","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2207,7 +2341,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>4039583644</v>
+        <v>4033186450</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -2218,10 +2352,10 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","Tintin",NULL,NULL,"4039583644","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("4","Tintin",NULL,NULL,"4033186450","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2230,7 +2364,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>4032258209</v>
+        <v>4031686732</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -2241,10 +2375,10 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5","UCalgary",NULL,NULL,"4032258209","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("5","UCalgary",NULL,NULL,"4031686732","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2256,7 +2390,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4032375907</v>
+        <v>4038169529</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -2273,11 +2407,432 @@
 IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),",",
 IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
 IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),",",
-IF(G7="","NULL",_xlfn.CONCAT("""",G7,"""")),");")</f>
-        <v>("6","James",NULL,"Gunn","4032375907","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA");</v>
+IF(G7="","NULL",_xlfn.CONCAT("""",G7,"""")),"),")</f>
+        <v>("6","James",NULL,"Gunn","4038169529","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>4036274705</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" ref="F8" si="3">_xlfn.CONCAT(LOWER(B8),IF(C8="","",_xlfn.CONCAT(".",LOWER(C8))),IF(D8="","",_xlfn.CONCAT(".",LOWER(D8))),"@ucalgary.ca")</f>
+        <v>emily.marasco@ucalgary.ca</v>
+      </c>
+      <c r="G8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A8="","NULL",_xlfn.CONCAT("""",A8,"""")),",",
+IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
+IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
+IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
+IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
+IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
+IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),"),")</f>
+        <v>("7","Emily",NULL,"Marasco","4036274705","emily.marasco@ucalgary.ca","1042 Hope Street, Edmonton AB"),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>4039593033</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ref="F9" si="4">_xlfn.CONCAT(LOWER(B9),IF(C9="","",_xlfn.CONCAT(".",LOWER(C9))),IF(D9="","",_xlfn.CONCAT(".",LOWER(D9))),"@ucalgary.ca")</f>
+        <v>kevin.durant@ucalgary.ca</v>
+      </c>
+      <c r="G9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I9" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A9="","NULL",_xlfn.CONCAT("""",A9,"""")),",",
+IF(B9="","NULL",_xlfn.CONCAT("""",B9,"""")),",",
+IF(C9="","NULL",_xlfn.CONCAT("""",C9,"""")),",",
+IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),",",
+IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),",",
+IF(F9="","NULL",_xlfn.CONCAT("""",F9,"""")),",",
+IF(G9="","NULL",_xlfn.CONCAT("""",G9,"""")),"),")</f>
+        <v>("8","Kevin",NULL,"Durant","4039593033","kevin.durant@ucalgary.ca","5463 Wallflower Road, San Francisco, CA 90315, USA"),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>4038453400</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" ref="F10:F12" si="5">_xlfn.CONCAT(LOWER(B10),IF(C10="","",_xlfn.CONCAT(".",LOWER(C10))),IF(D10="","",_xlfn.CONCAT(".",LOWER(D10))),"@ucalgary.ca")</f>
+        <v>jason.kamika.fukuda@ucalgary.ca</v>
+      </c>
+      <c r="G10" t="s">
+        <v>215</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ref="I10:I12" ca="1" si="6">_xlfn.CONCAT("(",
+IF(A10="","NULL",_xlfn.CONCAT("""",A10,"""")),",",
+IF(B10="","NULL",_xlfn.CONCAT("""",B10,"""")),",",
+IF(C10="","NULL",_xlfn.CONCAT("""",C10,"""")),",",
+IF(D10="","NULL",_xlfn.CONCAT("""",D10,"""")),",",
+IF(E10="","NULL",_xlfn.CONCAT("""",E10,"""")),",",
+IF(F10="","NULL",_xlfn.CONCAT("""",F10,"""")),",",
+IF(G10="","NULL",_xlfn.CONCAT("""",G10,"""")),"),")</f>
+        <v>("9","Jason","Kamika","Fukuda","4038453400","jason.kamika.fukuda@ucalgary.ca","1354 Douglasdale Blvd, Calgary,AB "),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>4033251185</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="5"/>
+        <v>jacob.d.brown@ucalgary.ca</v>
+      </c>
+      <c r="G11" t="s">
+        <v>216</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>("10","Jacob","D","Brown","4033251185","jacob.d.brown@ucalgary.ca","30 Building Way, San Francisco, CA 90315, USA"),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="1"/>
+        <v>4036457953</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="5"/>
+        <v>fred.kong@ucalgary.ca</v>
+      </c>
+      <c r="G12" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>("11","Fred",NULL,"Kong","4036457953","fred.kong@ucalgary.ca","6401 Jasper Ave, Edmonton AB"),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="1"/>
+        <v>4034267631</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F20" si="7">_xlfn.CONCAT(LOWER(B13),IF(C13="","",_xlfn.CONCAT(".",LOWER(C13))),IF(D13="","",_xlfn.CONCAT(".",LOWER(D13))),"@ucalgary.ca")</f>
+        <v>kyrie.irving@ucalgary.ca</v>
+      </c>
+      <c r="G13" t="s">
+        <v>218</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ref="I13:I20" ca="1" si="8">_xlfn.CONCAT("(",
+IF(A13="","NULL",_xlfn.CONCAT("""",A13,"""")),",",
+IF(B13="","NULL",_xlfn.CONCAT("""",B13,"""")),",",
+IF(C13="","NULL",_xlfn.CONCAT("""",C13,"""")),",",
+IF(D13="","NULL",_xlfn.CONCAT("""",D13,"""")),",",
+IF(E13="","NULL",_xlfn.CONCAT("""",E13,"""")),",",
+IF(F13="","NULL",_xlfn.CONCAT("""",F13,"""")),",",
+IF(G13="","NULL",_xlfn.CONCAT("""",G13,"""")),"),")</f>
+        <v>("12","Kyrie",NULL,"Irving","4034267631","kyrie.irving@ucalgary.ca","93 Essense Hall, Crawley, London"),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="1"/>
+        <v>4038575607</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="7"/>
+        <v>trinity.hope.smith@ucalgary.ca</v>
+      </c>
+      <c r="G14" t="s">
+        <v>219</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("13","Trinity","Hope","Smith","4038575607","trinity.hope.smith@ucalgary.ca","10 Guardian Manor, Fort McMurray, AB"),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="1"/>
+        <v>4035184239</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="7"/>
+        <v>kailey.camen.hoeld@ucalgary.ca</v>
+      </c>
+      <c r="G15" t="s">
+        <v>220</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("14","Kailey","Camen","Hoeld","4035184239","kailey.camen.hoeld@ucalgary.ca","172 Silin Forest Road, Fort McMurray, AB"),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="1"/>
+        <v>4037769246</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="7"/>
+        <v>elizabeth.price@ucalgary.ca</v>
+      </c>
+      <c r="G16" t="s">
+        <v>221</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("15","Elizabeth",NULL,"Price","4037769246","elizabeth.price@ucalgary.ca","2850 Delancey Crescent, San Francisco, CA 904361, USA"),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="1"/>
+        <v>4035575015</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="7"/>
+        <v>dillon.white@ucalgary.ca</v>
+      </c>
+      <c r="G17" t="s">
+        <v>223</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("16","Dillon",NULL,"White","4035575015","dillon.white@ucalgary.ca","326 Ricardo Road, Bogota, Colombia "),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="1"/>
+        <v>4034502790</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="7"/>
+        <v>amber.fair.polinski@ucalgary.ca</v>
+      </c>
+      <c r="G18" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("17","Amber","Fair","Polinski","4034502790","amber.fair.polinski@ucalgary.ca","1792 Camille Street, Medellin, Colombia "),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>4037535559</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="7"/>
+        <v>gurneet.kaur.dhillon@ucalgary.ca</v>
+      </c>
+      <c r="G19" t="s">
+        <v>222</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("18","Gurneet","Kaur","Dhillon","4037535559","gurneet.kaur.dhillon@ucalgary.ca","#401 Arera Colony, Bhopal, MP, India"),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="1"/>
+        <v>4035812945</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="7"/>
+        <v>ravi.teja.challa@ucalgary.ca</v>
+      </c>
+      <c r="G20" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>("19","Ravi","Teja","Challa","4035812945","ravi.teja.challa@ucalgary.ca","326 Hamptons Way, Calgary, AB"),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" ca="1" si="9">RANDBETWEEN(4031111111,4039999999)</f>
+        <v>4037450149</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" ref="F21" si="10">_xlfn.CONCAT(LOWER(B21),IF(C21="","",_xlfn.CONCAT(".",LOWER(C21))),IF(D21="","",_xlfn.CONCAT(".",LOWER(D21))),"@ucalgary.ca")</f>
+        <v>kevin.durant@ucalgary.ca</v>
+      </c>
+      <c r="G21" t="s">
+        <v>226</v>
+      </c>
+      <c r="I21" t="str">
+        <f ca="1">_xlfn.CONCAT("(",
+IF(A21="","NULL",_xlfn.CONCAT("""",A21,"""")),",",
+IF(B21="","NULL",_xlfn.CONCAT("""",B21,"""")),",",
+IF(C21="","NULL",_xlfn.CONCAT("""",C21,"""")),",",
+IF(D21="","NULL",_xlfn.CONCAT("""",D21,"""")),",",
+IF(E21="","NULL",_xlfn.CONCAT("""",E21,"""")),",",
+IF(F21="","NULL",_xlfn.CONCAT("""",F21,"""")),",",
+IF(G21="","NULL",_xlfn.CONCAT("""",G21,"""")),");")</f>
+        <v>("20","Kevin",NULL,"Durant","4037450149","kevin.durant@ucalgary.ca","564 Embarcodero Road, San Francisco, CA 953019, USA");</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2288,14 +2843,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="10.77734375" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="10.77734375" customWidth="1"/>
+    <col min="1" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -2349,7 +2904,7 @@
         <v xml:space="preserve">INSERT INTO users (u_userid,u_joiningdate,u_activationdate,u_terminationdate,u_firstname,u_middlename,u_lastname,u_role,u_emailid,u_passwordhash,u_passwordsalt,u_status) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2397,7 +2952,7 @@
         <v>("1","2017-12-01","2017-12-02",NULL,"Greg",NULL,"Boorman","0","greg.boorman@ucalgary.ca","passw0rd",NULL,"1"),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2445,7 +3000,7 @@
         <v>("2","2018-12-02","2018-12-03",NULL,"Teacher",NULL,"Admin","0","teacher.admin@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2481,7 +3036,7 @@
         <v>("3","2020-04-03","2020-04-04",NULL,"Technician",NULL,"A","2","technician.a@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2517,7 +3072,7 @@
         <v>("4","2017-12-11","2017-12-12",NULL,"Attendant",NULL,"B","1","attendant.b@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2556,7 +3111,7 @@
         <v>("5","2018-12-31","2019-01-01","2021-09-27","Teacher",NULL,"C","3","teacher.c@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2595,7 +3150,7 @@
         <v>("6","2020-04-07","2020-04-08","2023-01-03","Student",NULL,"D","4","student.d@ucalgary.ca","passw0rd",NULL,"0"),</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2655,18 +3210,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3D06D0-BF1F-4225-AF4B-50DA628F29F9}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
@@ -2692,7 +3247,7 @@
         <v xml:space="preserve">INSERT INTO weights (w_weightid,w_massinkg,w_recorddate,w_recordedby,w_animalid) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2704,7 +3259,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2716,10 +3271,10 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","5","2020-10-01","5","1"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("1","5","2020-10-01","6","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2731,7 +3286,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D29" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2743,10 +3298,10 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","4","2020-10-01","5","2"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("2","4","2020-10-01","6","2"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2768,7 +3323,7 @@
         <v>("3","30","2020-10-01","7","3"),</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2780,17 +3335,17 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","40","2020-10-01","6","4"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("4","40","2020-10-01","5","4"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2802,17 +3357,17 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","3","2020-10-01","4","5"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("5","3","2020-10-01","7","5"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2824,17 +3379,17 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","3","2020-10-01","7","6"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("6","3","2020-10-01","5","6"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2846,7 +3401,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -2858,10 +3413,10 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"),")</f>
-        <v>("7","1","2020-10-01","1","7"),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("7","1","2020-10-01","2","7"),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2873,7 +3428,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2885,10 +3440,10 @@
 IF(C9="","NULL",_xlfn.CONCAT("""",TEXT(C9,"YYYY-MM-DD"),"""")),",",
 IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),",",
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),"),")</f>
-        <v>("8","4","2020-11-03","4","1"),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("8","4","2020-11-03","7","1"),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2901,17 +3456,17 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("9","5.2","2020-11-03","4","2"),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("9","5.2","2020-11-03","2","2"),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2924,17 +3479,17 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("10","4.2","2020-11-03","3","3"),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("10","4.2","2020-11-03","5","3"),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2947,17 +3502,17 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("11","30.2","2020-11-03","6","4"),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("11","30.2","2020-11-03","4","4"),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2970,17 +3525,17 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <v>5</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("12","40.2","2020-11-03","1","5"),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("12","40.2","2020-11-03","6","5"),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2993,17 +3548,17 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>6</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("13","3.2","2020-11-03","7","6"),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("13","3.2","2020-11-03","3","6"),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3016,17 +3571,17 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("14","3.2","2020-11-03","4","7"),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("14","3.2","2020-11-03","5","7"),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3049,7 +3604,7 @@
         <v>("15","0.6","2020-11-29","5","1"),</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3062,17 +3617,17 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("16","3.6","2020-11-29","3","2"),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("16","3.6","2020-11-29","6","2"),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3085,17 +3640,17 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("17","4.8","2020-11-29","3","3"),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("17","4.8","2020-11-29","1","3"),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3108,17 +3663,17 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("18","3.8","2020-11-29","6","4"),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("18","3.8","2020-11-29","5","4"),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3131,17 +3686,17 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("19","29.8","2020-11-29","3","5"),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("19","29.8","2020-11-29","5","5"),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3154,17 +3709,17 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <v>6</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("20","39.8","2020-11-29","4","6"),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("20","39.8","2020-11-29","2","6"),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3177,17 +3732,17 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E22">
         <v>7</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("21","2.8","2020-11-29","2","7"),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("21","2.8","2020-11-29","6","7"),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3200,17 +3755,17 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("22","3.8","2021-02-28","7","1"),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("22","3.8","2021-02-28","6","1"),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3233,7 +3788,7 @@
         <v>("23","1.2","2021-02-28","7","2"),</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3256,7 +3811,7 @@
         <v>("24","4.2","2021-02-28","4","3"),</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3269,17 +3824,17 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("25","5.4","2021-02-28","5","4"),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("25","5.4","2021-02-28","6","4"),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3302,7 +3857,7 @@
         <v>("26","4.4","2021-02-28","1","5"),</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3315,17 +3870,17 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>6</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("27","30.4","2021-02-28","5","6"),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("27","30.4","2021-02-28","1","6"),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3338,7 +3893,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -3350,7 +3905,7 @@
 IF(C29="","NULL",_xlfn.CONCAT("""",TEXT(C29,"YYYY-MM-DD"),"""")),",",
 IF(D29="","NULL",_xlfn.CONCAT("""",D29,"""")),",",
 IF(E29="","NULL",_xlfn.CONCAT("""",E29,"""")),");")</f>
-        <v>("28","40.4","2021-02-28","7","7");</v>
+        <v>("28","40.4","2021-02-28","4","7");</v>
       </c>
     </row>
   </sheetData>
@@ -3365,12 +3920,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="10.77734375" customWidth="1"/>
+    <col min="1" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -3404,13 +3959,13 @@
         <v xml:space="preserve">INSERT INTO photos (p_photoid,p_photodesc,p_animalid,p_photolink,p_alttext,p_uploader,p_uploaddate) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
@@ -3420,7 +3975,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>44105</v>
@@ -3434,23 +3989,23 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1",NULL,"3","image1.png","neck","3","2020-10-01"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("1",NULL,"7","image1.png","neck","1","2020-10-01"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1">
         <v>44105</v>
@@ -3464,33 +4019,33 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2",NULL,"6","image2.png",NULL,"1","2020-10-01"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("2",NULL,"1","image2.png",NULL,"4","2020-10-01"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>102</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1">
         <v>44105</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3",NULL,"1","image4.png",NULL,"2","2020-10-01"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("3",NULL,"7","image4.png",NULL,"3","2020-10-01"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3499,80 +4054,80 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1">
         <v>44105</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","leg broken","3",NULL,NULL,"3","2020-10-01"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("4","leg broken","2",NULL,NULL,"6","2020-10-01"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>103</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1">
         <v>44105</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"1","image7.png",NULL,"4","2020-10-01"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("5",NULL,"5","image7.png",NULL,"3","2020-10-01"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>44105</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"2","image6.png",NULL,"5","2020-10-01"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>("6",NULL,"7","image6.png",NULL,"1","2020-10-01"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>105</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1">
         <v>44105</v>
@@ -3586,7 +4141,7 @@
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),");")</f>
-        <v>("7",NULL,"2","image5.png",NULL,"7","2020-10-01");</v>
+        <v>("7",NULL,"7","image5.png",NULL,"3","2020-10-01");</v>
       </c>
     </row>
   </sheetData>
@@ -3600,14 +4155,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -3633,7 +4188,7 @@
         <v xml:space="preserve">INSERT INTO comments (c_commentid,c_commentdesc,c_animalid,c_commentdate,c_commenter) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3642,7 +4197,7 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
@@ -3658,10 +4213,10 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","Nighttime terror","4","2021-12-08","4"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("1","Nighttime terror","7","2021-12-08","4"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3677,7 +4232,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
@@ -3686,10 +4241,10 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","Howling ","6","2021-12-09","4"),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("2","Howling ","6","2021-12-09","3"),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3705,74 +4260,74 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Pregnant ","7","2021-12-10","6"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("3","Pregnant ","7","2021-12-10","3"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4",NULL,"2","2021-12-08","1"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("4",NULL,"4","2021-12-08","4"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"6","2021-12-09","3"),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("5",NULL,"1","2021-12-09","5"),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"7","2021-12-10","3"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>("6",NULL,"2","2021-12-10","4"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3781,14 +4336,14 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>44538</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -3797,7 +4352,7 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",TEXT(D8,"YYYY-MM-DD"),"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),");")</f>
-        <v>("7","Not sleeping","2","2021-12-08","7");</v>
+        <v>("7","Not sleeping","6","2021-12-08","5");</v>
       </c>
     </row>
   </sheetData>
@@ -3811,15 +4366,15 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="6" width="10.77734375" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +4404,7 @@
         <v xml:space="preserve">INSERT INTO issues (i_issueid,i_issuedesc,i_detecteddate,i_animalid,i_raisedby,i_isresolved) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3861,7 +4416,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3877,10 +4432,10 @@
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("",F2,"")),"),")</f>
-        <v>("1","Limp Walk","2021-12-08","2","1",1),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>("1","Limp Walk","2021-12-08","1","1",1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3908,7 +4463,7 @@
         <v>("2",NULL,"2020-12-12","4","1",1),</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3920,7 +4475,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -3930,10 +4485,10 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Diabetes","2021-05-16","3","2",0),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>("3","Diabetes","2021-05-16","1","2",0),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3945,7 +4500,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3955,10 +4510,10 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","Inflammed limb","2021-05-29","1","1",0),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>("4","Inflammed limb","2021-05-29","4","1",0),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3970,7 +4525,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -3980,10 +4535,10 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","Bladder Infection","2021-05-16","2","5",0),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>("5","Bladder Infection","2021-05-16","3","5",0),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3995,7 +4550,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -4005,10 +4560,10 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","chronic kidney disease","2021-11-17","5","3",0),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>("6","chronic kidney disease","2021-11-17","2","3",0),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4050,16 +4605,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="2" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -4097,7 +4652,7 @@
         <v xml:space="preserve">INSERT INTO treatments (t_treatmentid,t_treatmentdesc,t_drugname,t_drugdose,t_deliverymethod,t_animalid,t_treatmentdate,t_treatedby) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4106,7 +4661,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1">
         <v>44538</v>
@@ -4124,10 +4679,10 @@
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),",",
 IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
-        <v>("1","Physical exam",NULL,NULL,NULL,"3","2021-12-08","1"),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>("1","Physical exam",NULL,NULL,NULL,"7","2021-12-08","1"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4157,7 +4712,7 @@
         <v>("2","Blood work",NULL,NULL,NULL,"7","2021-12-09","2"),</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4166,7 +4721,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1">
         <v>44540</v>
@@ -4176,10 +4731,10 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Da2pp",NULL,NULL,NULL,"6","2021-12-10","5"),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>("3","Da2pp",NULL,NULL,NULL,"7","2021-12-10","5"),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4188,7 +4743,7 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>44538</v>
@@ -4198,10 +4753,10 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","dental cleaning",NULL,NULL,NULL,"6","2021-12-08","3"),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>("4","dental cleaning",NULL,NULL,NULL,"1","2021-12-08","3"),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4223,7 +4778,7 @@
         <v>("5","drontal deworm",NULL,NULL,NULL,"7","2021-12-09","4"),</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4232,7 +4787,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1">
         <v>44540</v>
@@ -4242,10 +4797,10 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","rabies vaccination",NULL,NULL,NULL,"3","2021-12-10","2"),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>("6","rabies vaccination",NULL,NULL,NULL,"2","2021-12-10","2"),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4287,12 +4842,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="10.77734375" customWidth="1"/>
+    <col min="1" max="10" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
@@ -4338,7 +4893,7 @@
         <v xml:space="preserve">INSERT INTO requests (r_requestid,r_requestdesc,r_requeststatus,r_animalid,r_requester,r_requestdate,r_acceptadmindate,r_approvedate,r_canceldate,r_rejectdate) VALUES </v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4348,7 +4903,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1">
         <v>44105</v>
@@ -4369,20 +4924,20 @@
 IF(H2="","NULL",_xlfn.CONCAT("""",TEXT(H2,"YYYY-MM-DD"),"""")),",",
 IF(I2="","NULL",_xlfn.CONCAT("""",TEXT(I2,"YYYY-MM-DD"),"""")),",",
 IF(J2="","NULL",_xlfn.CONCAT("""",TEXT(J2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1",NULL,NULL,"1","3","2020-10-01",NULL,NULL,NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>("1",NULL,NULL,"1","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
         <v>44105</v>
@@ -4403,10 +4958,10 @@
 IF(H3="","NULL",_xlfn.CONCAT("""",TEXT(H3,"YYYY-MM-DD"),"""")),",",
 IF(I3="","NULL",_xlfn.CONCAT("""",TEXT(I3,"YYYY-MM-DD"),"""")),",",
 IF(J3="","NULL",_xlfn.CONCAT("""",TEXT(J3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2",NULL,NULL,"5","4","2020-10-01",NULL,NULL,NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>("2",NULL,NULL,"2","5","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4416,7 +4971,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1">
         <v>44105</v>
@@ -4427,16 +4982,16 @@
       <c r="J4" s="1"/>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3",NULL,NULL,"2","2","2020-10-01",NULL,NULL,NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>("3",NULL,NULL,"2","3","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -4451,10 +5006,10 @@
       <c r="J5" s="1"/>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4",NULL,NULL,"1","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>("4",NULL,NULL,"4","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4464,7 +5019,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
         <v>44105</v>
@@ -4475,20 +5030,20 @@
       <c r="J6" s="1"/>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,NULL,"4","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>("5",NULL,NULL,"4","2","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1">
         <v>44105</v>
@@ -4499,20 +5054,20 @@
       <c r="J7" s="1"/>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,NULL,"5","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>("6",NULL,NULL,"3","4","2020-10-01",NULL,NULL,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1">
         <v>44105</v>
@@ -4533,7 +5088,7 @@
 IF(H8="","NULL",_xlfn.CONCAT("""",TEXT(H8,"YYYY-MM-DD"),"""")),",",
 IF(I8="","NULL",_xlfn.CONCAT("""",TEXT(I8,"YYYY-MM-DD"),"""")),",",
 IF(J8="","NULL",_xlfn.CONCAT("""",TEXT(J8,"YYYY-MM-DD"),"""")),");")</f>
-        <v>("7",NULL,NULL,"7","7","2020-10-01",NULL,NULL,NULL,NULL);</v>
+        <v>("7",NULL,NULL,"2","2","2020-10-01",NULL,NULL,NULL,NULL);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore:[U888-62] added commenting for easy read
</commit_message>
<xml_diff>
--- a/sql/04_dummy_data_generator.xlsx
+++ b/sql/04_dummy_data_generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarangkumar/Documents/Software/Fall 2021/ENSF607/final-project-uofeng607-888/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771E020A-3EF4-164A-92AE-CEE8BC59C061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5306FBFD-2B44-134E-AB14-36DE9DECA595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26640" windowHeight="15320" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26640" windowHeight="15320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animals" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="326">
   <si>
     <t>a_animalid</t>
   </si>
@@ -1011,17 +1011,20 @@
     <t>injection</t>
   </si>
   <si>
-    <t>Note: For the 20th value - all values are empty strings unless shown above. For the 19th value, all values are NULL unless shown above.</t>
-  </si>
-  <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Note: For the 20th value - all values are empty strings unless shown above. (If there is value in 20th tuple, it is absolutely required). For the 19th value, all values are NULL unless shown above.</t>
+  </si>
+  <si>
+    <t>Note: For the 30th value - all values are empty strings unless shown above. (If there is value in 30th tuple, it is absolutely required). For the 29th value, all values are NULL unless shown above.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1158,6 +1161,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1510,10 +1520,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1872,7 +1883,7 @@
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2013,29 +2024,29 @@
       </c>
       <c r="J2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>305659665</v>
+        <v>198266560</v>
       </c>
       <c r="O2" t="s">
         <v>146</v>
       </c>
       <c r="P2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>181323639</v>
+        <v>328526719</v>
       </c>
       <c r="Q2">
         <f ca="1">RANDBETWEEN(123456789,345678912)</f>
-        <v>217715861</v>
+        <v>226206061</v>
       </c>
       <c r="R2" t="s">
         <v>70</v>
@@ -2068,7 +2079,7 @@
 IF(R2="","NULL",_xlfn.CONCAT("""",R2,"""")),",",
 IF(S2="","NULL",_xlfn.CONCAT("""",S2,"""")),",",
 IF(T2="","NULL",_xlfn.CONCAT("""",T2,"""")),"),")</f>
-        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","0","2017-12-01","3","0","10",NULL,"305659665","HOC sha","181323639","217715861","Black","sleeping pills","he can fly"),</v>
+        <v>("1","Ace","Dog","Canine","German shepherd",NULL,"Spain","0","2017-12-01","2","0","8",NULL,"198266560","HOC sha","328526719","226206061","Black","sleeping pills","he can fly"),</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -2092,36 +2103,36 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H19" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
         <v>43436</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J20" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:M20" ca="1" si="2">RANDBETWEEN(1,18)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:Q18" ca="1" si="3">RANDBETWEEN(123456789,345678912)</f>
-        <v>177894699</v>
+        <v>248308846</v>
       </c>
       <c r="O3" t="s">
         <v>147</v>
       </c>
       <c r="P3">
         <f t="shared" ca="1" si="3"/>
-        <v>325762777</v>
+        <v>303129593</v>
       </c>
       <c r="Q3">
         <f t="shared" ca="1" si="3"/>
-        <v>148795169</v>
+        <v>225613938</v>
       </c>
       <c r="R3" t="s">
         <v>64</v>
@@ -2151,7 +2162,7 @@
 IF(R3="","NULL",_xlfn.CONCAT("""",R3,"""")),",",
 IF(S3="","NULL",_xlfn.CONCAT("""",S3,"""")),",",
 IF(T3="","NULL",_xlfn.CONCAT("""",T3,"""")),"),")</f>
-        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","0","2018-12-02","3","0","13",NULL,"177894699","ORE esd","325762777","148795169","Brown",NULL,"high jumps"),</v>
+        <v>("2","Ampersand","Monkey","Ape","Capuchin monkey",NULL,"France","1","2018-12-02","2","0","16",NULL,"248308846","ORE esd","303129593","225613938","Brown",NULL,"high jumps"),</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -2182,29 +2193,29 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="3"/>
-        <v>217650536</v>
+        <v>192792825</v>
       </c>
       <c r="O4" t="s">
         <v>148</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="3"/>
-        <v>154740224</v>
+        <v>267338576</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="3"/>
-        <v>221696816</v>
+        <v>283667278</v>
       </c>
       <c r="R4" t="s">
         <v>71</v>
@@ -2214,7 +2225,7 @@
       </c>
       <c r="V4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","1","2020-04-03","2","0","12",NULL,"217650536","NKN sds","154740224","221696816","Brown, White",NULL,"bat-shaped patch on face"),</v>
+        <v>("3","Bat Cow","Cow","Bovine",NULL,"Dairy","US","1","2020-04-03","1","0","9",NULL,"192792825","NKN sds","267338576","283667278","Brown, White",NULL,"bat-shaped patch on face"),</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -2245,29 +2256,29 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="3"/>
-        <v>223858725</v>
+        <v>271547584</v>
       </c>
       <c r="O5" t="s">
         <v>149</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="3"/>
-        <v>129122686</v>
+        <v>282981564</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="3"/>
-        <v>234141801</v>
+        <v>163322638</v>
       </c>
       <c r="R5" t="s">
         <v>72</v>
@@ -2280,7 +2291,7 @@
       </c>
       <c r="V5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","1","2017-12-11","0","0","18",NULL,"223858725","HIS sdm","129122686","234141801","White","heart medication","spotted"),</v>
+        <v>("4","Comet","Horse","Gallopping","Canadian horse",NULL,"Canada","1","2017-12-11","2","0","15",NULL,"271547584","HIS sdm","282981564","163322638","White","heart medication","spotted"),</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -2304,43 +2315,43 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>43465</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="3"/>
-        <v>146806063</v>
+        <v>206677521</v>
       </c>
       <c r="O6" t="s">
         <v>150</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="3"/>
-        <v>327429098</v>
+        <v>221839152</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="3"/>
-        <v>329353977</v>
+        <v>224078570</v>
       </c>
       <c r="R6" t="s">
         <v>72</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","1","2018-12-31","2","0","12",NULL,"146806063","YSE mlc","327429098","329353977","White",NULL,NULL),</v>
+        <v>("5","Krypto","Dog","Canine","Labrador retriever",NULL,"Africa","0","2018-12-31","1","0","11",NULL,"206677521","YSE mlc","221839152","224078570","White",NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -2364,36 +2375,36 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
         <v>43928</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="3"/>
-        <v>235232233</v>
+        <v>147192505</v>
       </c>
       <c r="O7" t="s">
         <v>151</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="3"/>
-        <v>133389272</v>
+        <v>163675896</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="3"/>
-        <v>303031362</v>
+        <v>294072243</v>
       </c>
       <c r="R7" t="s">
         <v>72</v>
@@ -2406,7 +2417,7 @@
       </c>
       <c r="V7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","0","2020-04-07","2","0","10",NULL,"235232233","JSD sda","133389272","303031362","White","ACE Inhibitors","long ears"),</v>
+        <v>("6","Snowy","Dog","Canine","Wire Fox Terrier",NULL,"London","1","2020-04-07","3","0","9",NULL,"147192505","JSD sda","163675896","294072243","White","ACE Inhibitors","long ears"),</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -2430,36 +2441,36 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
         <v>44289</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="3"/>
-        <v>153618423</v>
+        <v>138283254</v>
       </c>
       <c r="O8" t="s">
         <v>152</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="3"/>
-        <v>268316292</v>
+        <v>139803432</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="3"/>
-        <v>256634316</v>
+        <v>289219833</v>
       </c>
       <c r="R8" t="s">
         <v>73</v>
@@ -2492,7 +2503,7 @@
 IF(R8="","NULL",_xlfn.CONCAT("""",R8,"""")),",",
 IF(S8="","NULL",_xlfn.CONCAT("""",S8,"""")),",",
 IF(T8="","NULL",_xlfn.CONCAT("""",T8,"""")),"),")</f>
-        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","1","2021-04-03","3","0","4",NULL,"153618423","DLF kjs","268316292","256634316","Orange","chronic painkillers","he can fly"),</v>
+        <v>("7","Streaky","Cat","Feline","Abyssinian",NULL,"Rome","0","2021-04-03","0","0","12",NULL,"138283254","DLF kjs","139803432","289219833","Orange","chronic painkillers","he can fly"),</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
@@ -2516,36 +2527,36 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
         <v>43194</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="3"/>
-        <v>160373627</v>
+        <v>152219464</v>
       </c>
       <c r="O9" t="s">
         <v>261</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="3"/>
-        <v>183608516</v>
+        <v>292583305</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="3"/>
-        <v>234840196</v>
+        <v>230614915</v>
       </c>
       <c r="R9" t="s">
         <v>70</v>
@@ -2575,7 +2586,7 @@
 IF(R9="","NULL",_xlfn.CONCAT("""",R9,"""")),",",
 IF(S9="","NULL",_xlfn.CONCAT("""",S9,"""")),",",
 IF(T9="","NULL",_xlfn.CONCAT("""",T9,"""")),"),")</f>
-        <v>("8","Fluffy","Monkey","Ape","Marmoset",NULL,"London","0","2018-04-04","2","0","1",NULL,"160373627","LEM skd","183608516","234840196","Black",NULL,"high jumps"),</v>
+        <v>("8","Fluffy","Monkey","Ape","Marmoset",NULL,"London","1","2018-04-04","3","0","12",NULL,"152219464","LEM skd","292583305","230614915","Black",NULL,"high jumps"),</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -2606,29 +2617,29 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="3"/>
-        <v>288512551</v>
+        <v>162991522</v>
       </c>
       <c r="O10" t="s">
         <v>262</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="3"/>
-        <v>134324801</v>
+        <v>309156238</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="3"/>
-        <v>300725737</v>
+        <v>125793326</v>
       </c>
       <c r="R10" t="s">
         <v>64</v>
@@ -2638,7 +2649,7 @@
       </c>
       <c r="V10" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("9","Yogi","Dog","Lupus","Pomeranian",NULL,"London","0","2019-04-05","3","0","14",NULL,"288512551","DKD dks","134324801","300725737","Brown",NULL,"bat-shaped patch on face"),</v>
+        <v>("9","Yogi","Dog","Lupus","Pomeranian",NULL,"London","0","2019-04-05","0","0","13",NULL,"162991522","DKD dks","309156238","125793326","Brown",NULL,"bat-shaped patch on face"),</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -2662,36 +2673,36 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
         <v>44292</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="3"/>
-        <v>312735505</v>
+        <v>158328823</v>
       </c>
       <c r="O11" t="s">
         <v>263</v>
       </c>
       <c r="P11">
         <f t="shared" ca="1" si="3"/>
-        <v>235669109</v>
+        <v>330374448</v>
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="3"/>
-        <v>320007534</v>
+        <v>179052189</v>
       </c>
       <c r="R11" t="s">
         <v>71</v>
@@ -2704,7 +2715,7 @@
       </c>
       <c r="V11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("10","Hari","Dog","Lupus","Poodle",NULL,"India","1","2021-04-06","3","0","15",NULL,"312735505","DKE kwl","235669109","320007534","Brown, White","SSRIs","spotted"),</v>
+        <v>("10","Hari","Dog","Lupus","Poodle",NULL,"India","0","2021-04-06","1","0","9",NULL,"158328823","DKE kwl","330374448","179052189","Brown, White","SSRIs","spotted"),</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -2735,29 +2746,29 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="3"/>
-        <v>151688909</v>
+        <v>211290913</v>
       </c>
       <c r="O12" t="s">
         <v>264</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="3"/>
-        <v>306180459</v>
+        <v>240925269</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="3"/>
-        <v>272071843</v>
+        <v>328418942</v>
       </c>
       <c r="R12" t="s">
         <v>72</v>
@@ -2767,7 +2778,7 @@
       </c>
       <c r="V12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("11","Mocha","Monkey","Ape","Baboon",NULL,"China","1","2020-04-07","0","0","7",NULL,"151688909","KDF ker","306180459","272071843","White","sleeping pills",NULL),</v>
+        <v>("11","Mocha","Monkey","Ape","Baboon",NULL,"China","1","2020-04-07","2","0","6",NULL,"211290913","KDF ker","240925269","328418942","White","sleeping pills",NULL),</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -2791,36 +2802,36 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <v>44294</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="3"/>
-        <v>189362967</v>
+        <v>141013132</v>
       </c>
       <c r="O13" t="s">
         <v>265</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="3"/>
-        <v>130132448</v>
+        <v>343921393</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="3"/>
-        <v>279912228</v>
+        <v>155220280</v>
       </c>
       <c r="R13" t="s">
         <v>72</v>
@@ -2830,7 +2841,7 @@
       </c>
       <c r="V13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("12","Pika","Cow","Zebu","Limousin",NULL,"Rome","1","2021-04-08","0","0","10",NULL,"189362967","ERL ker","130132448","279912228","White",NULL,"long ears"),</v>
+        <v>("12","Pika","Cow","Zebu","Limousin",NULL,"Rome","0","2021-04-08","1","0","17",NULL,"141013132","ERL ker","343921393","155220280","White",NULL,"long ears"),</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -2861,29 +2872,29 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="3"/>
-        <v>151876758</v>
+        <v>151470806</v>
       </c>
       <c r="O14" t="s">
         <v>266</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="3"/>
-        <v>153273531</v>
+        <v>211839160</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="3"/>
-        <v>234357451</v>
+        <v>341331290</v>
       </c>
       <c r="R14" t="s">
         <v>72</v>
@@ -2893,7 +2904,7 @@
       </c>
       <c r="V14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("13","Chewey","Dog","Canine","Chihuahua",NULL,"Rome","1","2021-04-09","2","0","15",NULL,"151876758","WEA wle","153273531","234357451","White",NULL,"he can fly"),</v>
+        <v>("13","Chewey","Dog","Canine","Chihuahua",NULL,"Rome","1","2021-04-09","1","0","1",NULL,"151470806","WEA wle","211839160","341331290","White",NULL,"he can fly"),</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -2917,7 +2928,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>44296</v>
@@ -2931,22 +2942,22 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="3"/>
-        <v>284608689</v>
+        <v>268715623</v>
       </c>
       <c r="O15" t="s">
         <v>267</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="3"/>
-        <v>284754815</v>
+        <v>233425283</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="3"/>
-        <v>313259625</v>
+        <v>157063652</v>
       </c>
       <c r="R15" t="s">
         <v>73</v>
@@ -2959,7 +2970,7 @@
       </c>
       <c r="V15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("14","Sir Eric","Horse","Tarpan","Shire",NULL,"Canada","1","2021-04-10","2","0","15",NULL,"284608689","VJD dfw","284754815","313259625","Orange","heart medication","high jumps"),</v>
+        <v>("14","Sir Eric","Horse","Tarpan","Shire",NULL,"Canada","0","2021-04-10","2","0","6",NULL,"268715623","VJD dfw","233425283","157063652","Orange","heart medication","high jumps"),</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -2983,7 +2994,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
         <v>44419</v>
@@ -2997,22 +3008,22 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="3"/>
-        <v>286724543</v>
+        <v>171873389</v>
       </c>
       <c r="O16" t="s">
         <v>268</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="3"/>
-        <v>300655221</v>
+        <v>330271818</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="3"/>
-        <v>276338698</v>
+        <v>188942930</v>
       </c>
       <c r="R16" t="s">
         <v>70</v>
@@ -3022,7 +3033,7 @@
       </c>
       <c r="V16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("15","Boomer","Horse","Tarpan","Arabian",NULL,"US","1","2021-08-11","2","0","2",NULL,"286724543","SLD wel","300655221","276338698","Black",NULL,"bat-shaped patch on face"),</v>
+        <v>("15","Boomer","Horse","Tarpan","Arabian",NULL,"US","0","2021-08-11","2","0","7",NULL,"171873389","SLD wel","330271818","188942930","Black",NULL,"bat-shaped patch on face"),</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -3046,36 +3057,36 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1">
         <v>44295</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="3"/>
-        <v>290511886</v>
+        <v>271808978</v>
       </c>
       <c r="O17" t="s">
         <v>269</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="3"/>
-        <v>288186653</v>
+        <v>222819986</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="3"/>
-        <v>302286981</v>
+        <v>226423794</v>
       </c>
       <c r="R17" t="s">
         <v>64</v>
@@ -3088,7 +3099,7 @@
       </c>
       <c r="V17" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("16","Kitty","Cat","Feline","Persian",NULL,"London","0","2021-04-09","3","0","16",NULL,"290511886","JLI oih","288186653","302286981","Brown","ACE Inhibitors","spotted"),</v>
+        <v>("16","Kitty","Cat","Feline","Persian",NULL,"London","1","2021-04-09","2","0","7",NULL,"271808978","JLI oih","222819986","226423794","Brown","ACE Inhibitors","spotted"),</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -3112,36 +3123,36 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1">
         <v>43571</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="3"/>
-        <v>323883836</v>
+        <v>124599931</v>
       </c>
       <c r="O18" t="s">
         <v>270</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="3"/>
-        <v>272119884</v>
+        <v>147292852</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="3"/>
-        <v>187162355</v>
+        <v>334167743</v>
       </c>
       <c r="R18" t="s">
         <v>71</v>
@@ -3151,7 +3162,7 @@
       </c>
       <c r="V18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("17","Brewster","Dog","Canine","Golden Retriever",NULL,"Spain","1","2019-04-16","1","0","12",NULL,"323883836","NLK jll","272119884","187162355","Brown, White","chronic painkillers",NULL),</v>
+        <v>("17","Brewster","Dog","Canine","Golden Retriever",NULL,"Spain","0","2019-04-16","3","0","3",NULL,"124599931","NLK jll","147292852","334167743","Brown, White","chronic painkillers",NULL),</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -3175,7 +3186,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <v>43606</v>
@@ -3189,22 +3200,22 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="N19">
         <f t="shared" ref="N19:Q19" ca="1" si="6">RANDBETWEEN(123456789,345678912)</f>
-        <v>144074287</v>
+        <v>241001562</v>
       </c>
       <c r="O19" t="s">
         <v>271</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="6"/>
-        <v>337663402</v>
+        <v>246276657</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="6"/>
-        <v>256669617</v>
+        <v>224466585</v>
       </c>
       <c r="R19" t="s">
         <v>72</v>
@@ -3214,7 +3225,7 @@
       </c>
       <c r="V19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("18","Jack","Dog","Lupus","Bulldog",NULL,"Spain","1","2019-05-21","2","0","1",NULL,"144074287","IEK kdo","337663402","256669617","White",NULL,"long ears"),</v>
+        <v>("18","Jack","Dog","Lupus","Bulldog",NULL,"Spain","0","2019-05-21","2","0","16",NULL,"241001562","IEK kdo","246276657","224466585","White",NULL,"long ears"),</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -3236,11 +3247,11 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>("19",NULL,NULL,NULL,NULL,NULL,NULL,"1","2019-04-16","3","0","11",NULL,NULL,NULL,NULL,NULL,NULL,NULL,NULL),</v>
+        <v>("19",NULL,NULL,NULL,NULL,NULL,NULL,"1","2019-04-16","3","0","3",NULL,NULL,NULL,NULL,NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
@@ -3262,7 +3273,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3273,10 +3284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B2892-340A-4DA8-A00C-A7D7ACDCDE8B}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3335,7 +3346,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4033490499</v>
+        <v>4037796381</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F7" si="0">_xlfn.CONCAT(LOWER(B2),IF(C2="","",_xlfn.CONCAT(".",LOWER(C2))),IF(D2="","",_xlfn.CONCAT(".",LOWER(D2))),"@ucalgary.ca")</f>
@@ -3353,7 +3364,7 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),"),")</f>
-        <v>("1","Damian","Bruce","Wayne","4033490499","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
+        <v>("1","Damian","Bruce","Wayne","4037796381","damian.bruce.wayne@ucalgary.ca","Wayne Manor"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3368,7 +3379,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E19" ca="1" si="1">RANDBETWEEN(4031111111,4039999999)</f>
-        <v>4036618139</v>
+        <v>4032715733</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
@@ -3383,7 +3394,7 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),"),")</f>
-        <v>("2","Yorrick",NULL,"Brown","4036618139","yorrick.brown@ucalgary.ca",NULL),</v>
+        <v>("2","Yorrick",NULL,"Brown","4032715733","yorrick.brown@ucalgary.ca",NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -3401,7 +3412,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4031679242</v>
+        <v>4039976724</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -3412,7 +3423,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Clark","Joseph","Kent","4031679242","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
+        <v>("3","Clark","Joseph","Kent","4039976724","clark.joseph.kent@ucalgary.ca","Smallville"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3424,7 +3435,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>4033707790</v>
+        <v>4036696635</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -3435,7 +3446,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","Tintin",NULL,NULL,"4033707790","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
+        <v>("4","Tintin",NULL,NULL,"4036696635","tintin@ucalgary.ca","Marlinspike Hall, Belgium"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3447,7 +3458,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>4032262774</v>
+        <v>4034443213</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -3458,7 +3469,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5","UCalgary",NULL,NULL,"4032262774","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
+        <v>("5","UCalgary",NULL,NULL,"4034443213","ucalgary@ucalgary.ca","2500 University Dr NW, Calgary, AB T2N 1N4"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3473,7 +3484,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4032057900</v>
+        <v>4039113114</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -3491,7 +3502,7 @@
 IF(E7="","NULL",_xlfn.CONCAT("""",E7,"""")),",",
 IF(F7="","NULL",_xlfn.CONCAT("""",F7,"""")),",",
 IF(G7="","NULL",_xlfn.CONCAT("""",G7,"""")),"),")</f>
-        <v>("6","James",NULL,"Gunn","4032057900","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA"),</v>
+        <v>("6","James",NULL,"Gunn","4039113114","james.gunn@ucalgary.ca","9336 Civic Center Drive, Beverly Hills, CA 90210-3604, USA"),</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3506,7 +3517,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>4035409869</v>
+        <v>4034043217</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" ref="F8" si="3">_xlfn.CONCAT(LOWER(B8),IF(C8="","",_xlfn.CONCAT(".",LOWER(C8))),IF(D8="","",_xlfn.CONCAT(".",LOWER(D8))),"@ucalgary.ca")</f>
@@ -3524,7 +3535,7 @@
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",G8,"""")),"),")</f>
-        <v>("7","Emily",NULL,"Marasco","4035409869","emily.marasco@ucalgary.ca","1042 Hope Street, Edmonton AB"),</v>
+        <v>("7","Emily",NULL,"Marasco","4034043217","emily.marasco@ucalgary.ca","1042 Hope Street, Edmonton AB"),</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3539,7 +3550,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>4037108797</v>
+        <v>4037529251</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" ref="F9" si="4">_xlfn.CONCAT(LOWER(B9),IF(C9="","",_xlfn.CONCAT(".",LOWER(C9))),IF(D9="","",_xlfn.CONCAT(".",LOWER(D9))),"@ucalgary.ca")</f>
@@ -3557,7 +3568,7 @@
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),",",
 IF(F9="","NULL",_xlfn.CONCAT("""",F9,"""")),",",
 IF(G9="","NULL",_xlfn.CONCAT("""",G9,"""")),"),")</f>
-        <v>("8","Kevin",NULL,"Durant","4037108797","kevin.durant@ucalgary.ca","5463 Wallflower Road, San Francisco, CA 90315, USA"),</v>
+        <v>("8","Kevin",NULL,"Durant","4037529251","kevin.durant@ucalgary.ca","5463 Wallflower Road, San Francisco, CA 90315, USA"),</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3575,7 +3586,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>4039993311</v>
+        <v>4036319918</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" ref="F10:F12" si="5">_xlfn.CONCAT(LOWER(B10),IF(C10="","",_xlfn.CONCAT(".",LOWER(C10))),IF(D10="","",_xlfn.CONCAT(".",LOWER(D10))),"@ucalgary.ca")</f>
@@ -3593,7 +3604,7 @@
 IF(E10="","NULL",_xlfn.CONCAT("""",E10,"""")),",",
 IF(F10="","NULL",_xlfn.CONCAT("""",F10,"""")),",",
 IF(G10="","NULL",_xlfn.CONCAT("""",G10,"""")),"),")</f>
-        <v>("9","Jason","Kamika","Fukuda","4039993311","jason.kamika.fukuda@ucalgary.ca","1354 Douglasdale Blvd, Calgary,AB "),</v>
+        <v>("9","Jason","Kamika","Fukuda","4036319918","jason.kamika.fukuda@ucalgary.ca","1354 Douglasdale Blvd, Calgary,AB "),</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3611,7 +3622,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>4036317073</v>
+        <v>4039718857</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="5"/>
@@ -3622,7 +3633,7 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>("10","Jacob","D","Brown","4036317073","jacob.d.brown@ucalgary.ca","30 Building Way, San Francisco, CA 90315, USA"),</v>
+        <v>("10","Jacob","D","Brown","4039718857","jacob.d.brown@ucalgary.ca","30 Building Way, San Francisco, CA 90315, USA"),</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3637,7 +3648,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>4032045558</v>
+        <v>4031177183</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="5"/>
@@ -3648,7 +3659,7 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>("11","Fred",NULL,"Kong","4032045558","fred.kong@ucalgary.ca","6401 Jasper Ave, Edmonton AB"),</v>
+        <v>("11","Fred",NULL,"Kong","4031177183","fred.kong@ucalgary.ca","6401 Jasper Ave, Edmonton AB"),</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3663,7 +3674,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>4038393727</v>
+        <v>4037044752</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ref="F13:F19" si="7">_xlfn.CONCAT(LOWER(B13),IF(C13="","",_xlfn.CONCAT(".",LOWER(C13))),IF(D13="","",_xlfn.CONCAT(".",LOWER(D13))),"@ucalgary.ca")</f>
@@ -3681,7 +3692,7 @@
 IF(E13="","NULL",_xlfn.CONCAT("""",E13,"""")),",",
 IF(F13="","NULL",_xlfn.CONCAT("""",F13,"""")),",",
 IF(G13="","NULL",_xlfn.CONCAT("""",G13,"""")),"),")</f>
-        <v>("12","Kyrie",NULL,"Irving","4038393727","kyrie.irving@ucalgary.ca","93 Essense Hall, Crawley, London"),</v>
+        <v>("12","Kyrie",NULL,"Irving","4037044752","kyrie.irving@ucalgary.ca","93 Essense Hall, Crawley, London"),</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3699,7 +3710,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>4037868960</v>
+        <v>4036014778</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="7"/>
@@ -3710,7 +3721,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>("13","Trinity","Hope","Smith","4037868960","trinity.hope.smith@ucalgary.ca","10 Guardian Manor, Fort McMurray, AB"),</v>
+        <v>("13","Trinity","Hope","Smith","4036014778","trinity.hope.smith@ucalgary.ca","10 Guardian Manor, Fort McMurray, AB"),</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3728,7 +3739,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>4037163052</v>
+        <v>4034607427</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="7"/>
@@ -3739,7 +3750,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>("14","Kailey","Camen","Hoeld","4037163052","kailey.camen.hoeld@ucalgary.ca","172 Silin Forest Road, Fort McMurray, AB"),</v>
+        <v>("14","Kailey","Camen","Hoeld","4034607427","kailey.camen.hoeld@ucalgary.ca","172 Silin Forest Road, Fort McMurray, AB"),</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3754,7 +3765,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>4031474881</v>
+        <v>4035442624</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="7"/>
@@ -3765,7 +3776,7 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>("15","Elizabeth",NULL,"Price","4031474881","elizabeth.price@ucalgary.ca","2850 Delancey Crescent, San Francisco, CA 904361, USA"),</v>
+        <v>("15","Elizabeth",NULL,"Price","4035442624","elizabeth.price@ucalgary.ca","2850 Delancey Crescent, San Francisco, CA 904361, USA"),</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -3780,7 +3791,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>4034053470</v>
+        <v>4037939914</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="7"/>
@@ -3791,7 +3802,7 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>("16","Dillon",NULL,"White","4034053470","dillon.white@ucalgary.ca","326 Ricardo Road, Bogota, Colombia "),</v>
+        <v>("16","Dillon",NULL,"White","4037939914","dillon.white@ucalgary.ca","326 Ricardo Road, Bogota, Colombia "),</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -3809,7 +3820,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>4039983321</v>
+        <v>4036430943</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="7"/>
@@ -3820,7 +3831,7 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>("17","Amber","Fair","Polinski","4039983321","amber.fair.polinski@ucalgary.ca","1792 Camille Street, Medellin, Colombia "),</v>
+        <v>("17","Amber","Fair","Polinski","4036430943","amber.fair.polinski@ucalgary.ca","1792 Camille Street, Medellin, Colombia "),</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -3838,7 +3849,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>4038282425</v>
+        <v>4038577100</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="7"/>
@@ -3849,7 +3860,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>("18","Gurneet","Kaur","Dhillon","4038282425","gurneet.kaur.dhillon@ucalgary.ca","#401 Arera Colony, Bhopal, MP, India"),</v>
+        <v>("18","Gurneet","Kaur","Dhillon","4038577100","gurneet.kaur.dhillon@ucalgary.ca","#401 Arera Colony, Bhopal, MP, India"),</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -3864,6 +3875,11 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3874,10 +3890,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A0186-44D9-498E-B660-5B0A566DD134}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4678,13 +4694,18 @@
         <v>44180</v>
       </c>
       <c r="D21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L21">
         <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -4694,10 +4715,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3D06D0-BF1F-4225-AF4B-50DA628F29F9}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4747,7 +4768,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -4759,7 +4780,7 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",TEXT(C2,"YYYY-MM-DD"),"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","5","2020-10-01","3","1"),</v>
+        <v>("1","5","2020-10-01","2","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -4774,7 +4795,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D29" ca="1" si="0">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -4786,7 +4807,7 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",TEXT(C3,"YYYY-MM-DD"),"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","4","2020-10-01","2","2"),</v>
+        <v>("2","4","2020-10-01","5","2"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4845,14 +4866,14 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","3","2020-10-01","6","5"),</v>
+        <v>("5","3","2020-10-01","1","5"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4867,14 +4888,14 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","3","2020-10-01","1","6"),</v>
+        <v>("6","3","2020-10-01","6","6"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -4889,7 +4910,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -4901,7 +4922,7 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",TEXT(C8,"YYYY-MM-DD"),"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"),")</f>
-        <v>("7","1","2020-10-01","4","7"),</v>
+        <v>("7","1","2020-10-01","3","7"),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4916,7 +4937,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -4928,7 +4949,7 @@
 IF(C9="","NULL",_xlfn.CONCAT("""",TEXT(C9,"YYYY-MM-DD"),"""")),",",
 IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),",",
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),"),")</f>
-        <v>("8","4","2020-11-03","7","1"),</v>
+        <v>("8","4","2020-11-03","6","1"),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -4944,14 +4965,14 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("9","5.2","2020-11-03","5","2"),</v>
+        <v>("9","5.2","2020-11-03","6","2"),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4967,14 +4988,14 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("10","4.2","2020-11-03","1","3"),</v>
+        <v>("10","4.2","2020-11-03","5","3"),</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -5013,14 +5034,14 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <v>5</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("12","40.2","2020-11-03","3","5"),</v>
+        <v>("12","40.2","2020-11-03","4","5"),</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -5059,14 +5080,14 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("14","3.2","2020-11-03","6","7"),</v>
+        <v>("14","3.2","2020-11-03","3","7"),</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -5105,14 +5126,14 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("16","3.6","2020-11-29","4","2"),</v>
+        <v>("16","3.6","2020-11-29","7","2"),</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -5128,14 +5149,14 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("17","4.8","2020-11-29","1","3"),</v>
+        <v>("17","4.8","2020-11-29","2","3"),</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -5151,14 +5172,14 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("18","3.8","2020-11-29","3","4"),</v>
+        <v>("18","3.8","2020-11-29","5","4"),</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -5174,14 +5195,14 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("19","29.8","2020-11-29","4","5"),</v>
+        <v>("19","29.8","2020-11-29","5","5"),</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -5197,14 +5218,14 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <v>6</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("20","39.8","2020-11-29","3","6"),</v>
+        <v>("20","39.8","2020-11-29","7","6"),</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -5220,14 +5241,14 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>7</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("21","2.8","2020-11-29","4","7"),</v>
+        <v>("21","2.8","2020-11-29","1","7"),</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -5243,14 +5264,14 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("22","3.8","2021-02-28","1","1"),</v>
+        <v>("22","3.8","2021-02-28","5","1"),</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -5266,14 +5287,14 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("23","1.2","2021-02-28","7","2"),</v>
+        <v>("23","1.2","2021-02-28","5","2"),</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -5289,14 +5310,14 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>3</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("24","4.2","2021-02-28","1","3"),</v>
+        <v>("24","4.2","2021-02-28","4","3"),</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -5312,14 +5333,14 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("25","5.4","2021-02-28","2","4"),</v>
+        <v>("25","5.4","2021-02-28","6","4"),</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -5335,14 +5356,14 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <v>5</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("26","4.4","2021-02-28","7","5"),</v>
+        <v>("26","4.4","2021-02-28","4","5"),</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -5358,14 +5379,14 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <v>6</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("27","30.4","2021-02-28","5","6"),</v>
+        <v>("27","30.4","2021-02-28","3","6"),</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -5381,7 +5402,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -5393,7 +5414,7 @@
 IF(C29="","NULL",_xlfn.CONCAT("""",TEXT(C29,"YYYY-MM-DD"),"""")),",",
 IF(D29="","NULL",_xlfn.CONCAT("""",D29,"""")),",",
 IF(E29="","NULL",_xlfn.CONCAT("""",E29,"""")),"),")</f>
-        <v>("28","40.4","2021-02-28","5","7"),</v>
+        <v>("28","40.4","2021-02-28","4","7"),</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -5436,6 +5457,11 @@
         <v>("29","40","2021-03-01",NULL,NULL),</v>
       </c>
     </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>325</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5444,10 +5470,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4EAFE5-CE5B-467E-B9FE-9E32C463D99E}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5495,7 +5521,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C7" ca="1" si="0">RANDBETWEEN(1,18)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
@@ -5505,7 +5531,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F19" ca="1" si="1">RANDBETWEEN(1,18)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>44105</v>
@@ -5519,7 +5545,7 @@
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1",NULL,"10","image1.png","neck","9","2020-10-01"),</v>
+        <v>("1",NULL,"9","image1.png","neck","5","2020-10-01"),</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5528,14 +5554,14 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>44105</v>
@@ -5549,7 +5575,7 @@
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2",NULL,"5","image2.png",NULL,"12","2020-10-01"),</v>
+        <v>("2",NULL,"10","image2.png",NULL,"1","2020-10-01"),</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5558,21 +5584,21 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>249</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1">
         <v>44105</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3",NULL,"17","image3.png",NULL,"15","2020-10-01"),</v>
+        <v>("3",NULL,"2","image3.png",NULL,"7","2020-10-01"),</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5584,21 +5610,21 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>102</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1">
         <v>44105</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","leg broken","10","image4.png",NULL,"12","2020-10-01"),</v>
+        <v>("4","leg broken","4","image4.png",NULL,"9","2020-10-01"),</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5607,21 +5633,21 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>105</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1">
         <v>44105</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"17","image5.png",NULL,"17","2020-10-01"),</v>
+        <v>("5",NULL,"9","image5.png",NULL,"11","2020-10-01"),</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5630,21 +5656,21 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
         <v>44105</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"4","image6.png",NULL,"1","2020-10-01"),</v>
+        <v>("6",NULL,"3","image6.png",NULL,"10","2020-10-01"),</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5653,14 +5679,14 @@
       </c>
       <c r="C8">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>103</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1">
         <v>44105</v>
@@ -5674,7 +5700,7 @@
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("7",NULL,"1","image7.png",NULL,"2","2020-10-01"),</v>
+        <v>("7",NULL,"12","image7.png",NULL,"15","2020-10-01"),</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5686,7 +5712,7 @@
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C19" ca="1" si="3">RANDBETWEEN(1,18)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>250</v>
@@ -5696,7 +5722,7 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1">
         <v>44329</v>
@@ -5710,7 +5736,7 @@
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),",",
 IF(F9="","NULL",_xlfn.CONCAT("""",F9,"""")),",",
 IF(G9="","NULL",_xlfn.CONCAT("""",TEXT(G9,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("8","initial photo","9","image8.png","baby","10","2021-05-13"),</v>
+        <v>("8","initial photo","18","image8.png","baby","5","2021-05-13"),</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5722,21 +5748,21 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>251</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1">
         <v>44315</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("9","initial photo","11","image9.png",NULL,"16","2021-04-29"),</v>
+        <v>("9","initial photo","16","image9.png",NULL,"5","2021-04-29"),</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5748,7 +5774,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>252</v>
@@ -5758,14 +5784,14 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G11" s="1">
         <v>44511</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("10","initial photo","17","image10.png","puberty","8","2021-11-11"),</v>
+        <v>("10","initial photo","3","image10.png","puberty","16","2021-11-11"),</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5784,14 +5810,14 @@
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1">
         <v>44361</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("11","initial photo","10","image11.png",NULL,"18","2021-06-14"),</v>
+        <v>("11","initial photo","10","image11.png",NULL,"8","2021-06-14"),</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5803,21 +5829,21 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>254</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1">
         <v>44366</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("12","initial photo","3","image12.png",NULL,"4","2021-06-19"),</v>
+        <v>("12","initial photo","17","image12.png",NULL,"15","2021-06-19"),</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -5826,21 +5852,21 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
         <v>255</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1">
         <v>44321</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("13",NULL,"10","image13.png",NULL,"3","2021-05-05"),</v>
+        <v>("13",NULL,"8","image13.png",NULL,"9","2021-05-05"),</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -5852,7 +5878,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>256</v>
@@ -5862,14 +5888,14 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1">
         <v>44440</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("14","knee replace","16","image14.png","knee","18","2021-09-01"),</v>
+        <v>("14","knee replace","2","image14.png","knee","8","2021-09-01"),</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5881,21 +5907,21 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
         <v>257</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16" s="1">
         <v>44274</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("15","losing fur","10","image15.png",NULL,"4","2021-03-19"),</v>
+        <v>("15","losing fur","6","image15.png",NULL,"2","2021-03-19"),</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5904,21 +5930,21 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
         <v>258</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1">
         <v>44472</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("16",NULL,"16","image16.png",NULL,"12","2021-10-03"),</v>
+        <v>("16",NULL,"15","image16.png",NULL,"13","2021-10-03"),</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -5930,21 +5956,21 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>259</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G18" s="1">
         <v>44443</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("17","post neuter ","1","image17.png",NULL,"5","2021-09-04"),</v>
+        <v>("17","post neuter ","7","image17.png",NULL,"11","2021-09-04"),</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -5953,21 +5979,21 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>260</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <v>44283</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>("18",NULL,"7","image18.png",NULL,"4","2021-03-28"),</v>
+        <v>("18",NULL,"17","image18.png",NULL,"1","2021-03-28"),</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -5984,13 +6010,18 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G21" s="1">
         <v>44283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -6000,10 +6031,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18B5F6C-A8DA-4DBA-AEF7-E7170CF7C840}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6048,14 +6079,14 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>44538</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -6064,7 +6095,7 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),"),")</f>
-        <v>("1","Nighttime terror","8","2021-12-08","13"),</v>
+        <v>("1","Nighttime terror","13","2021-12-08","1"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -6076,14 +6107,14 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C19" ca="1" si="0">RANDBETWEEN(1,18)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>44539</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E19" ca="1" si="1">RANDBETWEEN(1,18)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="2">_xlfn.CONCAT("(",
@@ -6092,7 +6123,7 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),"),")</f>
-        <v>("2","Howling ","9","2021-12-09","9"),</v>
+        <v>("2","Howling ","7","2021-12-09","15"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -6104,18 +6135,18 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>44540</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Pregnant ","16","2021-12-10","5"),</v>
+        <v>("3","Pregnant ","6","2021-12-10","7"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -6124,18 +6155,18 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <v>44538</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4",NULL,"15","2021-12-08","8"),</v>
+        <v>("4",NULL,"6","2021-12-08","15"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -6144,18 +6175,18 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>44539</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,"15","2021-12-09","15"),</v>
+        <v>("5",NULL,"9","2021-12-09","12"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -6164,18 +6195,18 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>44540</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,"18","2021-12-10","5"),</v>
+        <v>("6",NULL,"6","2021-12-10","2"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -6194,7 +6225,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -6203,7 +6234,7 @@
 IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
 IF(D8="","NULL",_xlfn.CONCAT("""",TEXT(D8,"YYYY-MM-DD"),"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),"),")</f>
-        <v>("7","Not sleeping","17","2021-12-08","5"),</v>
+        <v>("7","Not sleeping","17","2021-12-08","13"),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -6212,14 +6243,14 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1">
         <v>44105</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" ref="G9:G20" ca="1" si="3">_xlfn.CONCAT("(",
@@ -6228,7 +6259,7 @@
 IF(C9="","NULL",_xlfn.CONCAT("""",C9,"""")),",",
 IF(D9="","NULL",_xlfn.CONCAT("""",TEXT(D9,"YYYY-MM-DD"),"""")),",",
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),"),")</f>
-        <v>("8",NULL,"4","2020-10-01","5"),</v>
+        <v>("8",NULL,"14","2020-10-01","18"),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -6237,18 +6268,18 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1">
         <v>44105</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("9",NULL,"10","2020-10-01","1"),</v>
+        <v>("9",NULL,"8","2020-10-01","18"),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -6257,18 +6288,18 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <v>44329</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("10",NULL,"15","2021-05-13","8"),</v>
+        <v>("10",NULL,"4","2021-05-13","18"),</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -6277,18 +6308,18 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
         <v>44315</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("11",NULL,"9","2021-04-29","5"),</v>
+        <v>("11",NULL,"11","2021-04-29","9"),</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -6304,11 +6335,11 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("12",NULL,"9","2021-11-11","9"),</v>
+        <v>("12",NULL,"9","2021-11-11","16"),</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -6320,18 +6351,18 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1">
         <v>44361</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("13","Excessive scratching","7","2021-06-14","11"),</v>
+        <v>("13","Excessive scratching","6","2021-06-14","6"),</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -6340,18 +6371,18 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1">
         <v>44366</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("14",NULL,"1","2021-06-19","2"),</v>
+        <v>("14",NULL,"12","2021-06-19","9"),</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -6363,18 +6394,18 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
         <v>44321</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("15","Neuterization consult","1","2021-05-05","2"),</v>
+        <v>("15","Neuterization consult","4","2021-05-05","16"),</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -6383,7 +6414,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1">
         <v>44440</v>
@@ -6394,7 +6425,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("16",NULL,"1","2021-09-01","10"),</v>
+        <v>("16",NULL,"15","2021-09-01","10"),</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -6403,18 +6434,18 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1">
         <v>44274</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("17",NULL,"14","2021-03-19","8"),</v>
+        <v>("17",NULL,"9","2021-03-19","1"),</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -6423,18 +6454,18 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1">
         <v>44472</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("18",NULL,"6","2021-10-03","6"),</v>
+        <v>("18",NULL,"18","2021-10-03","13"),</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -6451,12 +6482,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D21" s="1">
         <v>44474</v>
       </c>
       <c r="E21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>324</v>
       </c>
     </row>
@@ -6467,10 +6503,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E769BC6-8AA4-47AC-8CDF-52C74C698B1A}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6523,11 +6559,11 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -6540,7 +6576,7 @@
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("",F2,"")),"),")</f>
-        <v>("1","Limp Walk","2021-12-08","3","4",1),</v>
+        <v>("1","Limp Walk","2021-12-08","7","11",1),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -6552,7 +6588,7 @@
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E20" ca="1" si="0">RANDBETWEEN(1,18)</f>
@@ -6569,7 +6605,7 @@
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("",F3,"")),"),")</f>
-        <v>("2",NULL,"2020-12-12","2","6",1),</v>
+        <v>("2",NULL,"2020-12-12","4","6",1),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -6584,18 +6620,18 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D20" ca="1" si="2">RANDBETWEEN(1,18)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("3","Diabetes","2021-05-16","15","1",0),</v>
+        <v>("3","Diabetes","2021-05-16","14","3",0),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -6610,18 +6646,18 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("4","Inflammed limb","2021-05-29","11","9",0),</v>
+        <v>("4","Inflammed limb","2021-05-29","3","6",0),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -6636,18 +6672,18 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("5","Bladder Infection","2021-05-16","4","2",0),</v>
+        <v>("5","Bladder Infection","2021-05-16","14","7",0),</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -6662,18 +6698,18 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>("6","chronic kidney disease","2021-11-17","11","13",0),</v>
+        <v>("6","chronic kidney disease","2021-11-17","16","14",0),</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -6688,11 +6724,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -6705,7 +6741,7 @@
 IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),",",
 IF(E8="","NULL",_xlfn.CONCAT("""",E8,"""")),",",
 IF(F8="","NULL",_xlfn.CONCAT("",F8,"")),"),")</f>
-        <v>("7","Upset Stomach","2021-11-17","15","12",0),</v>
+        <v>("7","Upset Stomach","2021-11-17","7","18",0),</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -6717,11 +6753,11 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
       </c>
       <c r="F9">
         <f ca="1">RANDBETWEEN(0,1)</f>
@@ -6735,7 +6771,7 @@
 IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),",",
 IF(E9="","NULL",_xlfn.CONCAT("""",E9,"""")),",",
 IF(F9="","NULL",_xlfn.CONCAT("",F9,"")),"),")</f>
-        <v>("8",NULL,"2021-12-08","7","16",0),</v>
+        <v>("8",NULL,"2021-12-08","2","7",0),</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -6747,19 +6783,19 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" ref="F10:F20" ca="1" si="4">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("9",NULL,"2021-12-09","18","4",0),</v>
+        <v>("9",NULL,"2021-12-09","6","1",1),</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -6775,7 +6811,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="4"/>
@@ -6783,7 +6819,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("10",NULL,"2021-12-10","14","8",1),</v>
+        <v>("10",NULL,"2021-12-10","14","6",1),</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -6795,19 +6831,19 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("11",NULL,"2021-12-08","16","10",0),</v>
+        <v>("11",NULL,"2021-12-08","6","18",1),</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -6819,19 +6855,19 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("12",NULL,"2020-10-01","3","2",0),</v>
+        <v>("12",NULL,"2020-10-01","11","9",1),</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -6843,11 +6879,11 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="4"/>
@@ -6855,7 +6891,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("13",NULL,"2020-10-01","4","17",0),</v>
+        <v>("13",NULL,"2020-10-01","11","6",0),</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -6867,19 +6903,19 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("14",NULL,"2021-05-13","1","12",1),</v>
+        <v>("14",NULL,"2021-05-13","3","16",0),</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -6891,7 +6927,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
@@ -6903,7 +6939,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("15",NULL,"2021-04-29","9","3",1),</v>
+        <v>("15",NULL,"2021-04-29","14","3",1),</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -6915,11 +6951,11 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="4"/>
@@ -6927,7 +6963,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("16",NULL,"2021-11-11","8","3",1),</v>
+        <v>("16",NULL,"2021-11-11","3","7",1),</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -6939,19 +6975,19 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("17",NULL,"2021-06-14","16","12",1),</v>
+        <v>("17",NULL,"2021-06-14","14","15",0),</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -6963,11 +6999,11 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="4"/>
@@ -6975,7 +7011,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("18",NULL,"2021-06-19","12","15",0),</v>
+        <v>("18",NULL,"2021-06-19","5","11",0),</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -6998,10 +7034,10 @@
         <v>44366</v>
       </c>
       <c r="D21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -7009,6 +7045,11 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>324</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7017,10 +7058,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B89DC6B-9FAC-4B83-94B7-9C2F8C662292}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7088,7 +7129,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(1,18)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1">
         <v>44538</v>
@@ -7107,7 +7148,7 @@
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),",",
 IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
-        <v>("1","Physical exam","Pfizer","0.5mg","transdermal","18","2021-12-08","13"),</v>
+        <v>("1","Physical exam","Pfizer","0.5mg","transdermal","9","2021-12-08","13"),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -7119,14 +7160,14 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F20" ca="1" si="0">RANDBETWEEN(1,18)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
         <v>44539</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H20" ca="1" si="1">RANDBETWEEN(1,18)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J7" ca="1" si="2">_xlfn.CONCAT("(",
@@ -7138,7 +7179,7 @@
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),",",
 IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
-        <v>("2","Blood work",NULL,NULL,NULL,"8","2021-12-09","13"),</v>
+        <v>("2","Blood work",NULL,NULL,NULL,"6","2021-12-09","11"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -7156,18 +7197,18 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
         <v>44540</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3","Da2pp","Astrazeneca","0.02mg",NULL,"5","2021-12-10","17"),</v>
+        <v>("3","Da2pp","Astrazeneca","0.02mg",NULL,"12","2021-12-10","4"),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -7179,18 +7220,18 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1">
         <v>44538</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4","dental cleaning",NULL,NULL,NULL,"12","2021-12-08","8"),</v>
+        <v>("4","dental cleaning",NULL,NULL,NULL,"15","2021-12-08","4"),</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -7211,18 +7252,18 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
         <v>44539</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5","drontal deworm","Moderna","0.2mg","intramuscular","11","2021-12-09","11"),</v>
+        <v>("5","drontal deworm","Moderna","0.2mg","intramuscular","7","2021-12-09","10"),</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -7234,18 +7275,18 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1">
         <v>44540</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6","rabies vaccination",NULL,NULL,NULL,"11","2021-12-10","10"),</v>
+        <v>("6","rabies vaccination",NULL,NULL,NULL,"13","2021-12-10","15"),</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -7260,14 +7301,14 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <v>44538</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J8" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -7279,7 +7320,7 @@
 IF(F8="","NULL",_xlfn.CONCAT("""",F8,"""")),",",
 IF(G8="","NULL",_xlfn.CONCAT("""",TEXT(G8,"YYYY-MM-DD"),"""")),",",
 IF(H8="","NULL",_xlfn.CONCAT("""",H8,"""")),"),")</f>
-        <v>("7","Revolution treatment","Pfizer",NULL,NULL,"13","2021-12-08","7"),</v>
+        <v>("7","Revolution treatment","Pfizer",NULL,NULL,"1","2021-12-08","4"),</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -7288,14 +7329,14 @@
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1">
         <v>44517</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" ref="J9:J20" ca="1" si="3">_xlfn.CONCAT("(",
@@ -7307,7 +7348,7 @@
 IF(F9="","NULL",_xlfn.CONCAT("""",F9,"""")),",",
 IF(G9="","NULL",_xlfn.CONCAT("""",TEXT(G9,"YYYY-MM-DD"),"""")),",",
 IF(H9="","NULL",_xlfn.CONCAT("""",H9,"""")),"),")</f>
-        <v>("8",NULL,NULL,NULL,NULL,"13","2021-11-17","3"),</v>
+        <v>("8",NULL,NULL,NULL,NULL,"17","2021-11-17","2"),</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -7319,14 +7360,14 @@
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1">
         <v>44517</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J10" t="str">
         <f ca="1">_xlfn.CONCAT("(",
@@ -7338,7 +7379,7 @@
 IF(F10="","NULL",_xlfn.CONCAT("""",F10,"""")),",",
 IF(G10="","NULL",_xlfn.CONCAT("""",TEXT(G10,"YYYY-MM-DD"),"""")),",",
 IF(H10="","NULL",_xlfn.CONCAT("""",H10,"""")),"),")</f>
-        <v>("9","knee replacement","Astrazeneca","0.1mg","injection","17","2021-11-17","12"),</v>
+        <v>("9","knee replacement","Astrazeneca","0.1mg","injection","13","2021-11-17","16"),</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -7350,18 +7391,18 @@
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1">
         <v>44538</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("10","leg amputation",NULL,NULL,NULL,"2","2021-12-08","6"),</v>
+        <v>("10","leg amputation",NULL,NULL,NULL,"4","2021-12-08","3"),</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -7377,11 +7418,11 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("11",NULL,NULL,NULL,NULL,"9","2021-12-09","3"),</v>
+        <v>("11",NULL,NULL,NULL,NULL,"9","2021-12-09","18"),</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -7390,18 +7431,18 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1">
         <v>44540</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("12",NULL,NULL,NULL,NULL,"9","2021-12-10","11"),</v>
+        <v>("12",NULL,NULL,NULL,NULL,"17","2021-12-10","8"),</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -7413,18 +7454,18 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G14" s="1">
         <v>44538</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("13","Physical exam",NULL,NULL,NULL,"4","2021-12-08","16"),</v>
+        <v>("13","Physical exam",NULL,NULL,NULL,"11","2021-12-08","13"),</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -7445,18 +7486,18 @@
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G15" s="1">
         <v>44538</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("14","Vaccine","Astrazeneca","0.1mg","injection","14","2021-12-08","6"),</v>
+        <v>("14","Vaccine","Astrazeneca","0.1mg","injection","6","2021-12-08","10"),</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -7468,18 +7509,18 @@
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1">
         <v>44105</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("15","Da2pp",NULL,NULL,NULL,"6","2020-10-01","12"),</v>
+        <v>("15","Da2pp",NULL,NULL,NULL,"7","2020-10-01","10"),</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -7494,18 +7535,18 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G17" s="1">
         <v>44329</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("16","dental cleaning","Astrazeneca",NULL,NULL,"16","2021-05-13","12"),</v>
+        <v>("16","dental cleaning","Astrazeneca",NULL,NULL,"7","2021-05-13","11"),</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -7517,18 +7558,18 @@
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G18" s="1">
         <v>44315</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("17","drontal deworm",NULL,NULL,NULL,"7","2021-04-29","12"),</v>
+        <v>("17","drontal deworm",NULL,NULL,NULL,"11","2021-04-29","3"),</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -7537,18 +7578,18 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <v>44511</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("18",NULL,NULL,NULL,NULL,"5","2021-11-11","16"),</v>
+        <v>("18",NULL,NULL,NULL,NULL,"1","2021-11-11","1"),</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -7557,18 +7598,18 @@
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>44512</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>("19",NULL,NULL,NULL,NULL,"6","2021-11-12","3"),</v>
+        <v>("19",NULL,NULL,NULL,NULL,"1","2021-11-12","15"),</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -7576,6 +7617,11 @@
         <v>44512</v>
       </c>
       <c r="H21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>324</v>
       </c>
     </row>
@@ -7589,7 +7635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F1D254-DAA5-4C45-81E9-439CA656FE0D}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7648,11 +7694,11 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
         <v>44105</v>
@@ -7673,7 +7719,7 @@
 IF(H2="","NULL",_xlfn.CONCAT("""",TEXT(H2,"YYYY-MM-DD"),"""")),",",
 IF(I2="","NULL",_xlfn.CONCAT("""",TEXT(I2,"YYYY-MM-DD"),"""")),",",
 IF(J2="","NULL",_xlfn.CONCAT("""",TEXT(J2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1",NULL,NULL,"1","4","2020-10-01",NULL,NULL,NULL,NULL),</v>
+        <v>("1",NULL,NULL,"4","5","2020-10-01",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -7686,7 +7732,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="1">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1">
         <v>44105</v>
@@ -7707,7 +7753,7 @@
 IF(H3="","NULL",_xlfn.CONCAT("""",TEXT(H3,"YYYY-MM-DD"),"""")),",",
 IF(I3="","NULL",_xlfn.CONCAT("""",TEXT(I3,"YYYY-MM-DD"),"""")),",",
 IF(J3="","NULL",_xlfn.CONCAT("""",TEXT(J3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2",NULL,NULL,"7","2","2020-10-01",NULL,NULL,NULL,NULL),</v>
+        <v>("2",NULL,NULL,"7","3","2020-10-01",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -7716,11 +7762,11 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
         <v>44105</v>
@@ -7731,7 +7777,7 @@
       <c r="J4" s="1"/>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("3",NULL,NULL,"3","3","2020-10-01",NULL,NULL,NULL,NULL),</v>
+        <v>("3",NULL,NULL,"1","1","2020-10-01",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -7740,11 +7786,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1">
         <v>44105</v>
@@ -7755,7 +7801,7 @@
       <c r="J5" s="1"/>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("4",NULL,NULL,"6","6","2020-10-01",NULL,NULL,NULL,NULL),</v>
+        <v>("4",NULL,NULL,"4","7","2020-10-01",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -7764,11 +7810,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1">
         <v>44105</v>
@@ -7779,7 +7825,7 @@
       <c r="J6" s="1"/>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("5",NULL,NULL,"1","4","2020-10-01",NULL,NULL,NULL,NULL),</v>
+        <v>("5",NULL,NULL,"2","7","2020-10-01",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -7788,7 +7834,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
@@ -7803,7 +7849,7 @@
       <c r="J7" s="1"/>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>("6",NULL,NULL,"2","1","2020-10-01",NULL,NULL,NULL,NULL),</v>
+        <v>("6",NULL,NULL,"7","1","2020-10-01",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -7812,11 +7858,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
         <v>44105</v>
@@ -7837,7 +7883,7 @@
 IF(H8="","NULL",_xlfn.CONCAT("""",TEXT(H8,"YYYY-MM-DD"),"""")),",",
 IF(I8="","NULL",_xlfn.CONCAT("""",TEXT(I8,"YYYY-MM-DD"),"""")),",",
 IF(J8="","NULL",_xlfn.CONCAT("""",TEXT(J8,"YYYY-MM-DD"),"""")),");")</f>
-        <v>("7",NULL,NULL,"3","7","2020-10-01",NULL,NULL,NULL,NULL);</v>
+        <v>("7",NULL,NULL,"4","6","2020-10-01",NULL,NULL,NULL,NULL);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>